<commit_message>
Refactor monitoring kpu sites
</commit_message>
<xml_diff>
--- a/data/premium-sites.xlsx
+++ b/data/premium-sites.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Local Repository\Telkom Projects\monitoring-site-premium-telegram-bot\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3391DA9-5E2F-4119-9C28-22756B7BD06E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D928D22-71AA-4F90-B22A-10EF29DF7B39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1198,8 +1198,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="H61" sqref="H61"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="G57" sqref="G57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Update datek premium WTG001
</commit_message>
<xml_diff>
--- a/data/premium-sites.xlsx
+++ b/data/premium-sites.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Local Repository\Telkom Projects\monitoring-site-premium-telegram-bot\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D928D22-71AA-4F90-B22A-10EF29DF7B39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A2846CE-5F51-4E25-B100-39DD94CCF75D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="662" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="670" uniqueCount="276">
   <si>
     <t>Subdistrict</t>
   </si>
@@ -245,22 +245,6 @@
     <t>SOPPENG</t>
   </si>
   <si>
-    <t>GPON02-D7-WTG-4</t>
-  </si>
-  <si>
-    <t>172.25.212.156</t>
-  </si>
-  <si>
-    <t>2/16/1</t>
-  </si>
-  <si>
-    <t>FHTT05e9e534</t>
-  </si>
-  <si>
-    <t>config
-show authorization 1/2/16 | include FHTT05e9e534</t>
-  </si>
-  <si>
     <t>SULTRA</t>
   </si>
   <si>
@@ -859,6 +843,24 @@
   </si>
   <si>
     <t>SN ONT</t>
+  </si>
+  <si>
+    <t>GigabitEthernet0/8/2</t>
+  </si>
+  <si>
+    <t>display interface GigabitEthernet0/8/2</t>
+  </si>
+  <si>
+    <t>GigabitEthernet0/8/2 current state : UP</t>
+  </si>
+  <si>
+    <t>GigabitEthernet0/8/3</t>
+  </si>
+  <si>
+    <t>display interface GigabitEthernet0/8/3</t>
+  </si>
+  <si>
+    <t>GigabitEthernet0/8/3 current state : UP</t>
   </si>
 </sst>
 </file>
@@ -1198,8 +1200,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="G57" sqref="G57"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1249,10 +1251,10 @@
         <v>8</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="L1" s="4" t="s">
         <v>9</v>
@@ -1518,7 +1520,7 @@
         <v>54</v>
       </c>
       <c r="K7" s="5" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="L7" s="5" t="s">
         <v>55</v>
@@ -1559,7 +1561,7 @@
         <v>57</v>
       </c>
       <c r="K8" s="5" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="L8" s="5" t="s">
         <v>58</v>
@@ -1634,7 +1636,7 @@
       <c r="L10" s="5"/>
       <c r="M10" s="5"/>
     </row>
-    <row r="11" spans="1:33" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>59</v>
       </c>
@@ -1648,13 +1650,13 @@
         <v>71</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>72</v>
+        <v>16</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>73</v>
+        <v>17</v>
       </c>
       <c r="H11" s="5" t="s">
         <v>18</v>
@@ -1663,16 +1665,16 @@
         <v>19</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>74</v>
+        <v>270</v>
       </c>
       <c r="K11" s="5" t="s">
-        <v>75</v>
+        <v>21</v>
       </c>
       <c r="L11" s="6" t="s">
-        <v>76</v>
+        <v>271</v>
       </c>
       <c r="M11" s="5" t="s">
-        <v>36</v>
+        <v>272</v>
       </c>
     </row>
     <row r="12" spans="1:33" x14ac:dyDescent="0.3">
@@ -1689,132 +1691,148 @@
         <v>71</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="5"/>
-      <c r="L12" s="5"/>
-      <c r="M12" s="5"/>
+        <v>15</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="K12" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="L12" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="M12" s="5" t="s">
+        <v>275</v>
+      </c>
     </row>
     <row r="13" spans="1:33" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D13" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="J13" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="K13" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="L13" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="M13" s="5" t="s">
         <v>81</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="H13" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="I13" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="J13" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="K13" s="5" t="s">
-        <v>267</v>
-      </c>
-      <c r="L13" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="M13" s="5" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="14" spans="1:33" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="G14" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="J14" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="H14" s="5" t="s">
+      <c r="K14" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="L14" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="I14" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="J14" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="K14" s="5" t="s">
-        <v>267</v>
-      </c>
-      <c r="L14" s="6" t="s">
-        <v>88</v>
-      </c>
       <c r="M14" s="5" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="15" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="J15" s="5" t="s">
         <v>54</v>
       </c>
       <c r="K15" s="5" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="L15" s="5" t="s">
         <v>55</v>
@@ -1825,37 +1843,37 @@
     </row>
     <row r="16" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="E16" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="J16" s="5" t="s">
         <v>57</v>
       </c>
       <c r="K16" s="5" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="L16" s="5" t="s">
         <v>58</v>
@@ -1866,40 +1884,40 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="K17" s="5" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="L17" s="5" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="M17" s="5" t="s">
         <v>56</v>
@@ -1907,40 +1925,40 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F18" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="H18" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="I18" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="J18" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="G18" s="5" t="s">
+      <c r="K18" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="L18" s="5" t="s">
         <v>99</v>
-      </c>
-      <c r="H18" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="I18" s="5" t="s">
-        <v>268</v>
-      </c>
-      <c r="J18" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="K18" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="L18" s="5" t="s">
-        <v>104</v>
       </c>
       <c r="M18" s="5" t="s">
         <v>56</v>
@@ -1948,25 +1966,25 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="E19" s="5" t="s">
         <v>15</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="H19" s="5" t="s">
         <v>18</v>
@@ -1975,39 +1993,39 @@
         <v>19</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="K19" s="5" t="s">
         <v>21</v>
       </c>
       <c r="L19" s="5" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="M19" s="5" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>15</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="H20" s="5" t="s">
         <v>18</v>
@@ -2016,39 +2034,39 @@
         <v>19</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="K20" s="5" t="s">
         <v>21</v>
       </c>
       <c r="L20" s="5" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="M20" s="5" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="21" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="E21" s="5" t="s">
         <v>30</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="H21" s="5" t="s">
         <v>18</v>
@@ -2057,13 +2075,13 @@
         <v>19</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="K21" s="5" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="L21" s="6" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="M21" s="5" t="s">
         <v>36</v>
@@ -2071,16 +2089,16 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="E22" s="5" t="s">
         <v>69</v>
@@ -2096,40 +2114,40 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D23" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="H23" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I23" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J23" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="K23" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="E23" s="5" t="s">
+      <c r="L23" s="5" t="s">
         <v>126</v>
-      </c>
-      <c r="F23" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="G23" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="H23" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I23" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J23" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="K23" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="L23" s="5" t="s">
-        <v>131</v>
       </c>
       <c r="M23" s="5" t="s">
         <v>43</v>
@@ -2137,40 +2155,40 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D24" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="H24" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I24" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J24" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="K24" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="E24" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="F24" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="G24" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="H24" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I24" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J24" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="K24" s="5" t="s">
+      <c r="L24" s="5" t="s">
         <v>130</v>
-      </c>
-      <c r="L24" s="5" t="s">
-        <v>135</v>
       </c>
       <c r="M24" s="5" t="s">
         <v>43</v>
@@ -2178,37 +2196,37 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="E25" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="H25" s="5" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="I25" s="5" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="J25" s="5" t="s">
         <v>54</v>
       </c>
       <c r="K25" s="5" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="L25" s="5" t="s">
         <v>55</v>
@@ -2219,37 +2237,37 @@
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="E26" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="I26" s="5" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="J26" s="5" t="s">
         <v>57</v>
       </c>
       <c r="K26" s="5" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="L26" s="5" t="s">
         <v>58</v>
@@ -2260,25 +2278,25 @@
     </row>
     <row r="27" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="E27" s="5" t="s">
         <v>30</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="H27" s="5" t="s">
         <v>18</v>
@@ -2287,13 +2305,13 @@
         <v>19</v>
       </c>
       <c r="J27" s="5" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="K27" s="5" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="L27" s="6" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="M27" s="5" t="s">
         <v>36</v>
@@ -2301,16 +2319,16 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="E28" s="5" t="s">
         <v>69</v>
@@ -2326,25 +2344,25 @@
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="E29" s="5" t="s">
         <v>37</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="H29" s="5" t="s">
         <v>18</v>
@@ -2353,13 +2371,13 @@
         <v>19</v>
       </c>
       <c r="J29" s="5" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="K29" s="5" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="L29" s="5" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="M29" s="5" t="s">
         <v>43</v>
@@ -2367,25 +2385,25 @@
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="E30" s="5" t="s">
         <v>37</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="H30" s="5" t="s">
         <v>18</v>
@@ -2394,13 +2412,13 @@
         <v>19</v>
       </c>
       <c r="J30" s="5" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="K30" s="5" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="L30" s="5" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="M30" s="5" t="s">
         <v>43</v>
@@ -2408,25 +2426,25 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="C31" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="E31" s="5" t="s">
         <v>37</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="H31" s="5" t="s">
         <v>18</v>
@@ -2435,13 +2453,13 @@
         <v>19</v>
       </c>
       <c r="J31" s="5" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="K31" s="5" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="L31" s="5" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="M31" s="5" t="s">
         <v>43</v>
@@ -2449,25 +2467,25 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="C32" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="E32" s="5" t="s">
         <v>37</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="H32" s="5" t="s">
         <v>18</v>
@@ -2476,13 +2494,13 @@
         <v>19</v>
       </c>
       <c r="J32" s="5" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="K32" s="5" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="L32" s="5" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="M32" s="5" t="s">
         <v>43</v>
@@ -2490,25 +2508,25 @@
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="C33" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="H33" s="5" t="s">
         <v>18</v>
@@ -2520,36 +2538,36 @@
         <v>54</v>
       </c>
       <c r="K33" s="5" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="L33" s="5" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="M33" s="5" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="C34" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="G34" s="5" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="H34" s="5" t="s">
         <v>18</v>
@@ -2561,36 +2579,36 @@
         <v>57</v>
       </c>
       <c r="K34" s="5" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="L34" s="5" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="M34" s="5" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
     </row>
     <row r="35" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="C35" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="E35" s="5" t="s">
         <v>30</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="H35" s="5" t="s">
         <v>18</v>
@@ -2599,13 +2617,13 @@
         <v>19</v>
       </c>
       <c r="J35" s="5" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="K35" s="5" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="L35" s="6" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="M35" s="5" t="s">
         <v>36</v>
@@ -2613,16 +2631,16 @@
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="C36" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="E36" s="5" t="s">
         <v>69</v>
@@ -2638,25 +2656,25 @@
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="C37" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="E37" s="5" t="s">
         <v>37</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="H37" s="5" t="s">
         <v>18</v>
@@ -2665,13 +2683,13 @@
         <v>19</v>
       </c>
       <c r="J37" s="5" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="K37" s="5" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="L37" s="5" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="M37" s="5" t="s">
         <v>43</v>
@@ -2679,25 +2697,25 @@
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="E38" s="5" t="s">
         <v>37</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="G38" s="5" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="H38" s="5" t="s">
         <v>18</v>
@@ -2706,13 +2724,13 @@
         <v>19</v>
       </c>
       <c r="J38" s="5" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="K38" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="L38" s="5" t="s">
         <v>182</v>
-      </c>
-      <c r="L38" s="5" t="s">
-        <v>187</v>
       </c>
       <c r="M38" s="5" t="s">
         <v>43</v>
@@ -2720,25 +2738,25 @@
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="E39" s="5" t="s">
         <v>37</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="H39" s="5" t="s">
         <v>18</v>
@@ -2747,13 +2765,13 @@
         <v>19</v>
       </c>
       <c r="J39" s="5" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="K39" s="5" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="L39" s="5" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="M39" s="5" t="s">
         <v>43</v>
@@ -2761,25 +2779,25 @@
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="C40" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="E40" s="5" t="s">
         <v>37</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="G40" s="5" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="H40" s="5" t="s">
         <v>18</v>
@@ -2788,13 +2806,13 @@
         <v>19</v>
       </c>
       <c r="J40" s="5" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="K40" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="L40" s="5" t="s">
         <v>193</v>
-      </c>
-      <c r="L40" s="5" t="s">
-        <v>198</v>
       </c>
       <c r="M40" s="5" t="s">
         <v>43</v>
@@ -2802,25 +2820,25 @@
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41" s="5" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="C41" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="E41" s="5" t="s">
         <v>37</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="H41" s="5" t="s">
         <v>18</v>
@@ -2829,13 +2847,13 @@
         <v>19</v>
       </c>
       <c r="J41" s="5" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="K41" s="5" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="L41" s="5" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="M41" s="5" t="s">
         <v>43</v>
@@ -2843,40 +2861,40 @@
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="C42" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="E42" s="5" t="s">
         <v>37</v>
       </c>
       <c r="F42" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="G42" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="H42" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I42" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J42" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="G42" s="5" t="s">
+      <c r="K42" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="L42" s="5" t="s">
         <v>202</v>
-      </c>
-      <c r="H42" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I42" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J42" s="5" t="s">
-        <v>206</v>
-      </c>
-      <c r="K42" s="5" t="s">
-        <v>204</v>
-      </c>
-      <c r="L42" s="5" t="s">
-        <v>207</v>
       </c>
       <c r="M42" s="5" t="s">
         <v>43</v>
@@ -2884,37 +2902,37 @@
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="C43" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="E43" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="H43" s="5" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="I43" s="5" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="J43" s="5" t="s">
         <v>54</v>
       </c>
       <c r="K43" s="5" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="L43" s="5" t="s">
         <v>55</v>
@@ -2925,37 +2943,37 @@
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="C44" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="E44" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="G44" s="5" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="H44" s="5" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="I44" s="5" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="J44" s="5" t="s">
         <v>57</v>
       </c>
       <c r="K44" s="5" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="L44" s="5" t="s">
         <v>58</v>
@@ -2966,25 +2984,25 @@
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="C45" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="E45" s="5" t="s">
         <v>15</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="G45" s="5" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="H45" s="5" t="s">
         <v>18</v>
@@ -2993,95 +3011,95 @@
         <v>19</v>
       </c>
       <c r="J45" s="5" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="K45" s="5" t="s">
         <v>21</v>
       </c>
       <c r="L45" s="5" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="M45" s="5" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46" s="5" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="C46" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="E46" s="5" t="s">
         <v>15</v>
       </c>
       <c r="F46" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="G46" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="H46" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I46" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J46" s="5" t="s">
         <v>215</v>
-      </c>
-      <c r="G46" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="H46" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I46" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J46" s="5" t="s">
-        <v>220</v>
       </c>
       <c r="K46" s="5" t="s">
         <v>21</v>
       </c>
       <c r="L46" s="5" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="M46" s="5" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A47" s="5" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="C47" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D47" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="E47" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="F47" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="G47" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="H47" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I47" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J47" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="K47" s="5" t="s">
         <v>224</v>
       </c>
-      <c r="E47" s="5" t="s">
+      <c r="L47" s="5" t="s">
         <v>225</v>
-      </c>
-      <c r="F47" s="5" t="s">
-        <v>226</v>
-      </c>
-      <c r="G47" s="5" t="s">
-        <v>227</v>
-      </c>
-      <c r="H47" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I47" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J47" s="5" t="s">
-        <v>228</v>
-      </c>
-      <c r="K47" s="5" t="s">
-        <v>229</v>
-      </c>
-      <c r="L47" s="5" t="s">
-        <v>230</v>
       </c>
       <c r="M47" s="5" t="s">
         <v>43</v>
@@ -3089,40 +3107,40 @@
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="C48" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D48" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="E48" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="F48" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="G48" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="H48" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I48" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J48" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="K48" s="5" t="s">
         <v>224</v>
       </c>
-      <c r="E48" s="5" t="s">
-        <v>225</v>
-      </c>
-      <c r="F48" s="5" t="s">
-        <v>231</v>
-      </c>
-      <c r="G48" s="5" t="s">
-        <v>232</v>
-      </c>
-      <c r="H48" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I48" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J48" s="5" t="s">
-        <v>233</v>
-      </c>
-      <c r="K48" s="5" t="s">
+      <c r="L48" s="5" t="s">
         <v>229</v>
-      </c>
-      <c r="L48" s="5" t="s">
-        <v>234</v>
       </c>
       <c r="M48" s="5" t="s">
         <v>43</v>
@@ -3130,25 +3148,25 @@
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="C49" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="G49" s="5" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="H49" s="5" t="s">
         <v>18</v>
@@ -3157,13 +3175,13 @@
         <v>19</v>
       </c>
       <c r="J49" s="5" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="K49" s="5" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="L49" s="5" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="M49" s="5" t="s">
         <v>43</v>
@@ -3171,40 +3189,40 @@
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="C50" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D50" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="E50" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="F50" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="G50" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="H50" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I50" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J50" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="K50" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="L50" s="5" t="s">
         <v>236</v>
-      </c>
-      <c r="E50" s="5" t="s">
-        <v>225</v>
-      </c>
-      <c r="F50" s="5" t="s">
-        <v>231</v>
-      </c>
-      <c r="G50" s="5" t="s">
-        <v>232</v>
-      </c>
-      <c r="H50" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I50" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J50" s="5" t="s">
-        <v>240</v>
-      </c>
-      <c r="K50" s="5" t="s">
-        <v>238</v>
-      </c>
-      <c r="L50" s="5" t="s">
-        <v>241</v>
       </c>
       <c r="M50" s="5" t="s">
         <v>43</v>
@@ -3212,66 +3230,66 @@
     </row>
     <row r="51" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="C51" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D51" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="E51" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="F51" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="G51" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="H51" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="I51" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="J51" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="K51" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="L51" s="6" t="s">
+        <v>242</v>
+      </c>
+      <c r="M51" s="5" t="s">
         <v>243</v>
-      </c>
-      <c r="E51" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="F51" s="5" t="s">
-        <v>244</v>
-      </c>
-      <c r="G51" s="5" t="s">
-        <v>245</v>
-      </c>
-      <c r="H51" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="I51" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="J51" s="5" t="s">
-        <v>246</v>
-      </c>
-      <c r="K51" s="5" t="s">
-        <v>273</v>
-      </c>
-      <c r="L51" s="6" t="s">
-        <v>247</v>
-      </c>
-      <c r="M51" s="5" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="C52" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="E52" s="5" t="s">
         <v>37</v>
       </c>
       <c r="F52" s="5" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="G52" s="5" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="H52" s="5" t="s">
         <v>18</v>
@@ -3280,13 +3298,13 @@
         <v>19</v>
       </c>
       <c r="J52" s="5" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="K52" s="5" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="L52" s="5" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="M52" s="5" t="s">
         <v>43</v>
@@ -3294,40 +3312,40 @@
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A53" s="5" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="C53" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D53" s="5" t="s">
+        <v>251</v>
+      </c>
+      <c r="E53" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="F53" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="G53" s="5" t="s">
+        <v>253</v>
+      </c>
+      <c r="H53" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I53" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J53" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="K53" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="L53" s="5" t="s">
         <v>256</v>
-      </c>
-      <c r="E53" s="5" t="s">
-        <v>225</v>
-      </c>
-      <c r="F53" s="5" t="s">
-        <v>257</v>
-      </c>
-      <c r="G53" s="5" t="s">
-        <v>258</v>
-      </c>
-      <c r="H53" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I53" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J53" s="5" t="s">
-        <v>259</v>
-      </c>
-      <c r="K53" s="5" t="s">
-        <v>260</v>
-      </c>
-      <c r="L53" s="5" t="s">
-        <v>261</v>
       </c>
       <c r="M53" s="5" t="s">
         <v>43</v>
@@ -3335,40 +3353,40 @@
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A54" s="5" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="C54" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="E54" s="5" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="F54" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="G54" s="5" t="s">
+        <v>253</v>
+      </c>
+      <c r="H54" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I54" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J54" s="5" t="s">
         <v>257</v>
       </c>
-      <c r="G54" s="5" t="s">
+      <c r="K54" s="5" t="s">
         <v>258</v>
       </c>
-      <c r="H54" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I54" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J54" s="5" t="s">
-        <v>262</v>
-      </c>
-      <c r="K54" s="5" t="s">
-        <v>263</v>
-      </c>
       <c r="L54" s="5" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="M54" s="5" t="s">
         <v>43</v>

</xml_diff>

<commit_message>
Update Link Site UPD104
</commit_message>
<xml_diff>
--- a/data/premium-sites.xlsx
+++ b/data/premium-sites.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Local Repository\Telkom Projects\monitoring-site-premium-telegram-bot\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A2846CE-5F51-4E25-B100-39DD94CCF75D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43350C98-8436-4341-8AC0-83C7708053C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="670" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="696" uniqueCount="289">
   <si>
     <t>Subdistrict</t>
   </si>
@@ -861,6 +861,45 @@
   </si>
   <si>
     <t>GigabitEthernet0/8/3 current state : UP</t>
+  </si>
+  <si>
+    <t>L2SW RAISECOM</t>
+  </si>
+  <si>
+    <t>L2SW-D7-UPD104</t>
+  </si>
+  <si>
+    <t>10.198.5.6</t>
+  </si>
+  <si>
+    <t>raisecom</t>
+  </si>
+  <si>
+    <t>tengigabitethernet 1/1/25</t>
+  </si>
+  <si>
+    <t>101625004100A24409A0092G</t>
+  </si>
+  <si>
+    <t>show interface tengigabitethernet 1/1/25</t>
+  </si>
+  <si>
+    <t>tengigabitethernet1/1/25 is UP, administrative status is UP</t>
+  </si>
+  <si>
+    <t>tengigabitethernet 1/1/26</t>
+  </si>
+  <si>
+    <t>show interface tengigabitethernet 1/1/26</t>
+  </si>
+  <si>
+    <t>tengigabitethernet1/1/26 is UP, administrative status is UP</t>
+  </si>
+  <si>
+    <t>Link 4</t>
+  </si>
+  <si>
+    <t>Link 5</t>
   </si>
 </sst>
 </file>
@@ -1198,10 +1237,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AG54"/>
+  <dimension ref="A1:AG56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1215,10 +1254,10 @@
     <col min="7" max="7" width="13.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23" style="1" customWidth="1"/>
+    <col min="10" max="10" width="22.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="50.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="32.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="49.21875" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="33" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
@@ -1365,7 +1404,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:33" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>11</v>
       </c>
@@ -1379,31 +1418,31 @@
         <v>29</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>30</v>
+        <v>276</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>31</v>
+        <v>277</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>32</v>
+        <v>278</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>18</v>
+        <v>279</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>19</v>
+        <v>279</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>33</v>
+        <v>280</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>34</v>
+        <v>281</v>
       </c>
       <c r="L4" s="6" t="s">
-        <v>35</v>
+        <v>282</v>
       </c>
       <c r="M4" s="5" t="s">
-        <v>36</v>
+        <v>283</v>
       </c>
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.3">
@@ -1420,34 +1459,34 @@
         <v>29</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>37</v>
+        <v>276</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>38</v>
+        <v>277</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>39</v>
+        <v>278</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>18</v>
+        <v>279</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>19</v>
+        <v>279</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>40</v>
+        <v>284</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>41</v>
+        <v>281</v>
       </c>
       <c r="L5" s="5" t="s">
-        <v>42</v>
+        <v>285</v>
       </c>
       <c r="M5" s="5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.3">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>11</v>
       </c>
@@ -1461,13 +1500,13 @@
         <v>29</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="H6" s="5" t="s">
         <v>18</v>
@@ -1476,16 +1515,16 @@
         <v>19</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="L6" s="5" t="s">
-        <v>48</v>
+        <v>34</v>
+      </c>
+      <c r="L6" s="6" t="s">
+        <v>35</v>
       </c>
       <c r="M6" s="5" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:33" x14ac:dyDescent="0.3">
@@ -1493,22 +1532,22 @@
         <v>11</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>49</v>
+        <v>28</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>13</v>
+        <v>287</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="H7" s="5" t="s">
         <v>18</v>
@@ -1517,16 +1556,16 @@
         <v>19</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="K7" s="5" t="s">
-        <v>261</v>
+        <v>41</v>
       </c>
       <c r="L7" s="5" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="M7" s="5" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:33" x14ac:dyDescent="0.3">
@@ -1534,63 +1573,63 @@
         <v>11</v>
       </c>
       <c r="B8" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="K8" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="L8" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="M8" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>49</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="H8" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I8" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J8" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="K8" s="5" t="s">
-        <v>261</v>
-      </c>
-      <c r="L8" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="M8" s="5" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="9" spans="1:33" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>60</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="H9" s="5" t="s">
         <v>18</v>
@@ -1599,64 +1638,80 @@
         <v>19</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="L9" s="6" t="s">
-        <v>67</v>
+        <v>261</v>
+      </c>
+      <c r="L9" s="5" t="s">
+        <v>55</v>
       </c>
       <c r="M9" s="5" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
-        <v>59</v>
+        <v>11</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="5"/>
-      <c r="L10" s="5"/>
-      <c r="M10" s="5"/>
-    </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="K10" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="L10" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="M10" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:33" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>59</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>15</v>
+        <v>62</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>16</v>
+        <v>63</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>17</v>
+        <v>64</v>
       </c>
       <c r="H11" s="5" t="s">
         <v>18</v>
@@ -1665,16 +1720,16 @@
         <v>19</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>270</v>
+        <v>65</v>
       </c>
       <c r="K11" s="5" t="s">
-        <v>21</v>
+        <v>66</v>
       </c>
       <c r="L11" s="6" t="s">
-        <v>271</v>
+        <v>67</v>
       </c>
       <c r="M11" s="5" t="s">
-        <v>272</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:33" x14ac:dyDescent="0.3">
@@ -1682,204 +1737,188 @@
         <v>59</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="G12" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H12" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I12" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J12" s="5" t="s">
-        <v>273</v>
-      </c>
-      <c r="K12" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="L12" s="5" t="s">
-        <v>274</v>
-      </c>
-      <c r="M12" s="5" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="13" spans="1:33" ht="28.8" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="5"/>
+    </row>
+    <row r="13" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>75</v>
+        <v>15</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>76</v>
+        <v>16</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>77</v>
+        <v>17</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>78</v>
+        <v>18</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>78</v>
+        <v>19</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>79</v>
+        <v>270</v>
       </c>
       <c r="K13" s="5" t="s">
-        <v>262</v>
+        <v>21</v>
       </c>
       <c r="L13" s="6" t="s">
-        <v>80</v>
+        <v>271</v>
       </c>
       <c r="M13" s="5" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="14" spans="1:33" ht="28.8" x14ac:dyDescent="0.3">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="14" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>75</v>
+        <v>15</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>76</v>
+        <v>16</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>77</v>
+        <v>17</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>78</v>
+        <v>18</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>78</v>
+        <v>19</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>82</v>
+        <v>273</v>
       </c>
       <c r="K14" s="5" t="s">
-        <v>262</v>
-      </c>
-      <c r="L14" s="6" t="s">
-        <v>83</v>
+        <v>21</v>
+      </c>
+      <c r="L14" s="5" t="s">
+        <v>274</v>
       </c>
       <c r="M14" s="5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.3">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="15" spans="1:33" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>72</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>51</v>
+        <v>75</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>263</v>
+        <v>78</v>
       </c>
       <c r="J15" s="5" t="s">
-        <v>54</v>
+        <v>79</v>
       </c>
       <c r="K15" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="L15" s="5" t="s">
-        <v>55</v>
+        <v>262</v>
+      </c>
+      <c r="L15" s="6" t="s">
+        <v>80</v>
       </c>
       <c r="M15" s="5" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="16" spans="1:33" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>72</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>51</v>
+        <v>75</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>263</v>
+        <v>78</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>57</v>
+        <v>82</v>
       </c>
       <c r="K16" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="L16" s="5" t="s">
-        <v>58</v>
+        <v>262</v>
+      </c>
+      <c r="L16" s="6" t="s">
+        <v>83</v>
       </c>
       <c r="M16" s="5" t="s">
-        <v>56</v>
+        <v>84</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
@@ -1887,22 +1926,22 @@
         <v>72</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="H17" s="5" t="s">
         <v>89</v>
@@ -1911,13 +1950,13 @@
         <v>263</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>95</v>
+        <v>54</v>
       </c>
       <c r="K17" s="5" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="L17" s="5" t="s">
-        <v>97</v>
+        <v>55</v>
       </c>
       <c r="M17" s="5" t="s">
         <v>56</v>
@@ -1928,22 +1967,22 @@
         <v>72</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="H18" s="5" t="s">
         <v>89</v>
@@ -1952,13 +1991,13 @@
         <v>263</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>98</v>
+        <v>57</v>
       </c>
       <c r="K18" s="5" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="L18" s="5" t="s">
-        <v>99</v>
+        <v>58</v>
       </c>
       <c r="M18" s="5" t="s">
         <v>56</v>
@@ -1969,40 +2008,40 @@
         <v>72</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>15</v>
+        <v>51</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>18</v>
+        <v>89</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>19</v>
+        <v>263</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="K19" s="5" t="s">
-        <v>21</v>
+        <v>96</v>
       </c>
       <c r="L19" s="5" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="M19" s="5" t="s">
-        <v>106</v>
+        <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
@@ -2010,63 +2049,63 @@
         <v>72</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>15</v>
+        <v>51</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>18</v>
+        <v>89</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>19</v>
+        <v>263</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="K20" s="5" t="s">
-        <v>21</v>
+        <v>96</v>
       </c>
       <c r="L20" s="5" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="M20" s="5" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>72</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
       <c r="H21" s="5" t="s">
         <v>18</v>
@@ -2075,16 +2114,16 @@
         <v>19</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>264</v>
+        <v>104</v>
       </c>
       <c r="K21" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="L21" s="6" t="s">
-        <v>117</v>
+        <v>21</v>
+      </c>
+      <c r="L21" s="5" t="s">
+        <v>105</v>
       </c>
       <c r="M21" s="5" t="s">
-        <v>36</v>
+        <v>106</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
@@ -2092,47 +2131,63 @@
         <v>72</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="5"/>
-      <c r="J22" s="5"/>
-      <c r="K22" s="5"/>
-      <c r="L22" s="5"/>
-      <c r="M22" s="5"/>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="H22" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I22" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J22" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="K22" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="L22" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="M22" s="5" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
-        <v>118</v>
+        <v>72</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>121</v>
+        <v>30</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="H23" s="5" t="s">
         <v>18</v>
@@ -2141,98 +2196,82 @@
         <v>19</v>
       </c>
       <c r="J23" s="5" t="s">
-        <v>124</v>
+        <v>264</v>
       </c>
       <c r="K23" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="L23" s="5" t="s">
-        <v>126</v>
+        <v>116</v>
+      </c>
+      <c r="L23" s="6" t="s">
+        <v>117</v>
       </c>
       <c r="M23" s="5" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
-        <v>118</v>
+        <v>72</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="F24" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="G24" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="H24" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I24" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J24" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="K24" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="L24" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="M24" s="5" t="s">
-        <v>43</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="5"/>
+      <c r="J24" s="5"/>
+      <c r="K24" s="5"/>
+      <c r="L24" s="5"/>
+      <c r="M24" s="5"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
         <v>118</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>51</v>
+        <v>121</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="H25" s="5" t="s">
-        <v>89</v>
+        <v>18</v>
       </c>
       <c r="I25" s="5" t="s">
-        <v>263</v>
+        <v>19</v>
       </c>
       <c r="J25" s="5" t="s">
-        <v>54</v>
+        <v>124</v>
       </c>
       <c r="K25" s="5" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="L25" s="5" t="s">
-        <v>55</v>
+        <v>126</v>
       </c>
       <c r="M25" s="5" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
@@ -2240,81 +2279,81 @@
         <v>118</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>51</v>
+        <v>121</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>89</v>
+        <v>18</v>
       </c>
       <c r="I26" s="5" t="s">
-        <v>263</v>
+        <v>19</v>
       </c>
       <c r="J26" s="5" t="s">
-        <v>57</v>
+        <v>129</v>
       </c>
       <c r="K26" s="5" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="L26" s="5" t="s">
-        <v>58</v>
+        <v>130</v>
       </c>
       <c r="M26" s="5" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
         <v>118</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>18</v>
+        <v>89</v>
       </c>
       <c r="I27" s="5" t="s">
-        <v>19</v>
+        <v>263</v>
       </c>
       <c r="J27" s="5" t="s">
-        <v>140</v>
+        <v>54</v>
       </c>
       <c r="K27" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="L27" s="6" t="s">
-        <v>142</v>
+        <v>135</v>
+      </c>
+      <c r="L27" s="5" t="s">
+        <v>55</v>
       </c>
       <c r="M27" s="5" t="s">
-        <v>36</v>
+        <v>56</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
@@ -2322,47 +2361,63 @@
         <v>118</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="F28" s="5"/>
-      <c r="G28" s="5"/>
-      <c r="H28" s="5"/>
-      <c r="I28" s="5"/>
-      <c r="J28" s="5"/>
-      <c r="K28" s="5"/>
-      <c r="L28" s="5"/>
-      <c r="M28" s="5"/>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="G28" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="H28" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="I28" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="J28" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="K28" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="L28" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="M28" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
         <v>118</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>122</v>
+        <v>138</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>123</v>
+        <v>139</v>
       </c>
       <c r="H29" s="5" t="s">
         <v>18</v>
@@ -2371,16 +2426,16 @@
         <v>19</v>
       </c>
       <c r="J29" s="5" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="K29" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="L29" s="5" t="s">
-        <v>147</v>
+        <v>141</v>
+      </c>
+      <c r="L29" s="6" t="s">
+        <v>142</v>
       </c>
       <c r="M29" s="5" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
@@ -2388,54 +2443,38 @@
         <v>118</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="F30" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="G30" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="H30" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I30" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J30" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="K30" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="L30" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="M30" s="5" t="s">
-        <v>43</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
+      <c r="H30" s="5"/>
+      <c r="I30" s="5"/>
+      <c r="J30" s="5"/>
+      <c r="K30" s="5"/>
+      <c r="L30" s="5"/>
+      <c r="M30" s="5"/>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
         <v>118</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="C31" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="E31" s="5" t="s">
         <v>37</v>
@@ -2453,13 +2492,13 @@
         <v>19</v>
       </c>
       <c r="J31" s="5" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="K31" s="5" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="L31" s="5" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="M31" s="5" t="s">
         <v>43</v>
@@ -2470,13 +2509,13 @@
         <v>118</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="C32" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="E32" s="5" t="s">
         <v>37</v>
@@ -2494,13 +2533,13 @@
         <v>19</v>
       </c>
       <c r="J32" s="5" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="K32" s="5" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="L32" s="5" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="M32" s="5" t="s">
         <v>43</v>
@@ -2508,25 +2547,25 @@
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
-        <v>157</v>
+        <v>118</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="C33" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>160</v>
+        <v>37</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>161</v>
+        <v>122</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>162</v>
+        <v>123</v>
       </c>
       <c r="H33" s="5" t="s">
         <v>18</v>
@@ -2535,39 +2574,39 @@
         <v>19</v>
       </c>
       <c r="J33" s="5" t="s">
-        <v>54</v>
+        <v>152</v>
       </c>
       <c r="K33" s="5" t="s">
-        <v>265</v>
+        <v>153</v>
       </c>
       <c r="L33" s="5" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="M33" s="5" t="s">
-        <v>164</v>
+        <v>43</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
-        <v>157</v>
+        <v>118</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="C34" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>160</v>
+        <v>37</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>161</v>
+        <v>127</v>
       </c>
       <c r="G34" s="5" t="s">
-        <v>162</v>
+        <v>128</v>
       </c>
       <c r="H34" s="5" t="s">
         <v>18</v>
@@ -2576,39 +2615,39 @@
         <v>19</v>
       </c>
       <c r="J34" s="5" t="s">
-        <v>57</v>
+        <v>155</v>
       </c>
       <c r="K34" s="5" t="s">
-        <v>265</v>
+        <v>153</v>
       </c>
       <c r="L34" s="5" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="M34" s="5" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
         <v>157</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C35" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>30</v>
+        <v>160</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="H35" s="5" t="s">
         <v>18</v>
@@ -2617,16 +2656,16 @@
         <v>19</v>
       </c>
       <c r="J35" s="5" t="s">
-        <v>266</v>
+        <v>54</v>
       </c>
       <c r="K35" s="5" t="s">
-        <v>170</v>
-      </c>
-      <c r="L35" s="6" t="s">
-        <v>171</v>
+        <v>265</v>
+      </c>
+      <c r="L35" s="5" t="s">
+        <v>163</v>
       </c>
       <c r="M35" s="5" t="s">
-        <v>36</v>
+        <v>164</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.3">
@@ -2634,47 +2673,63 @@
         <v>157</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C36" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="F36" s="5"/>
-      <c r="G36" s="5"/>
-      <c r="H36" s="5"/>
-      <c r="I36" s="5"/>
-      <c r="J36" s="5"/>
-      <c r="K36" s="5"/>
-      <c r="L36" s="5"/>
-      <c r="M36" s="5"/>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+        <v>160</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="G36" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="H36" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I36" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J36" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="K36" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="L36" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="M36" s="5" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
         <v>157</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="C37" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="H37" s="5" t="s">
         <v>18</v>
@@ -2683,16 +2738,16 @@
         <v>19</v>
       </c>
       <c r="J37" s="5" t="s">
-        <v>176</v>
+        <v>266</v>
       </c>
       <c r="K37" s="5" t="s">
-        <v>177</v>
-      </c>
-      <c r="L37" s="5" t="s">
-        <v>178</v>
+        <v>170</v>
+      </c>
+      <c r="L37" s="6" t="s">
+        <v>171</v>
       </c>
       <c r="M37" s="5" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.3">
@@ -2700,63 +2755,47 @@
         <v>157</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="F38" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="G38" s="5" t="s">
-        <v>180</v>
-      </c>
-      <c r="H38" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I38" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J38" s="5" t="s">
-        <v>181</v>
-      </c>
-      <c r="K38" s="5" t="s">
-        <v>177</v>
-      </c>
-      <c r="L38" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="M38" s="5" t="s">
-        <v>43</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="F38" s="5"/>
+      <c r="G38" s="5"/>
+      <c r="H38" s="5"/>
+      <c r="I38" s="5"/>
+      <c r="J38" s="5"/>
+      <c r="K38" s="5"/>
+      <c r="L38" s="5"/>
+      <c r="M38" s="5"/>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
         <v>157</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="E39" s="5" t="s">
         <v>37</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="H39" s="5" t="s">
         <v>18</v>
@@ -2765,13 +2804,13 @@
         <v>19</v>
       </c>
       <c r="J39" s="5" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="K39" s="5" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
       <c r="L39" s="5" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="M39" s="5" t="s">
         <v>43</v>
@@ -2782,22 +2821,22 @@
         <v>157</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="C40" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="E40" s="5" t="s">
         <v>37</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="G40" s="5" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
       <c r="H40" s="5" t="s">
         <v>18</v>
@@ -2806,13 +2845,13 @@
         <v>19</v>
       </c>
       <c r="J40" s="5" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="K40" s="5" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
       <c r="L40" s="5" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="M40" s="5" t="s">
         <v>43</v>
@@ -2823,22 +2862,22 @@
         <v>157</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="C41" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="E41" s="5" t="s">
         <v>37</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
       <c r="H41" s="5" t="s">
         <v>18</v>
@@ -2847,13 +2886,13 @@
         <v>19</v>
       </c>
       <c r="J41" s="5" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
       <c r="K41" s="5" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="L41" s="5" t="s">
-        <v>200</v>
+        <v>189</v>
       </c>
       <c r="M41" s="5" t="s">
         <v>43</v>
@@ -2864,22 +2903,22 @@
         <v>157</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="C42" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="E42" s="5" t="s">
         <v>37</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="G42" s="5" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="H42" s="5" t="s">
         <v>18</v>
@@ -2888,13 +2927,13 @@
         <v>19</v>
       </c>
       <c r="J42" s="5" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="K42" s="5" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="L42" s="5" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="M42" s="5" t="s">
         <v>43</v>
@@ -2905,40 +2944,40 @@
         <v>157</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="C43" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="H43" s="5" t="s">
-        <v>89</v>
+        <v>18</v>
       </c>
       <c r="I43" s="5" t="s">
-        <v>263</v>
+        <v>19</v>
       </c>
       <c r="J43" s="5" t="s">
-        <v>54</v>
+        <v>198</v>
       </c>
       <c r="K43" s="5" t="s">
-        <v>267</v>
+        <v>199</v>
       </c>
       <c r="L43" s="5" t="s">
-        <v>55</v>
+        <v>200</v>
       </c>
       <c r="M43" s="5" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.3">
@@ -2946,122 +2985,122 @@
         <v>157</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="C44" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="G44" s="5" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="H44" s="5" t="s">
-        <v>89</v>
+        <v>18</v>
       </c>
       <c r="I44" s="5" t="s">
-        <v>263</v>
+        <v>19</v>
       </c>
       <c r="J44" s="5" t="s">
-        <v>57</v>
+        <v>201</v>
       </c>
       <c r="K44" s="5" t="s">
-        <v>267</v>
+        <v>199</v>
       </c>
       <c r="L44" s="5" t="s">
-        <v>58</v>
+        <v>202</v>
       </c>
       <c r="M44" s="5" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
-        <v>207</v>
+        <v>157</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="C45" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>15</v>
+        <v>51</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="G45" s="5" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="H45" s="5" t="s">
-        <v>18</v>
+        <v>89</v>
       </c>
       <c r="I45" s="5" t="s">
-        <v>19</v>
+        <v>263</v>
       </c>
       <c r="J45" s="5" t="s">
-        <v>212</v>
+        <v>54</v>
       </c>
       <c r="K45" s="5" t="s">
-        <v>21</v>
+        <v>267</v>
       </c>
       <c r="L45" s="5" t="s">
-        <v>213</v>
+        <v>55</v>
       </c>
       <c r="M45" s="5" t="s">
-        <v>214</v>
+        <v>56</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46" s="5" t="s">
-        <v>207</v>
+        <v>157</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="C46" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>15</v>
+        <v>51</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="G46" s="5" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="H46" s="5" t="s">
-        <v>18</v>
+        <v>89</v>
       </c>
       <c r="I46" s="5" t="s">
-        <v>19</v>
+        <v>263</v>
       </c>
       <c r="J46" s="5" t="s">
-        <v>215</v>
+        <v>57</v>
       </c>
       <c r="K46" s="5" t="s">
-        <v>21</v>
+        <v>267</v>
       </c>
       <c r="L46" s="5" t="s">
-        <v>216</v>
+        <v>58</v>
       </c>
       <c r="M46" s="5" t="s">
-        <v>217</v>
+        <v>56</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.3">
@@ -3069,22 +3108,22 @@
         <v>207</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
       <c r="C47" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>220</v>
+        <v>15</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>221</v>
+        <v>210</v>
       </c>
       <c r="G47" s="5" t="s">
-        <v>222</v>
+        <v>211</v>
       </c>
       <c r="H47" s="5" t="s">
         <v>18</v>
@@ -3093,16 +3132,16 @@
         <v>19</v>
       </c>
       <c r="J47" s="5" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="K47" s="5" t="s">
-        <v>224</v>
+        <v>21</v>
       </c>
       <c r="L47" s="5" t="s">
-        <v>225</v>
+        <v>213</v>
       </c>
       <c r="M47" s="5" t="s">
-        <v>43</v>
+        <v>214</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.3">
@@ -3110,22 +3149,22 @@
         <v>207</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
       <c r="C48" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>220</v>
+        <v>15</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>226</v>
+        <v>210</v>
       </c>
       <c r="G48" s="5" t="s">
-        <v>227</v>
+        <v>211</v>
       </c>
       <c r="H48" s="5" t="s">
         <v>18</v>
@@ -3134,16 +3173,16 @@
         <v>19</v>
       </c>
       <c r="J48" s="5" t="s">
-        <v>228</v>
+        <v>215</v>
       </c>
       <c r="K48" s="5" t="s">
-        <v>224</v>
+        <v>21</v>
       </c>
       <c r="L48" s="5" t="s">
-        <v>229</v>
+        <v>216</v>
       </c>
       <c r="M48" s="5" t="s">
-        <v>43</v>
+        <v>217</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.3">
@@ -3151,13 +3190,13 @@
         <v>207</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>230</v>
+        <v>218</v>
       </c>
       <c r="C49" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>231</v>
+        <v>219</v>
       </c>
       <c r="E49" s="5" t="s">
         <v>220</v>
@@ -3175,13 +3214,13 @@
         <v>19</v>
       </c>
       <c r="J49" s="5" t="s">
-        <v>232</v>
+        <v>223</v>
       </c>
       <c r="K49" s="5" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="L49" s="5" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="M49" s="5" t="s">
         <v>43</v>
@@ -3192,13 +3231,13 @@
         <v>207</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>230</v>
+        <v>218</v>
       </c>
       <c r="C50" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>231</v>
+        <v>219</v>
       </c>
       <c r="E50" s="5" t="s">
         <v>220</v>
@@ -3216,57 +3255,57 @@
         <v>19</v>
       </c>
       <c r="J50" s="5" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="K50" s="5" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="L50" s="5" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="M50" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="51" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
         <v>207</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="C51" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>75</v>
+        <v>220</v>
       </c>
       <c r="F51" s="5" t="s">
-        <v>239</v>
+        <v>221</v>
       </c>
       <c r="G51" s="5" t="s">
-        <v>240</v>
+        <v>222</v>
       </c>
       <c r="H51" s="5" t="s">
-        <v>78</v>
+        <v>18</v>
       </c>
       <c r="I51" s="5" t="s">
-        <v>78</v>
+        <v>19</v>
       </c>
       <c r="J51" s="5" t="s">
-        <v>241</v>
+        <v>232</v>
       </c>
       <c r="K51" s="5" t="s">
-        <v>268</v>
-      </c>
-      <c r="L51" s="6" t="s">
-        <v>242</v>
+        <v>233</v>
+      </c>
+      <c r="L51" s="5" t="s">
+        <v>234</v>
       </c>
       <c r="M51" s="5" t="s">
-        <v>243</v>
+        <v>43</v>
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.3">
@@ -3274,22 +3313,22 @@
         <v>207</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="C52" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>37</v>
+        <v>220</v>
       </c>
       <c r="F52" s="5" t="s">
-        <v>244</v>
+        <v>226</v>
       </c>
       <c r="G52" s="5" t="s">
-        <v>245</v>
+        <v>227</v>
       </c>
       <c r="H52" s="5" t="s">
         <v>18</v>
@@ -3298,97 +3337,179 @@
         <v>19</v>
       </c>
       <c r="J52" s="5" t="s">
-        <v>246</v>
+        <v>235</v>
       </c>
       <c r="K52" s="5" t="s">
-        <v>247</v>
+        <v>233</v>
       </c>
       <c r="L52" s="5" t="s">
-        <v>248</v>
+        <v>236</v>
       </c>
       <c r="M52" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A53" s="5" t="s">
-        <v>249</v>
+        <v>207</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>250</v>
+        <v>237</v>
       </c>
       <c r="C53" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>251</v>
+        <v>238</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>220</v>
+        <v>75</v>
       </c>
       <c r="F53" s="5" t="s">
-        <v>252</v>
+        <v>239</v>
       </c>
       <c r="G53" s="5" t="s">
-        <v>253</v>
+        <v>240</v>
       </c>
       <c r="H53" s="5" t="s">
-        <v>18</v>
+        <v>78</v>
       </c>
       <c r="I53" s="5" t="s">
-        <v>19</v>
+        <v>78</v>
       </c>
       <c r="J53" s="5" t="s">
-        <v>254</v>
+        <v>241</v>
       </c>
       <c r="K53" s="5" t="s">
-        <v>255</v>
-      </c>
-      <c r="L53" s="5" t="s">
-        <v>256</v>
+        <v>268</v>
+      </c>
+      <c r="L53" s="6" t="s">
+        <v>242</v>
       </c>
       <c r="M53" s="5" t="s">
-        <v>43</v>
+        <v>243</v>
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A54" s="5" t="s">
-        <v>249</v>
+        <v>207</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>250</v>
+        <v>237</v>
       </c>
       <c r="C54" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D54" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="E54" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F54" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="G54" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="H54" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I54" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J54" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="K54" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="L54" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="M54" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A55" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="C55" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D55" s="5" t="s">
         <v>251</v>
       </c>
-      <c r="E54" s="5" t="s">
+      <c r="E55" s="5" t="s">
         <v>220</v>
       </c>
-      <c r="F54" s="5" t="s">
+      <c r="F55" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="G54" s="5" t="s">
+      <c r="G55" s="5" t="s">
         <v>253</v>
       </c>
-      <c r="H54" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I54" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J54" s="5" t="s">
+      <c r="H55" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I55" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J55" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="K55" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="L55" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="M55" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A56" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="C56" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D56" s="5" t="s">
+        <v>251</v>
+      </c>
+      <c r="E56" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="F56" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="G56" s="5" t="s">
+        <v>253</v>
+      </c>
+      <c r="H56" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I56" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J56" s="5" t="s">
         <v>257</v>
       </c>
-      <c r="K54" s="5" t="s">
+      <c r="K56" s="5" t="s">
         <v>258</v>
       </c>
-      <c r="L54" s="5" t="s">
+      <c r="L56" s="5" t="s">
         <v>259</v>
       </c>
-      <c r="M54" s="5" t="s">
+      <c r="M56" s="5" t="s">
         <v>43</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Site Premium UNH001
</commit_message>
<xml_diff>
--- a/data/premium-sites.xlsx
+++ b/data/premium-sites.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Local Repository\Telkom Projects\monitoring-site-premium-telegram-bot\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43350C98-8436-4341-8AC0-83C7708053C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C59CA81C-DE63-4E1C-BE89-B1CB057C3BB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="696" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="704" uniqueCount="288">
   <si>
     <t>Subdistrict</t>
   </si>
@@ -373,19 +373,6 @@
     <t>UNAAHA</t>
   </si>
   <si>
-    <t>GPON03-D7-UNH-4</t>
-  </si>
-  <si>
-    <t>172.25.230.161</t>
-  </si>
-  <si>
-    <t>FHTT05e9e531</t>
-  </si>
-  <si>
-    <t>config
-show authorization 1/3/7 | include FHTT05e9e531</t>
-  </si>
-  <si>
     <t>SULTENG</t>
   </si>
   <si>
@@ -827,9 +814,6 @@
     <t>12345</t>
   </si>
   <si>
-    <t>3/7/50</t>
-  </si>
-  <si>
     <t>121526160016</t>
   </si>
   <si>
@@ -900,6 +884,18 @@
   </si>
   <si>
     <t>Link 5</t>
+  </si>
+  <si>
+    <t>SW-D7-UNH001</t>
+  </si>
+  <si>
+    <t>10.199.107.90</t>
+  </si>
+  <si>
+    <t>Telkom135</t>
+  </si>
+  <si>
+    <t>NYUKWIB10260</t>
   </si>
 </sst>
 </file>
@@ -1239,8 +1235,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1290,10 +1286,10 @@
         <v>8</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="L1" s="4" t="s">
         <v>9</v>
@@ -1418,31 +1414,31 @@
         <v>29</v>
       </c>
       <c r="E4" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="K4" s="5" t="s">
         <v>276</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="L4" s="6" t="s">
         <v>277</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="M4" s="5" t="s">
         <v>278</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>279</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>279</v>
-      </c>
-      <c r="J4" s="5" t="s">
-        <v>280</v>
-      </c>
-      <c r="K4" s="5" t="s">
-        <v>281</v>
-      </c>
-      <c r="L4" s="6" t="s">
-        <v>282</v>
-      </c>
-      <c r="M4" s="5" t="s">
-        <v>283</v>
       </c>
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.3">
@@ -1459,31 +1455,31 @@
         <v>29</v>
       </c>
       <c r="E5" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="K5" s="5" t="s">
         <v>276</v>
       </c>
-      <c r="F5" s="5" t="s">
-        <v>277</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>278</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>279</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>279</v>
-      </c>
-      <c r="J5" s="5" t="s">
-        <v>284</v>
-      </c>
-      <c r="K5" s="5" t="s">
+      <c r="L5" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="M5" s="5" t="s">
         <v>281</v>
-      </c>
-      <c r="L5" s="5" t="s">
-        <v>285</v>
-      </c>
-      <c r="M5" s="5" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="6" spans="1:33" ht="28.8" x14ac:dyDescent="0.3">
@@ -1535,7 +1531,7 @@
         <v>28</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>29</v>
@@ -1576,7 +1572,7 @@
         <v>28</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>29</v>
@@ -1641,7 +1637,7 @@
         <v>54</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="L9" s="5" t="s">
         <v>55</v>
@@ -1682,7 +1678,7 @@
         <v>57</v>
       </c>
       <c r="K10" s="5" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="L10" s="5" t="s">
         <v>58</v>
@@ -1786,16 +1782,16 @@
         <v>19</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="K13" s="5" t="s">
         <v>21</v>
       </c>
       <c r="L13" s="6" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="M13" s="5" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
     </row>
     <row r="14" spans="1:33" x14ac:dyDescent="0.3">
@@ -1827,16 +1823,16 @@
         <v>19</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="K14" s="5" t="s">
         <v>21</v>
       </c>
       <c r="L14" s="5" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="M14" s="5" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
     </row>
     <row r="15" spans="1:33" ht="28.8" x14ac:dyDescent="0.3">
@@ -1871,7 +1867,7 @@
         <v>79</v>
       </c>
       <c r="K15" s="5" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="L15" s="6" t="s">
         <v>80</v>
@@ -1912,7 +1908,7 @@
         <v>82</v>
       </c>
       <c r="K16" s="5" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="L16" s="6" t="s">
         <v>83</v>
@@ -1947,7 +1943,7 @@
         <v>89</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="J17" s="5" t="s">
         <v>54</v>
@@ -1988,7 +1984,7 @@
         <v>89</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="J18" s="5" t="s">
         <v>57</v>
@@ -2029,7 +2025,7 @@
         <v>89</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="J19" s="5" t="s">
         <v>95</v>
@@ -2070,7 +2066,7 @@
         <v>89</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="J20" s="5" t="s">
         <v>98</v>
@@ -2167,7 +2163,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
         <v>72</v>
       </c>
@@ -2181,31 +2177,31 @@
         <v>113</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>114</v>
+        <v>284</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>115</v>
+        <v>285</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>18</v>
+        <v>89</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>19</v>
+        <v>286</v>
       </c>
       <c r="J23" s="5" t="s">
-        <v>264</v>
+        <v>54</v>
       </c>
       <c r="K23" s="5" t="s">
-        <v>116</v>
+        <v>287</v>
       </c>
       <c r="L23" s="6" t="s">
-        <v>117</v>
+        <v>55</v>
       </c>
       <c r="M23" s="5" t="s">
-        <v>36</v>
+        <v>56</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
@@ -2222,53 +2218,69 @@
         <v>113</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
-      <c r="H24" s="5"/>
-      <c r="I24" s="5"/>
-      <c r="J24" s="5"/>
-      <c r="K24" s="5"/>
-      <c r="L24" s="5"/>
-      <c r="M24" s="5"/>
+        <v>51</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="H24" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="I24" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="J24" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="K24" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="L24" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="M24" s="5" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D25" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="H25" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I25" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J25" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="E25" s="5" t="s">
+      <c r="K25" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="F25" s="5" t="s">
+      <c r="L25" s="5" t="s">
         <v>122</v>
-      </c>
-      <c r="G25" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="H25" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I25" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J25" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="K25" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="L25" s="5" t="s">
-        <v>126</v>
       </c>
       <c r="M25" s="5" t="s">
         <v>43</v>
@@ -2276,40 +2288,40 @@
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="E26" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="G26" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="H26" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I26" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J26" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="K26" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="F26" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="G26" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="H26" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I26" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J26" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="K26" s="5" t="s">
-        <v>125</v>
-      </c>
       <c r="L26" s="5" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="M26" s="5" t="s">
         <v>43</v>
@@ -2317,37 +2329,37 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="E27" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="H27" s="5" t="s">
         <v>89</v>
       </c>
       <c r="I27" s="5" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="J27" s="5" t="s">
         <v>54</v>
       </c>
       <c r="K27" s="5" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="L27" s="5" t="s">
         <v>55</v>
@@ -2358,37 +2370,37 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="E28" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="H28" s="5" t="s">
         <v>89</v>
       </c>
       <c r="I28" s="5" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="J28" s="5" t="s">
         <v>57</v>
       </c>
       <c r="K28" s="5" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="L28" s="5" t="s">
         <v>58</v>
@@ -2399,40 +2411,40 @@
     </row>
     <row r="29" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="E29" s="5" t="s">
         <v>30</v>
       </c>
       <c r="F29" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="G29" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="H29" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I29" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J29" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="K29" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="L29" s="6" t="s">
         <v>138</v>
-      </c>
-      <c r="G29" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="H29" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I29" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J29" s="5" t="s">
-        <v>140</v>
-      </c>
-      <c r="K29" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="L29" s="6" t="s">
-        <v>142</v>
       </c>
       <c r="M29" s="5" t="s">
         <v>36</v>
@@ -2440,16 +2452,16 @@
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="E30" s="5" t="s">
         <v>69</v>
@@ -2465,25 +2477,25 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C31" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="E31" s="5" t="s">
         <v>37</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="H31" s="5" t="s">
         <v>18</v>
@@ -2492,13 +2504,13 @@
         <v>19</v>
       </c>
       <c r="J31" s="5" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="K31" s="5" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="L31" s="5" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="M31" s="5" t="s">
         <v>43</v>
@@ -2506,25 +2518,25 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C32" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="E32" s="5" t="s">
         <v>37</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="H32" s="5" t="s">
         <v>18</v>
@@ -2533,13 +2545,13 @@
         <v>19</v>
       </c>
       <c r="J32" s="5" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="K32" s="5" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="L32" s="5" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="M32" s="5" t="s">
         <v>43</v>
@@ -2547,25 +2559,25 @@
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C33" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="E33" s="5" t="s">
         <v>37</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="H33" s="5" t="s">
         <v>18</v>
@@ -2574,13 +2586,13 @@
         <v>19</v>
       </c>
       <c r="J33" s="5" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="K33" s="5" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="L33" s="5" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="M33" s="5" t="s">
         <v>43</v>
@@ -2588,25 +2600,25 @@
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C34" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="E34" s="5" t="s">
         <v>37</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="G34" s="5" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="H34" s="5" t="s">
         <v>18</v>
@@ -2615,13 +2627,13 @@
         <v>19</v>
       </c>
       <c r="J34" s="5" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="K34" s="5" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="L34" s="5" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="M34" s="5" t="s">
         <v>43</v>
@@ -2629,25 +2641,25 @@
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C35" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="H35" s="5" t="s">
         <v>18</v>
@@ -2659,36 +2671,36 @@
         <v>54</v>
       </c>
       <c r="K35" s="5" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="L35" s="5" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="M35" s="5" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C36" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="G36" s="5" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="H36" s="5" t="s">
         <v>18</v>
@@ -2700,36 +2712,36 @@
         <v>57</v>
       </c>
       <c r="K36" s="5" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="L36" s="5" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="M36" s="5" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="37" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C37" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="E37" s="5" t="s">
         <v>30</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="H37" s="5" t="s">
         <v>18</v>
@@ -2738,13 +2750,13 @@
         <v>19</v>
       </c>
       <c r="J37" s="5" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="K37" s="5" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="L37" s="6" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="M37" s="5" t="s">
         <v>36</v>
@@ -2752,16 +2764,16 @@
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="E38" s="5" t="s">
         <v>69</v>
@@ -2777,40 +2789,40 @@
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="E39" s="5" t="s">
         <v>37</v>
       </c>
       <c r="F39" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="G39" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="H39" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I39" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J39" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="K39" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="L39" s="5" t="s">
         <v>174</v>
-      </c>
-      <c r="G39" s="5" t="s">
-        <v>175</v>
-      </c>
-      <c r="H39" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I39" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J39" s="5" t="s">
-        <v>176</v>
-      </c>
-      <c r="K39" s="5" t="s">
-        <v>177</v>
-      </c>
-      <c r="L39" s="5" t="s">
-        <v>178</v>
       </c>
       <c r="M39" s="5" t="s">
         <v>43</v>
@@ -2818,25 +2830,25 @@
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C40" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="E40" s="5" t="s">
         <v>37</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="G40" s="5" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="H40" s="5" t="s">
         <v>18</v>
@@ -2845,13 +2857,13 @@
         <v>19</v>
       </c>
       <c r="J40" s="5" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="K40" s="5" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="L40" s="5" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="M40" s="5" t="s">
         <v>43</v>
@@ -2859,40 +2871,40 @@
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41" s="5" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C41" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="E41" s="5" t="s">
         <v>37</v>
       </c>
       <c r="F41" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="G41" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="H41" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I41" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J41" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="K41" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="L41" s="5" t="s">
         <v>185</v>
-      </c>
-      <c r="G41" s="5" t="s">
-        <v>186</v>
-      </c>
-      <c r="H41" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I41" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J41" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="K41" s="5" t="s">
-        <v>188</v>
-      </c>
-      <c r="L41" s="5" t="s">
-        <v>189</v>
       </c>
       <c r="M41" s="5" t="s">
         <v>43</v>
@@ -2900,25 +2912,25 @@
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C42" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="E42" s="5" t="s">
         <v>37</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="G42" s="5" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="H42" s="5" t="s">
         <v>18</v>
@@ -2927,13 +2939,13 @@
         <v>19</v>
       </c>
       <c r="J42" s="5" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="K42" s="5" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="L42" s="5" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="M42" s="5" t="s">
         <v>43</v>
@@ -2941,40 +2953,40 @@
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C43" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="E43" s="5" t="s">
         <v>37</v>
       </c>
       <c r="F43" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="G43" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="H43" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I43" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J43" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="K43" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="L43" s="5" t="s">
         <v>196</v>
-      </c>
-      <c r="G43" s="5" t="s">
-        <v>197</v>
-      </c>
-      <c r="H43" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I43" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J43" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="K43" s="5" t="s">
-        <v>199</v>
-      </c>
-      <c r="L43" s="5" t="s">
-        <v>200</v>
       </c>
       <c r="M43" s="5" t="s">
         <v>43</v>
@@ -2982,40 +2994,40 @@
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C44" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="E44" s="5" t="s">
         <v>37</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="G44" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="H44" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I44" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J44" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="H44" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I44" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J44" s="5" t="s">
-        <v>201</v>
-      </c>
       <c r="K44" s="5" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="L44" s="5" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="M44" s="5" t="s">
         <v>43</v>
@@ -3023,37 +3035,37 @@
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="C45" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="E45" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="G45" s="5" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="H45" s="5" t="s">
         <v>89</v>
       </c>
       <c r="I45" s="5" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="J45" s="5" t="s">
         <v>54</v>
       </c>
       <c r="K45" s="5" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="L45" s="5" t="s">
         <v>55</v>
@@ -3064,37 +3076,37 @@
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46" s="5" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="C46" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="E46" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="G46" s="5" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="H46" s="5" t="s">
         <v>89</v>
       </c>
       <c r="I46" s="5" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="J46" s="5" t="s">
         <v>57</v>
       </c>
       <c r="K46" s="5" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="L46" s="5" t="s">
         <v>58</v>
@@ -3105,25 +3117,25 @@
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A47" s="5" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="C47" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="E47" s="5" t="s">
         <v>15</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="G47" s="5" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="H47" s="5" t="s">
         <v>18</v>
@@ -3132,95 +3144,95 @@
         <v>19</v>
       </c>
       <c r="J47" s="5" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="K47" s="5" t="s">
         <v>21</v>
       </c>
       <c r="L47" s="5" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="M47" s="5" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="C48" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="E48" s="5" t="s">
         <v>15</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="G48" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="H48" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I48" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J48" s="5" t="s">
         <v>211</v>
-      </c>
-      <c r="H48" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I48" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J48" s="5" t="s">
-        <v>215</v>
       </c>
       <c r="K48" s="5" t="s">
         <v>21</v>
       </c>
       <c r="L48" s="5" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="M48" s="5" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="C49" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D49" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="E49" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="F49" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="G49" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="H49" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I49" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J49" s="5" t="s">
         <v>219</v>
       </c>
-      <c r="E49" s="5" t="s">
+      <c r="K49" s="5" t="s">
         <v>220</v>
       </c>
-      <c r="F49" s="5" t="s">
+      <c r="L49" s="5" t="s">
         <v>221</v>
-      </c>
-      <c r="G49" s="5" t="s">
-        <v>222</v>
-      </c>
-      <c r="H49" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I49" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J49" s="5" t="s">
-        <v>223</v>
-      </c>
-      <c r="K49" s="5" t="s">
-        <v>224</v>
-      </c>
-      <c r="L49" s="5" t="s">
-        <v>225</v>
       </c>
       <c r="M49" s="5" t="s">
         <v>43</v>
@@ -3228,40 +3240,40 @@
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="C50" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="E50" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="F50" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="G50" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="H50" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I50" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J50" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="K50" s="5" t="s">
         <v>220</v>
       </c>
-      <c r="F50" s="5" t="s">
-        <v>226</v>
-      </c>
-      <c r="G50" s="5" t="s">
-        <v>227</v>
-      </c>
-      <c r="H50" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I50" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J50" s="5" t="s">
-        <v>228</v>
-      </c>
-      <c r="K50" s="5" t="s">
-        <v>224</v>
-      </c>
       <c r="L50" s="5" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="M50" s="5" t="s">
         <v>43</v>
@@ -3269,25 +3281,25 @@
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="C51" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="F51" s="5" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="G51" s="5" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="H51" s="5" t="s">
         <v>18</v>
@@ -3296,13 +3308,13 @@
         <v>19</v>
       </c>
       <c r="J51" s="5" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="K51" s="5" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="L51" s="5" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="M51" s="5" t="s">
         <v>43</v>
@@ -3310,40 +3322,40 @@
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="C52" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D52" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="E52" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="F52" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="G52" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="H52" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I52" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J52" s="5" t="s">
         <v>231</v>
       </c>
-      <c r="E52" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="F52" s="5" t="s">
-        <v>226</v>
-      </c>
-      <c r="G52" s="5" t="s">
-        <v>227</v>
-      </c>
-      <c r="H52" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I52" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J52" s="5" t="s">
-        <v>235</v>
-      </c>
       <c r="K52" s="5" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="L52" s="5" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="M52" s="5" t="s">
         <v>43</v>
@@ -3351,25 +3363,25 @@
     </row>
     <row r="53" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A53" s="5" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="C53" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="E53" s="5" t="s">
         <v>75</v>
       </c>
       <c r="F53" s="5" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="G53" s="5" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="H53" s="5" t="s">
         <v>78</v>
@@ -3378,54 +3390,54 @@
         <v>78</v>
       </c>
       <c r="J53" s="5" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="K53" s="5" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="L53" s="6" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="M53" s="5" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A54" s="5" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="C54" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="E54" s="5" t="s">
         <v>37</v>
       </c>
       <c r="F54" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="G54" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="H54" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I54" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J54" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="K54" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="L54" s="5" t="s">
         <v>244</v>
-      </c>
-      <c r="G54" s="5" t="s">
-        <v>245</v>
-      </c>
-      <c r="H54" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I54" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J54" s="5" t="s">
-        <v>246</v>
-      </c>
-      <c r="K54" s="5" t="s">
-        <v>247</v>
-      </c>
-      <c r="L54" s="5" t="s">
-        <v>248</v>
       </c>
       <c r="M54" s="5" t="s">
         <v>43</v>
@@ -3433,40 +3445,40 @@
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A55" s="5" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="C55" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D55" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="E55" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="F55" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="G55" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="H55" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I55" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J55" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="K55" s="5" t="s">
         <v>251</v>
       </c>
-      <c r="E55" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="F55" s="5" t="s">
+      <c r="L55" s="5" t="s">
         <v>252</v>
-      </c>
-      <c r="G55" s="5" t="s">
-        <v>253</v>
-      </c>
-      <c r="H55" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I55" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J55" s="5" t="s">
-        <v>254</v>
-      </c>
-      <c r="K55" s="5" t="s">
-        <v>255</v>
-      </c>
-      <c r="L55" s="5" t="s">
-        <v>256</v>
       </c>
       <c r="M55" s="5" t="s">
         <v>43</v>
@@ -3474,40 +3486,40 @@
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A56" s="5" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="C56" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="E56" s="5" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="F56" s="5" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="G56" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="H56" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I56" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J56" s="5" t="s">
         <v>253</v>
       </c>
-      <c r="H56" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I56" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J56" s="5" t="s">
-        <v>257</v>
-      </c>
       <c r="K56" s="5" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="L56" s="5" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="M56" s="5" t="s">
         <v>43</v>

</xml_diff>

<commit_message>
Update Site Premium PAL016 Link 2
</commit_message>
<xml_diff>
--- a/data/premium-sites.xlsx
+++ b/data/premium-sites.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Local Repository\Telkom Projects\monitoring-site-premium-telegram-bot\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C59CA81C-DE63-4E1C-BE89-B1CB057C3BB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E8B0D38-26B6-4A60-AED5-0EFC46759E52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="704" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="712" uniqueCount="293">
   <si>
     <t>Subdistrict</t>
   </si>
@@ -896,6 +896,21 @@
   </si>
   <si>
     <t>NYUKWIB10260</t>
+  </si>
+  <si>
+    <t>GPON00-D7-TWL-3</t>
+  </si>
+  <si>
+    <t>172.25.209.120</t>
+  </si>
+  <si>
+    <t>1/6/12:50</t>
+  </si>
+  <si>
+    <t>ZTEG90089CC3</t>
+  </si>
+  <si>
+    <t>show gpon onu detail gpon-onu_1/6/12:50</t>
   </si>
 </sst>
 </file>
@@ -1235,8 +1250,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2464,16 +2479,32 @@
         <v>133</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="F30" s="5"/>
-      <c r="G30" s="5"/>
-      <c r="H30" s="5"/>
-      <c r="I30" s="5"/>
-      <c r="J30" s="5"/>
-      <c r="K30" s="5"/>
-      <c r="L30" s="5"/>
-      <c r="M30" s="5"/>
+        <v>37</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="G30" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="H30" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I30" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J30" s="5" t="s">
+        <v>290</v>
+      </c>
+      <c r="K30" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="L30" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="M30" s="5" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">

</xml_diff>

<commit_message>
Update Site Premium MDO004 Link 1 & Link 2
</commit_message>
<xml_diff>
--- a/data/premium-sites.xlsx
+++ b/data/premium-sites.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Local Repository\Telkom Projects\monitoring-site-premium-telegram-bot\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E8B0D38-26B6-4A60-AED5-0EFC46759E52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61A5313A-EEDC-4A67-A73A-CF0CCD5732AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="712" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="293">
   <si>
     <t>Subdistrict</t>
   </si>
@@ -524,19 +524,6 @@
     <t>Hiltop</t>
   </si>
   <si>
-    <t>GPON11-D7-MDO-4</t>
-  </si>
-  <si>
-    <t>172.27.227.223</t>
-  </si>
-  <si>
-    <t>FHTT05e9bb83</t>
-  </si>
-  <si>
-    <t>config
-show authorization 1/13/9 | include FHTT05e9bb83</t>
-  </si>
-  <si>
     <t>MDO029</t>
   </si>
   <si>
@@ -817,9 +804,6 @@
     <t>121526160016</t>
   </si>
   <si>
-    <t>13/9/50</t>
-  </si>
-  <si>
     <t>121502990017</t>
   </si>
   <si>
@@ -911,6 +895,21 @@
   </si>
   <si>
     <t>show gpon onu detail gpon-onu_1/6/12:50</t>
+  </si>
+  <si>
+    <t>GPON06-D7-MDO-3</t>
+  </si>
+  <si>
+    <t>172.25.220.43</t>
+  </si>
+  <si>
+    <t>ZTEG900891C5</t>
+  </si>
+  <si>
+    <t>1/5/7:50</t>
+  </si>
+  <si>
+    <t>show gpon onu detail gpon-onu_1/5/7:50</t>
   </si>
 </sst>
 </file>
@@ -1251,7 +1250,7 @@
   <dimension ref="A1:AG56"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1301,10 +1300,10 @@
         <v>8</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="L1" s="4" t="s">
         <v>9</v>
@@ -1429,31 +1428,31 @@
         <v>29</v>
       </c>
       <c r="E4" s="5" t="s">
+        <v>266</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>269</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>269</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="K4" s="5" t="s">
         <v>271</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="L4" s="6" t="s">
         <v>272</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="M4" s="5" t="s">
         <v>273</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>274</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>274</v>
-      </c>
-      <c r="J4" s="5" t="s">
-        <v>275</v>
-      </c>
-      <c r="K4" s="5" t="s">
-        <v>276</v>
-      </c>
-      <c r="L4" s="6" t="s">
-        <v>277</v>
-      </c>
-      <c r="M4" s="5" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.3">
@@ -1470,31 +1469,31 @@
         <v>29</v>
       </c>
       <c r="E5" s="5" t="s">
+        <v>266</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>269</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>269</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="K5" s="5" t="s">
         <v>271</v>
       </c>
-      <c r="F5" s="5" t="s">
-        <v>272</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>273</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>274</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>274</v>
-      </c>
-      <c r="J5" s="5" t="s">
-        <v>279</v>
-      </c>
-      <c r="K5" s="5" t="s">
+      <c r="L5" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="M5" s="5" t="s">
         <v>276</v>
-      </c>
-      <c r="L5" s="5" t="s">
-        <v>280</v>
-      </c>
-      <c r="M5" s="5" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="6" spans="1:33" ht="28.8" x14ac:dyDescent="0.3">
@@ -1546,7 +1545,7 @@
         <v>28</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>29</v>
@@ -1587,7 +1586,7 @@
         <v>28</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>29</v>
@@ -1652,7 +1651,7 @@
         <v>54</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="L9" s="5" t="s">
         <v>55</v>
@@ -1693,7 +1692,7 @@
         <v>57</v>
       </c>
       <c r="K10" s="5" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="L10" s="5" t="s">
         <v>58</v>
@@ -1797,16 +1796,16 @@
         <v>19</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="K13" s="5" t="s">
         <v>21</v>
       </c>
       <c r="L13" s="6" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="M13" s="5" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
     </row>
     <row r="14" spans="1:33" x14ac:dyDescent="0.3">
@@ -1838,16 +1837,16 @@
         <v>19</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="K14" s="5" t="s">
         <v>21</v>
       </c>
       <c r="L14" s="5" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="M14" s="5" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
     </row>
     <row r="15" spans="1:33" ht="28.8" x14ac:dyDescent="0.3">
@@ -1882,7 +1881,7 @@
         <v>79</v>
       </c>
       <c r="K15" s="5" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="L15" s="6" t="s">
         <v>80</v>
@@ -1923,7 +1922,7 @@
         <v>82</v>
       </c>
       <c r="K16" s="5" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="L16" s="6" t="s">
         <v>83</v>
@@ -1958,7 +1957,7 @@
         <v>89</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="J17" s="5" t="s">
         <v>54</v>
@@ -1999,7 +1998,7 @@
         <v>89</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="J18" s="5" t="s">
         <v>57</v>
@@ -2040,7 +2039,7 @@
         <v>89</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="J19" s="5" t="s">
         <v>95</v>
@@ -2081,7 +2080,7 @@
         <v>89</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="J20" s="5" t="s">
         <v>98</v>
@@ -2195,22 +2194,22 @@
         <v>51</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="H23" s="5" t="s">
         <v>89</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="J23" s="5" t="s">
         <v>54</v>
       </c>
       <c r="K23" s="5" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="L23" s="6" t="s">
         <v>55</v>
@@ -2236,22 +2235,22 @@
         <v>51</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="H24" s="5" t="s">
         <v>89</v>
       </c>
       <c r="I24" s="5" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="J24" s="5" t="s">
         <v>57</v>
       </c>
       <c r="K24" s="5" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="L24" s="5" t="s">
         <v>58</v>
@@ -2368,7 +2367,7 @@
         <v>89</v>
       </c>
       <c r="I27" s="5" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="J27" s="5" t="s">
         <v>54</v>
@@ -2409,7 +2408,7 @@
         <v>89</v>
       </c>
       <c r="I28" s="5" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="J28" s="5" t="s">
         <v>57</v>
@@ -2482,10 +2481,10 @@
         <v>37</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="H30" s="5" t="s">
         <v>18</v>
@@ -2494,13 +2493,13 @@
         <v>19</v>
       </c>
       <c r="J30" s="5" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="K30" s="5" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="L30" s="5" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="M30" s="5" t="s">
         <v>43</v>
@@ -2702,7 +2701,7 @@
         <v>54</v>
       </c>
       <c r="K35" s="5" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="L35" s="5" t="s">
         <v>159</v>
@@ -2743,7 +2742,7 @@
         <v>57</v>
       </c>
       <c r="K36" s="5" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="L36" s="5" t="s">
         <v>161</v>
@@ -2752,7 +2751,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="37" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
         <v>153</v>
       </c>
@@ -2766,13 +2765,13 @@
         <v>163</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>164</v>
+        <v>288</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>165</v>
+        <v>289</v>
       </c>
       <c r="H37" s="5" t="s">
         <v>18</v>
@@ -2781,16 +2780,16 @@
         <v>19</v>
       </c>
       <c r="J37" s="5" t="s">
-        <v>261</v>
+        <v>173</v>
       </c>
       <c r="K37" s="5" t="s">
-        <v>166</v>
+        <v>290</v>
       </c>
       <c r="L37" s="6" t="s">
-        <v>167</v>
+        <v>174</v>
       </c>
       <c r="M37" s="5" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.3">
@@ -2807,53 +2806,69 @@
         <v>163</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="F38" s="5"/>
-      <c r="G38" s="5"/>
-      <c r="H38" s="5"/>
-      <c r="I38" s="5"/>
-      <c r="J38" s="5"/>
-      <c r="K38" s="5"/>
-      <c r="L38" s="5"/>
-      <c r="M38" s="5"/>
+        <v>37</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="G38" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="H38" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I38" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J38" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="K38" s="5" t="s">
+        <v>290</v>
+      </c>
+      <c r="L38" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="M38" s="5" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
         <v>153</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="E39" s="5" t="s">
         <v>37</v>
       </c>
       <c r="F39" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="G39" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="H39" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I39" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J39" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="K39" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="L39" s="5" t="s">
         <v>170</v>
-      </c>
-      <c r="G39" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="H39" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I39" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J39" s="5" t="s">
-        <v>172</v>
-      </c>
-      <c r="K39" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="L39" s="5" t="s">
-        <v>174</v>
       </c>
       <c r="M39" s="5" t="s">
         <v>43</v>
@@ -2864,22 +2879,22 @@
         <v>153</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="C40" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="E40" s="5" t="s">
         <v>37</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="G40" s="5" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="H40" s="5" t="s">
         <v>18</v>
@@ -2888,13 +2903,13 @@
         <v>19</v>
       </c>
       <c r="J40" s="5" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="K40" s="5" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="L40" s="5" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="M40" s="5" t="s">
         <v>43</v>
@@ -2905,37 +2920,37 @@
         <v>153</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C41" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="E41" s="5" t="s">
         <v>37</v>
       </c>
       <c r="F41" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="G41" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="H41" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I41" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J41" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="K41" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="L41" s="5" t="s">
         <v>181</v>
-      </c>
-      <c r="G41" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="H41" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I41" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J41" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="K41" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="L41" s="5" t="s">
-        <v>185</v>
       </c>
       <c r="M41" s="5" t="s">
         <v>43</v>
@@ -2946,22 +2961,22 @@
         <v>153</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C42" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="E42" s="5" t="s">
         <v>37</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="G42" s="5" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="H42" s="5" t="s">
         <v>18</v>
@@ -2970,13 +2985,13 @@
         <v>19</v>
       </c>
       <c r="J42" s="5" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="K42" s="5" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="L42" s="5" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="M42" s="5" t="s">
         <v>43</v>
@@ -2987,37 +3002,37 @@
         <v>153</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C43" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="E43" s="5" t="s">
         <v>37</v>
       </c>
       <c r="F43" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="G43" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="H43" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I43" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J43" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="K43" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="L43" s="5" t="s">
         <v>192</v>
-      </c>
-      <c r="G43" s="5" t="s">
-        <v>193</v>
-      </c>
-      <c r="H43" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I43" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J43" s="5" t="s">
-        <v>194</v>
-      </c>
-      <c r="K43" s="5" t="s">
-        <v>195</v>
-      </c>
-      <c r="L43" s="5" t="s">
-        <v>196</v>
       </c>
       <c r="M43" s="5" t="s">
         <v>43</v>
@@ -3028,37 +3043,37 @@
         <v>153</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C44" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="E44" s="5" t="s">
         <v>37</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="G44" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="H44" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I44" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J44" s="5" t="s">
         <v>193</v>
       </c>
-      <c r="H44" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I44" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J44" s="5" t="s">
-        <v>197</v>
-      </c>
       <c r="K44" s="5" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="L44" s="5" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="M44" s="5" t="s">
         <v>43</v>
@@ -3069,34 +3084,34 @@
         <v>153</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="C45" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="E45" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="G45" s="5" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="H45" s="5" t="s">
         <v>89</v>
       </c>
       <c r="I45" s="5" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="J45" s="5" t="s">
         <v>54</v>
       </c>
       <c r="K45" s="5" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="L45" s="5" t="s">
         <v>55</v>
@@ -3110,34 +3125,34 @@
         <v>153</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="C46" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="E46" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="G46" s="5" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="H46" s="5" t="s">
         <v>89</v>
       </c>
       <c r="I46" s="5" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="J46" s="5" t="s">
         <v>57</v>
       </c>
       <c r="K46" s="5" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="L46" s="5" t="s">
         <v>58</v>
@@ -3148,25 +3163,25 @@
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A47" s="5" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="C47" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="E47" s="5" t="s">
         <v>15</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="G47" s="5" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="H47" s="5" t="s">
         <v>18</v>
@@ -3175,95 +3190,95 @@
         <v>19</v>
       </c>
       <c r="J47" s="5" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="K47" s="5" t="s">
         <v>21</v>
       </c>
       <c r="L47" s="5" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="M47" s="5" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="C48" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="E48" s="5" t="s">
         <v>15</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="G48" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="H48" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I48" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J48" s="5" t="s">
         <v>207</v>
-      </c>
-      <c r="H48" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I48" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J48" s="5" t="s">
-        <v>211</v>
       </c>
       <c r="K48" s="5" t="s">
         <v>21</v>
       </c>
       <c r="L48" s="5" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="M48" s="5" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="C49" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D49" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="E49" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="F49" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="G49" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="H49" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I49" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J49" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="E49" s="5" t="s">
+      <c r="K49" s="5" t="s">
         <v>216</v>
       </c>
-      <c r="F49" s="5" t="s">
+      <c r="L49" s="5" t="s">
         <v>217</v>
-      </c>
-      <c r="G49" s="5" t="s">
-        <v>218</v>
-      </c>
-      <c r="H49" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I49" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J49" s="5" t="s">
-        <v>219</v>
-      </c>
-      <c r="K49" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="L49" s="5" t="s">
-        <v>221</v>
       </c>
       <c r="M49" s="5" t="s">
         <v>43</v>
@@ -3271,40 +3286,40 @@
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="C50" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="E50" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="F50" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="G50" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="H50" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I50" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J50" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="K50" s="5" t="s">
         <v>216</v>
       </c>
-      <c r="F50" s="5" t="s">
-        <v>222</v>
-      </c>
-      <c r="G50" s="5" t="s">
-        <v>223</v>
-      </c>
-      <c r="H50" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I50" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J50" s="5" t="s">
-        <v>224</v>
-      </c>
-      <c r="K50" s="5" t="s">
-        <v>220</v>
-      </c>
       <c r="L50" s="5" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="M50" s="5" t="s">
         <v>43</v>
@@ -3312,25 +3327,25 @@
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="C51" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="F51" s="5" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="G51" s="5" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="H51" s="5" t="s">
         <v>18</v>
@@ -3339,13 +3354,13 @@
         <v>19</v>
       </c>
       <c r="J51" s="5" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="K51" s="5" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="L51" s="5" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="M51" s="5" t="s">
         <v>43</v>
@@ -3353,40 +3368,40 @@
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="C52" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D52" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="E52" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="F52" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="G52" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="H52" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I52" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J52" s="5" t="s">
         <v>227</v>
       </c>
-      <c r="E52" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="F52" s="5" t="s">
-        <v>222</v>
-      </c>
-      <c r="G52" s="5" t="s">
-        <v>223</v>
-      </c>
-      <c r="H52" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I52" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J52" s="5" t="s">
-        <v>231</v>
-      </c>
       <c r="K52" s="5" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="L52" s="5" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="M52" s="5" t="s">
         <v>43</v>
@@ -3394,25 +3409,25 @@
     </row>
     <row r="53" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A53" s="5" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="C53" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="E53" s="5" t="s">
         <v>75</v>
       </c>
       <c r="F53" s="5" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="G53" s="5" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="H53" s="5" t="s">
         <v>78</v>
@@ -3421,54 +3436,54 @@
         <v>78</v>
       </c>
       <c r="J53" s="5" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="K53" s="5" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="L53" s="6" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="M53" s="5" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A54" s="5" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="C54" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="E54" s="5" t="s">
         <v>37</v>
       </c>
       <c r="F54" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="G54" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="H54" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I54" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J54" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="K54" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="L54" s="5" t="s">
         <v>240</v>
-      </c>
-      <c r="G54" s="5" t="s">
-        <v>241</v>
-      </c>
-      <c r="H54" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I54" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J54" s="5" t="s">
-        <v>242</v>
-      </c>
-      <c r="K54" s="5" t="s">
-        <v>243</v>
-      </c>
-      <c r="L54" s="5" t="s">
-        <v>244</v>
       </c>
       <c r="M54" s="5" t="s">
         <v>43</v>
@@ -3476,40 +3491,40 @@
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A55" s="5" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="C55" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D55" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="E55" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="F55" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="G55" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="H55" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I55" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J55" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="K55" s="5" t="s">
         <v>247</v>
       </c>
-      <c r="E55" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="F55" s="5" t="s">
+      <c r="L55" s="5" t="s">
         <v>248</v>
-      </c>
-      <c r="G55" s="5" t="s">
-        <v>249</v>
-      </c>
-      <c r="H55" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I55" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J55" s="5" t="s">
-        <v>250</v>
-      </c>
-      <c r="K55" s="5" t="s">
-        <v>251</v>
-      </c>
-      <c r="L55" s="5" t="s">
-        <v>252</v>
       </c>
       <c r="M55" s="5" t="s">
         <v>43</v>
@@ -3517,40 +3532,40 @@
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A56" s="5" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="C56" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="E56" s="5" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="F56" s="5" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="G56" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="H56" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I56" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J56" s="5" t="s">
         <v>249</v>
       </c>
-      <c r="H56" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I56" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J56" s="5" t="s">
-        <v>253</v>
-      </c>
       <c r="K56" s="5" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="L56" s="5" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="M56" s="5" t="s">
         <v>43</v>

</xml_diff>

<commit_message>
Update SN Site Premium MDO029
</commit_message>
<xml_diff>
--- a/data/premium-sites.xlsx
+++ b/data/premium-sites.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Local Repository\Telkom Projects\monitoring-site-premium-telegram-bot\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61A5313A-EEDC-4A67-A73A-CF0CCD5732AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13B8DD8C-428A-4E5B-BF8C-3416B40532E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -539,9 +539,6 @@
     <t>1/3/16:50</t>
   </si>
   <si>
-    <t>ZTEG900887BB</t>
-  </si>
-  <si>
     <t>show gpon onu detail gpon-onu_1/3/16:50</t>
   </si>
   <si>
@@ -910,6 +907,9 @@
   </si>
   <si>
     <t>show gpon onu detail gpon-onu_1/5/7:50</t>
+  </si>
+  <si>
+    <t>ZTEG900891C6</t>
   </si>
 </sst>
 </file>
@@ -1249,8 +1249,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="J40" sqref="J40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1300,10 +1300,10 @@
         <v>8</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="L1" s="4" t="s">
         <v>9</v>
@@ -1428,31 +1428,31 @@
         <v>29</v>
       </c>
       <c r="E4" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="F4" s="5" t="s">
         <v>266</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="G4" s="5" t="s">
         <v>267</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="H4" s="5" t="s">
         <v>268</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="I4" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="J4" s="5" t="s">
         <v>269</v>
       </c>
-      <c r="I4" s="5" t="s">
-        <v>269</v>
-      </c>
-      <c r="J4" s="5" t="s">
+      <c r="K4" s="5" t="s">
         <v>270</v>
       </c>
-      <c r="K4" s="5" t="s">
+      <c r="L4" s="6" t="s">
         <v>271</v>
       </c>
-      <c r="L4" s="6" t="s">
+      <c r="M4" s="5" t="s">
         <v>272</v>
-      </c>
-      <c r="M4" s="5" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.3">
@@ -1469,31 +1469,31 @@
         <v>29</v>
       </c>
       <c r="E5" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="F5" s="5" t="s">
         <v>266</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="G5" s="5" t="s">
         <v>267</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="H5" s="5" t="s">
         <v>268</v>
       </c>
-      <c r="H5" s="5" t="s">
-        <v>269</v>
-      </c>
       <c r="I5" s="5" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="J5" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="L5" s="5" t="s">
         <v>274</v>
       </c>
-      <c r="K5" s="5" t="s">
-        <v>271</v>
-      </c>
-      <c r="L5" s="5" t="s">
+      <c r="M5" s="5" t="s">
         <v>275</v>
-      </c>
-      <c r="M5" s="5" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="6" spans="1:33" ht="28.8" x14ac:dyDescent="0.3">
@@ -1545,7 +1545,7 @@
         <v>28</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>29</v>
@@ -1586,7 +1586,7 @@
         <v>28</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>29</v>
@@ -1651,7 +1651,7 @@
         <v>54</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="L9" s="5" t="s">
         <v>55</v>
@@ -1692,7 +1692,7 @@
         <v>57</v>
       </c>
       <c r="K10" s="5" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="L10" s="5" t="s">
         <v>58</v>
@@ -1796,16 +1796,16 @@
         <v>19</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="K13" s="5" t="s">
         <v>21</v>
       </c>
       <c r="L13" s="6" t="s">
+        <v>260</v>
+      </c>
+      <c r="M13" s="5" t="s">
         <v>261</v>
-      </c>
-      <c r="M13" s="5" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="14" spans="1:33" x14ac:dyDescent="0.3">
@@ -1837,16 +1837,16 @@
         <v>19</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="K14" s="5" t="s">
         <v>21</v>
       </c>
       <c r="L14" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="M14" s="5" t="s">
         <v>264</v>
-      </c>
-      <c r="M14" s="5" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="15" spans="1:33" ht="28.8" x14ac:dyDescent="0.3">
@@ -1881,7 +1881,7 @@
         <v>79</v>
       </c>
       <c r="K15" s="5" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="L15" s="6" t="s">
         <v>80</v>
@@ -1922,7 +1922,7 @@
         <v>82</v>
       </c>
       <c r="K16" s="5" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="L16" s="6" t="s">
         <v>83</v>
@@ -1957,7 +1957,7 @@
         <v>89</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="J17" s="5" t="s">
         <v>54</v>
@@ -1998,7 +1998,7 @@
         <v>89</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="J18" s="5" t="s">
         <v>57</v>
@@ -2039,7 +2039,7 @@
         <v>89</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="J19" s="5" t="s">
         <v>95</v>
@@ -2080,7 +2080,7 @@
         <v>89</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="J20" s="5" t="s">
         <v>98</v>
@@ -2194,22 +2194,22 @@
         <v>51</v>
       </c>
       <c r="F23" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="G23" s="5" t="s">
         <v>279</v>
-      </c>
-      <c r="G23" s="5" t="s">
-        <v>280</v>
       </c>
       <c r="H23" s="5" t="s">
         <v>89</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="J23" s="5" t="s">
         <v>54</v>
       </c>
       <c r="K23" s="5" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="L23" s="6" t="s">
         <v>55</v>
@@ -2235,22 +2235,22 @@
         <v>51</v>
       </c>
       <c r="F24" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="G24" s="5" t="s">
         <v>279</v>
-      </c>
-      <c r="G24" s="5" t="s">
-        <v>280</v>
       </c>
       <c r="H24" s="5" t="s">
         <v>89</v>
       </c>
       <c r="I24" s="5" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="J24" s="5" t="s">
         <v>57</v>
       </c>
       <c r="K24" s="5" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="L24" s="5" t="s">
         <v>58</v>
@@ -2367,7 +2367,7 @@
         <v>89</v>
       </c>
       <c r="I27" s="5" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="J27" s="5" t="s">
         <v>54</v>
@@ -2408,7 +2408,7 @@
         <v>89</v>
       </c>
       <c r="I28" s="5" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="J28" s="5" t="s">
         <v>57</v>
@@ -2481,25 +2481,25 @@
         <v>37</v>
       </c>
       <c r="F30" s="5" t="s">
+        <v>282</v>
+      </c>
+      <c r="G30" s="5" t="s">
         <v>283</v>
       </c>
-      <c r="G30" s="5" t="s">
+      <c r="H30" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I30" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J30" s="5" t="s">
         <v>284</v>
       </c>
-      <c r="H30" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I30" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J30" s="5" t="s">
+      <c r="K30" s="5" t="s">
         <v>285</v>
       </c>
-      <c r="K30" s="5" t="s">
+      <c r="L30" s="5" t="s">
         <v>286</v>
-      </c>
-      <c r="L30" s="5" t="s">
-        <v>287</v>
       </c>
       <c r="M30" s="5" t="s">
         <v>43</v>
@@ -2701,7 +2701,7 @@
         <v>54</v>
       </c>
       <c r="K35" s="5" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="L35" s="5" t="s">
         <v>159</v>
@@ -2742,7 +2742,7 @@
         <v>57</v>
       </c>
       <c r="K36" s="5" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="L36" s="5" t="s">
         <v>161</v>
@@ -2768,25 +2768,25 @@
         <v>37</v>
       </c>
       <c r="F37" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="G37" s="5" t="s">
         <v>288</v>
       </c>
-      <c r="G37" s="5" t="s">
+      <c r="H37" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I37" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J37" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="K37" s="5" t="s">
         <v>289</v>
       </c>
-      <c r="H37" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I37" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J37" s="5" t="s">
+      <c r="L37" s="6" t="s">
         <v>173</v>
-      </c>
-      <c r="K37" s="5" t="s">
-        <v>290</v>
-      </c>
-      <c r="L37" s="6" t="s">
-        <v>174</v>
       </c>
       <c r="M37" s="5" t="s">
         <v>43</v>
@@ -2809,25 +2809,25 @@
         <v>37</v>
       </c>
       <c r="F38" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="G38" s="5" t="s">
         <v>288</v>
       </c>
-      <c r="G38" s="5" t="s">
+      <c r="H38" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I38" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J38" s="5" t="s">
+        <v>290</v>
+      </c>
+      <c r="K38" s="5" t="s">
         <v>289</v>
       </c>
-      <c r="H38" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I38" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J38" s="5" t="s">
+      <c r="L38" s="5" t="s">
         <v>291</v>
-      </c>
-      <c r="K38" s="5" t="s">
-        <v>290</v>
-      </c>
-      <c r="L38" s="5" t="s">
-        <v>292</v>
       </c>
       <c r="M38" s="5" t="s">
         <v>43</v>
@@ -2865,10 +2865,10 @@
         <v>168</v>
       </c>
       <c r="K39" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="L39" s="5" t="s">
         <v>169</v>
-      </c>
-      <c r="L39" s="5" t="s">
-        <v>170</v>
       </c>
       <c r="M39" s="5" t="s">
         <v>43</v>
@@ -2891,25 +2891,25 @@
         <v>37</v>
       </c>
       <c r="F40" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="G40" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="G40" s="5" t="s">
+      <c r="H40" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I40" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J40" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="H40" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I40" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J40" s="5" t="s">
+      <c r="K40" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="L40" s="5" t="s">
         <v>173</v>
-      </c>
-      <c r="K40" s="5" t="s">
-        <v>169</v>
-      </c>
-      <c r="L40" s="5" t="s">
-        <v>174</v>
       </c>
       <c r="M40" s="5" t="s">
         <v>43</v>
@@ -2920,37 +2920,37 @@
         <v>153</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C41" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E41" s="5" t="s">
         <v>37</v>
       </c>
       <c r="F41" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="G41" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="G41" s="5" t="s">
+      <c r="H41" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I41" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J41" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="H41" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I41" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J41" s="5" t="s">
+      <c r="K41" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="K41" s="5" t="s">
+      <c r="L41" s="5" t="s">
         <v>180</v>
-      </c>
-      <c r="L41" s="5" t="s">
-        <v>181</v>
       </c>
       <c r="M41" s="5" t="s">
         <v>43</v>
@@ -2961,37 +2961,37 @@
         <v>153</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C42" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E42" s="5" t="s">
         <v>37</v>
       </c>
       <c r="F42" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="G42" s="5" t="s">
         <v>182</v>
       </c>
-      <c r="G42" s="5" t="s">
+      <c r="H42" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I42" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J42" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="H42" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I42" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J42" s="5" t="s">
+      <c r="K42" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="L42" s="5" t="s">
         <v>184</v>
-      </c>
-      <c r="K42" s="5" t="s">
-        <v>180</v>
-      </c>
-      <c r="L42" s="5" t="s">
-        <v>185</v>
       </c>
       <c r="M42" s="5" t="s">
         <v>43</v>
@@ -3002,37 +3002,37 @@
         <v>153</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C43" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E43" s="5" t="s">
         <v>37</v>
       </c>
       <c r="F43" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="G43" s="5" t="s">
         <v>188</v>
       </c>
-      <c r="G43" s="5" t="s">
+      <c r="H43" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I43" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J43" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="H43" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I43" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J43" s="5" t="s">
+      <c r="K43" s="5" t="s">
         <v>190</v>
       </c>
-      <c r="K43" s="5" t="s">
+      <c r="L43" s="5" t="s">
         <v>191</v>
-      </c>
-      <c r="L43" s="5" t="s">
-        <v>192</v>
       </c>
       <c r="M43" s="5" t="s">
         <v>43</v>
@@ -3043,23 +3043,23 @@
         <v>153</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C44" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E44" s="5" t="s">
         <v>37</v>
       </c>
       <c r="F44" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="G44" s="5" t="s">
         <v>188</v>
       </c>
-      <c r="G44" s="5" t="s">
-        <v>189</v>
-      </c>
       <c r="H44" s="5" t="s">
         <v>18</v>
       </c>
@@ -3067,13 +3067,13 @@
         <v>19</v>
       </c>
       <c r="J44" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="K44" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="L44" s="5" t="s">
         <v>193</v>
-      </c>
-      <c r="K44" s="5" t="s">
-        <v>191</v>
-      </c>
-      <c r="L44" s="5" t="s">
-        <v>194</v>
       </c>
       <c r="M44" s="5" t="s">
         <v>43</v>
@@ -3084,34 +3084,34 @@
         <v>153</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C45" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E45" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F45" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="G45" s="5" t="s">
         <v>197</v>
-      </c>
-      <c r="G45" s="5" t="s">
-        <v>198</v>
       </c>
       <c r="H45" s="5" t="s">
         <v>89</v>
       </c>
       <c r="I45" s="5" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="J45" s="5" t="s">
         <v>54</v>
       </c>
       <c r="K45" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="L45" s="5" t="s">
         <v>55</v>
@@ -3125,34 +3125,34 @@
         <v>153</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C46" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E46" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F46" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="G46" s="5" t="s">
         <v>197</v>
-      </c>
-      <c r="G46" s="5" t="s">
-        <v>198</v>
       </c>
       <c r="H46" s="5" t="s">
         <v>89</v>
       </c>
       <c r="I46" s="5" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="J46" s="5" t="s">
         <v>57</v>
       </c>
       <c r="K46" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="L46" s="5" t="s">
         <v>58</v>
@@ -3163,67 +3163,67 @@
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A47" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="B47" s="5" t="s">
         <v>199</v>
-      </c>
-      <c r="B47" s="5" t="s">
-        <v>200</v>
       </c>
       <c r="C47" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E47" s="5" t="s">
         <v>15</v>
       </c>
       <c r="F47" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="G47" s="5" t="s">
         <v>202</v>
       </c>
-      <c r="G47" s="5" t="s">
+      <c r="H47" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I47" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J47" s="5" t="s">
         <v>203</v>
-      </c>
-      <c r="H47" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I47" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J47" s="5" t="s">
-        <v>204</v>
       </c>
       <c r="K47" s="5" t="s">
         <v>21</v>
       </c>
       <c r="L47" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="M47" s="5" t="s">
         <v>205</v>
-      </c>
-      <c r="M47" s="5" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="B48" s="5" t="s">
         <v>199</v>
-      </c>
-      <c r="B48" s="5" t="s">
-        <v>200</v>
       </c>
       <c r="C48" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E48" s="5" t="s">
         <v>15</v>
       </c>
       <c r="F48" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="G48" s="5" t="s">
         <v>202</v>
       </c>
-      <c r="G48" s="5" t="s">
-        <v>203</v>
-      </c>
       <c r="H48" s="5" t="s">
         <v>18</v>
       </c>
@@ -3231,54 +3231,54 @@
         <v>19</v>
       </c>
       <c r="J48" s="5" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="K48" s="5" t="s">
         <v>21</v>
       </c>
       <c r="L48" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="M48" s="5" t="s">
         <v>208</v>
-      </c>
-      <c r="M48" s="5" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C49" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D49" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="E49" s="5" t="s">
         <v>211</v>
       </c>
-      <c r="E49" s="5" t="s">
+      <c r="F49" s="5" t="s">
         <v>212</v>
       </c>
-      <c r="F49" s="5" t="s">
+      <c r="G49" s="5" t="s">
         <v>213</v>
       </c>
-      <c r="G49" s="5" t="s">
+      <c r="H49" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I49" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J49" s="5" t="s">
         <v>214</v>
       </c>
-      <c r="H49" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I49" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J49" s="5" t="s">
+      <c r="K49" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="K49" s="5" t="s">
+      <c r="L49" s="5" t="s">
         <v>216</v>
-      </c>
-      <c r="L49" s="5" t="s">
-        <v>217</v>
       </c>
       <c r="M49" s="5" t="s">
         <v>43</v>
@@ -3286,40 +3286,40 @@
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C50" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D50" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="E50" s="5" t="s">
         <v>211</v>
       </c>
-      <c r="E50" s="5" t="s">
-        <v>212</v>
-      </c>
       <c r="F50" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="G50" s="5" t="s">
         <v>218</v>
       </c>
-      <c r="G50" s="5" t="s">
+      <c r="H50" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I50" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J50" s="5" t="s">
         <v>219</v>
       </c>
-      <c r="H50" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I50" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J50" s="5" t="s">
+      <c r="K50" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="L50" s="5" t="s">
         <v>220</v>
-      </c>
-      <c r="K50" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="L50" s="5" t="s">
-        <v>221</v>
       </c>
       <c r="M50" s="5" t="s">
         <v>43</v>
@@ -3327,40 +3327,40 @@
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C51" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D51" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="E51" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="F51" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="G51" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="H51" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I51" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J51" s="5" t="s">
         <v>223</v>
       </c>
-      <c r="E51" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="F51" s="5" t="s">
-        <v>213</v>
-      </c>
-      <c r="G51" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="H51" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I51" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J51" s="5" t="s">
+      <c r="K51" s="5" t="s">
         <v>224</v>
       </c>
-      <c r="K51" s="5" t="s">
+      <c r="L51" s="5" t="s">
         <v>225</v>
-      </c>
-      <c r="L51" s="5" t="s">
-        <v>226</v>
       </c>
       <c r="M51" s="5" t="s">
         <v>43</v>
@@ -3368,26 +3368,26 @@
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C52" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F52" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="G52" s="5" t="s">
         <v>218</v>
       </c>
-      <c r="G52" s="5" t="s">
-        <v>219</v>
-      </c>
       <c r="H52" s="5" t="s">
         <v>18</v>
       </c>
@@ -3395,13 +3395,13 @@
         <v>19</v>
       </c>
       <c r="J52" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="K52" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="L52" s="5" t="s">
         <v>227</v>
-      </c>
-      <c r="K52" s="5" t="s">
-        <v>225</v>
-      </c>
-      <c r="L52" s="5" t="s">
-        <v>228</v>
       </c>
       <c r="M52" s="5" t="s">
         <v>43</v>
@@ -3409,25 +3409,25 @@
     </row>
     <row r="53" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A53" s="5" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C53" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E53" s="5" t="s">
         <v>75</v>
       </c>
       <c r="F53" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="G53" s="5" t="s">
         <v>231</v>
-      </c>
-      <c r="G53" s="5" t="s">
-        <v>232</v>
       </c>
       <c r="H53" s="5" t="s">
         <v>78</v>
@@ -3436,54 +3436,54 @@
         <v>78</v>
       </c>
       <c r="J53" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="K53" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="L53" s="6" t="s">
         <v>233</v>
       </c>
-      <c r="K53" s="5" t="s">
-        <v>258</v>
-      </c>
-      <c r="L53" s="6" t="s">
+      <c r="M53" s="5" t="s">
         <v>234</v>
-      </c>
-      <c r="M53" s="5" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A54" s="5" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C54" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E54" s="5" t="s">
         <v>37</v>
       </c>
       <c r="F54" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="G54" s="5" t="s">
         <v>236</v>
       </c>
-      <c r="G54" s="5" t="s">
+      <c r="H54" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I54" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J54" s="5" t="s">
         <v>237</v>
       </c>
-      <c r="H54" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I54" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J54" s="5" t="s">
+      <c r="K54" s="5" t="s">
         <v>238</v>
       </c>
-      <c r="K54" s="5" t="s">
+      <c r="L54" s="5" t="s">
         <v>239</v>
-      </c>
-      <c r="L54" s="5" t="s">
-        <v>240</v>
       </c>
       <c r="M54" s="5" t="s">
         <v>43</v>
@@ -3491,40 +3491,40 @@
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A55" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="B55" s="5" t="s">
         <v>241</v>
-      </c>
-      <c r="B55" s="5" t="s">
-        <v>242</v>
       </c>
       <c r="C55" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D55" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="E55" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="F55" s="5" t="s">
         <v>243</v>
       </c>
-      <c r="E55" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="F55" s="5" t="s">
+      <c r="G55" s="5" t="s">
         <v>244</v>
       </c>
-      <c r="G55" s="5" t="s">
+      <c r="H55" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I55" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J55" s="5" t="s">
         <v>245</v>
       </c>
-      <c r="H55" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I55" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J55" s="5" t="s">
+      <c r="K55" s="5" t="s">
         <v>246</v>
       </c>
-      <c r="K55" s="5" t="s">
+      <c r="L55" s="5" t="s">
         <v>247</v>
-      </c>
-      <c r="L55" s="5" t="s">
-        <v>248</v>
       </c>
       <c r="M55" s="5" t="s">
         <v>43</v>
@@ -3532,26 +3532,26 @@
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A56" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="B56" s="5" t="s">
         <v>241</v>
-      </c>
-      <c r="B56" s="5" t="s">
-        <v>242</v>
       </c>
       <c r="C56" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D56" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="E56" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="F56" s="5" t="s">
         <v>243</v>
       </c>
-      <c r="E56" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="F56" s="5" t="s">
+      <c r="G56" s="5" t="s">
         <v>244</v>
       </c>
-      <c r="G56" s="5" t="s">
-        <v>245</v>
-      </c>
       <c r="H56" s="5" t="s">
         <v>18</v>
       </c>
@@ -3559,13 +3559,13 @@
         <v>19</v>
       </c>
       <c r="J56" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="K56" s="5" t="s">
         <v>249</v>
       </c>
-      <c r="K56" s="5" t="s">
+      <c r="L56" s="5" t="s">
         <v>250</v>
-      </c>
-      <c r="L56" s="5" t="s">
-        <v>251</v>
       </c>
       <c r="M56" s="5" t="s">
         <v>43</v>

</xml_diff>

<commit_message>
Update Site Premium PAL016 Link 1 & Link 2
</commit_message>
<xml_diff>
--- a/data/premium-sites.xlsx
+++ b/data/premium-sites.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Local Repository\Telkom Projects\monitoring-site-premium-telegram-bot\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13B8DD8C-428A-4E5B-BF8C-3416B40532E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0989A925-0414-4AF4-BE19-B95DED8E4671}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="290">
   <si>
     <t>Subdistrict</t>
   </si>
@@ -433,22 +433,6 @@
     <t>Pelabuhan Wani</t>
   </si>
   <si>
-    <t>GPON02-D7-TWL-4</t>
-  </si>
-  <si>
-    <t>172.25.244.140</t>
-  </si>
-  <si>
-    <t>1/16/1</t>
-  </si>
-  <si>
-    <t>FHTT05ee31ff</t>
-  </si>
-  <si>
-    <t>config
-show authorization 1/1/16 | include FHTT05ee31ff</t>
-  </si>
-  <si>
     <t>PAL125</t>
   </si>
   <si>
@@ -910,6 +894,12 @@
   </si>
   <si>
     <t>ZTEG900891C6</t>
+  </si>
+  <si>
+    <t>1/4/6:50</t>
+  </si>
+  <si>
+    <t>show gpon onu detail gpon-onu_1/4/6:50</t>
   </si>
 </sst>
 </file>
@@ -1250,7 +1240,7 @@
   <dimension ref="A1:AG56"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="J40" sqref="J40"/>
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1300,10 +1290,10 @@
         <v>8</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="L1" s="4" t="s">
         <v>9</v>
@@ -1428,31 +1418,31 @@
         <v>29</v>
       </c>
       <c r="E4" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>264</v>
+      </c>
+      <c r="K4" s="5" t="s">
         <v>265</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="L4" s="6" t="s">
         <v>266</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="M4" s="5" t="s">
         <v>267</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>268</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>268</v>
-      </c>
-      <c r="J4" s="5" t="s">
-        <v>269</v>
-      </c>
-      <c r="K4" s="5" t="s">
-        <v>270</v>
-      </c>
-      <c r="L4" s="6" t="s">
-        <v>271</v>
-      </c>
-      <c r="M4" s="5" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.3">
@@ -1469,31 +1459,31 @@
         <v>29</v>
       </c>
       <c r="E5" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="K5" s="5" t="s">
         <v>265</v>
       </c>
-      <c r="F5" s="5" t="s">
-        <v>266</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>267</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>268</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>268</v>
-      </c>
-      <c r="J5" s="5" t="s">
-        <v>273</v>
-      </c>
-      <c r="K5" s="5" t="s">
+      <c r="L5" s="5" t="s">
+        <v>269</v>
+      </c>
+      <c r="M5" s="5" t="s">
         <v>270</v>
-      </c>
-      <c r="L5" s="5" t="s">
-        <v>274</v>
-      </c>
-      <c r="M5" s="5" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="6" spans="1:33" ht="28.8" x14ac:dyDescent="0.3">
@@ -1545,7 +1535,7 @@
         <v>28</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>29</v>
@@ -1586,7 +1576,7 @@
         <v>28</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>29</v>
@@ -1651,7 +1641,7 @@
         <v>54</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="L9" s="5" t="s">
         <v>55</v>
@@ -1692,7 +1682,7 @@
         <v>57</v>
       </c>
       <c r="K10" s="5" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="L10" s="5" t="s">
         <v>58</v>
@@ -1796,16 +1786,16 @@
         <v>19</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="K13" s="5" t="s">
         <v>21</v>
       </c>
       <c r="L13" s="6" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="M13" s="5" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
     </row>
     <row r="14" spans="1:33" x14ac:dyDescent="0.3">
@@ -1837,16 +1827,16 @@
         <v>19</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="K14" s="5" t="s">
         <v>21</v>
       </c>
       <c r="L14" s="5" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="M14" s="5" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
     </row>
     <row r="15" spans="1:33" ht="28.8" x14ac:dyDescent="0.3">
@@ -1881,7 +1871,7 @@
         <v>79</v>
       </c>
       <c r="K15" s="5" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="L15" s="6" t="s">
         <v>80</v>
@@ -1922,7 +1912,7 @@
         <v>82</v>
       </c>
       <c r="K16" s="5" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="L16" s="6" t="s">
         <v>83</v>
@@ -1957,7 +1947,7 @@
         <v>89</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="J17" s="5" t="s">
         <v>54</v>
@@ -1998,7 +1988,7 @@
         <v>89</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="J18" s="5" t="s">
         <v>57</v>
@@ -2039,7 +2029,7 @@
         <v>89</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="J19" s="5" t="s">
         <v>95</v>
@@ -2080,7 +2070,7 @@
         <v>89</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="J20" s="5" t="s">
         <v>98</v>
@@ -2194,22 +2184,22 @@
         <v>51</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="H23" s="5" t="s">
         <v>89</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="J23" s="5" t="s">
         <v>54</v>
       </c>
       <c r="K23" s="5" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="L23" s="6" t="s">
         <v>55</v>
@@ -2235,22 +2225,22 @@
         <v>51</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="H24" s="5" t="s">
         <v>89</v>
       </c>
       <c r="I24" s="5" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="J24" s="5" t="s">
         <v>57</v>
       </c>
       <c r="K24" s="5" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="L24" s="5" t="s">
         <v>58</v>
@@ -2367,7 +2357,7 @@
         <v>89</v>
       </c>
       <c r="I27" s="5" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="J27" s="5" t="s">
         <v>54</v>
@@ -2408,7 +2398,7 @@
         <v>89</v>
       </c>
       <c r="I28" s="5" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="J28" s="5" t="s">
         <v>57</v>
@@ -2423,7 +2413,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
         <v>114</v>
       </c>
@@ -2437,13 +2427,13 @@
         <v>133</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>134</v>
+        <v>277</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>135</v>
+        <v>278</v>
       </c>
       <c r="H29" s="5" t="s">
         <v>18</v>
@@ -2452,16 +2442,16 @@
         <v>19</v>
       </c>
       <c r="J29" s="5" t="s">
-        <v>136</v>
+        <v>279</v>
       </c>
       <c r="K29" s="5" t="s">
-        <v>137</v>
+        <v>280</v>
       </c>
       <c r="L29" s="6" t="s">
-        <v>138</v>
+        <v>281</v>
       </c>
       <c r="M29" s="5" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
@@ -2481,10 +2471,10 @@
         <v>37</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="H30" s="5" t="s">
         <v>18</v>
@@ -2493,13 +2483,13 @@
         <v>19</v>
       </c>
       <c r="J30" s="5" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="K30" s="5" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="L30" s="5" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="M30" s="5" t="s">
         <v>43</v>
@@ -2510,13 +2500,13 @@
         <v>114</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="C31" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="E31" s="5" t="s">
         <v>37</v>
@@ -2534,13 +2524,13 @@
         <v>19</v>
       </c>
       <c r="J31" s="5" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="K31" s="5" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="L31" s="5" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="M31" s="5" t="s">
         <v>43</v>
@@ -2551,13 +2541,13 @@
         <v>114</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="C32" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="E32" s="5" t="s">
         <v>37</v>
@@ -2575,13 +2565,13 @@
         <v>19</v>
       </c>
       <c r="J32" s="5" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="K32" s="5" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="L32" s="5" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="M32" s="5" t="s">
         <v>43</v>
@@ -2592,13 +2582,13 @@
         <v>114</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="C33" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="E33" s="5" t="s">
         <v>37</v>
@@ -2616,13 +2606,13 @@
         <v>19</v>
       </c>
       <c r="J33" s="5" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="K33" s="5" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="L33" s="5" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="M33" s="5" t="s">
         <v>43</v>
@@ -2633,13 +2623,13 @@
         <v>114</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="C34" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="E34" s="5" t="s">
         <v>37</v>
@@ -2657,13 +2647,13 @@
         <v>19</v>
       </c>
       <c r="J34" s="5" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="K34" s="5" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="L34" s="5" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="M34" s="5" t="s">
         <v>43</v>
@@ -2671,25 +2661,25 @@
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="C35" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="H35" s="5" t="s">
         <v>18</v>
@@ -2701,36 +2691,36 @@
         <v>54</v>
       </c>
       <c r="K35" s="5" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="L35" s="5" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="M35" s="5" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="C36" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="G36" s="5" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="H36" s="5" t="s">
         <v>18</v>
@@ -2742,36 +2732,36 @@
         <v>57</v>
       </c>
       <c r="K36" s="5" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="L36" s="5" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="M36" s="5" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="C37" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="E37" s="5" t="s">
         <v>37</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="H37" s="5" t="s">
         <v>18</v>
@@ -2780,13 +2770,13 @@
         <v>19</v>
       </c>
       <c r="J37" s="5" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="K37" s="5" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="L37" s="6" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="M37" s="5" t="s">
         <v>43</v>
@@ -2794,25 +2784,25 @@
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="E38" s="5" t="s">
         <v>37</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="G38" s="5" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="H38" s="5" t="s">
         <v>18</v>
@@ -2821,13 +2811,13 @@
         <v>19</v>
       </c>
       <c r="J38" s="5" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="K38" s="5" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="L38" s="5" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="M38" s="5" t="s">
         <v>43</v>
@@ -2835,25 +2825,25 @@
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="E39" s="5" t="s">
         <v>37</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="H39" s="5" t="s">
         <v>18</v>
@@ -2862,13 +2852,13 @@
         <v>19</v>
       </c>
       <c r="J39" s="5" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="K39" s="5" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="L39" s="5" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="M39" s="5" t="s">
         <v>43</v>
@@ -2876,25 +2866,25 @@
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="C40" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="E40" s="5" t="s">
         <v>37</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="G40" s="5" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="H40" s="5" t="s">
         <v>18</v>
@@ -2903,13 +2893,13 @@
         <v>19</v>
       </c>
       <c r="J40" s="5" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="K40" s="5" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="L40" s="5" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="M40" s="5" t="s">
         <v>43</v>
@@ -2917,25 +2907,25 @@
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41" s="5" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="C41" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="E41" s="5" t="s">
         <v>37</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="H41" s="5" t="s">
         <v>18</v>
@@ -2944,13 +2934,13 @@
         <v>19</v>
       </c>
       <c r="J41" s="5" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="K41" s="5" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="L41" s="5" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="M41" s="5" t="s">
         <v>43</v>
@@ -2958,25 +2948,25 @@
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="C42" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="E42" s="5" t="s">
         <v>37</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="G42" s="5" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="H42" s="5" t="s">
         <v>18</v>
@@ -2985,13 +2975,13 @@
         <v>19</v>
       </c>
       <c r="J42" s="5" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="K42" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="L42" s="5" t="s">
         <v>179</v>
-      </c>
-      <c r="L42" s="5" t="s">
-        <v>184</v>
       </c>
       <c r="M42" s="5" t="s">
         <v>43</v>
@@ -2999,25 +2989,25 @@
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="C43" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="E43" s="5" t="s">
         <v>37</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="H43" s="5" t="s">
         <v>18</v>
@@ -3026,13 +3016,13 @@
         <v>19</v>
       </c>
       <c r="J43" s="5" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="K43" s="5" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="L43" s="5" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="M43" s="5" t="s">
         <v>43</v>
@@ -3040,40 +3030,40 @@
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="C44" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="E44" s="5" t="s">
         <v>37</v>
       </c>
       <c r="F44" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="G44" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="H44" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I44" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J44" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="G44" s="5" t="s">
+      <c r="K44" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="L44" s="5" t="s">
         <v>188</v>
-      </c>
-      <c r="H44" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I44" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J44" s="5" t="s">
-        <v>192</v>
-      </c>
-      <c r="K44" s="5" t="s">
-        <v>190</v>
-      </c>
-      <c r="L44" s="5" t="s">
-        <v>193</v>
       </c>
       <c r="M44" s="5" t="s">
         <v>43</v>
@@ -3081,37 +3071,37 @@
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="C45" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="E45" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="G45" s="5" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="H45" s="5" t="s">
         <v>89</v>
       </c>
       <c r="I45" s="5" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="J45" s="5" t="s">
         <v>54</v>
       </c>
       <c r="K45" s="5" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="L45" s="5" t="s">
         <v>55</v>
@@ -3122,37 +3112,37 @@
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46" s="5" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="C46" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="E46" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="G46" s="5" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="H46" s="5" t="s">
         <v>89</v>
       </c>
       <c r="I46" s="5" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="J46" s="5" t="s">
         <v>57</v>
       </c>
       <c r="K46" s="5" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="L46" s="5" t="s">
         <v>58</v>
@@ -3163,25 +3153,25 @@
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A47" s="5" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="C47" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="E47" s="5" t="s">
         <v>15</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="G47" s="5" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="H47" s="5" t="s">
         <v>18</v>
@@ -3190,95 +3180,95 @@
         <v>19</v>
       </c>
       <c r="J47" s="5" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="K47" s="5" t="s">
         <v>21</v>
       </c>
       <c r="L47" s="5" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="M47" s="5" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="C48" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="E48" s="5" t="s">
         <v>15</v>
       </c>
       <c r="F48" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="G48" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="H48" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I48" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J48" s="5" t="s">
         <v>201</v>
-      </c>
-      <c r="G48" s="5" t="s">
-        <v>202</v>
-      </c>
-      <c r="H48" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I48" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J48" s="5" t="s">
-        <v>206</v>
       </c>
       <c r="K48" s="5" t="s">
         <v>21</v>
       </c>
       <c r="L48" s="5" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="M48" s="5" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="C49" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D49" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="E49" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="F49" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="G49" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="H49" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I49" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J49" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="K49" s="5" t="s">
         <v>210</v>
       </c>
-      <c r="E49" s="5" t="s">
+      <c r="L49" s="5" t="s">
         <v>211</v>
-      </c>
-      <c r="F49" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="G49" s="5" t="s">
-        <v>213</v>
-      </c>
-      <c r="H49" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I49" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J49" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="K49" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="L49" s="5" t="s">
-        <v>216</v>
       </c>
       <c r="M49" s="5" t="s">
         <v>43</v>
@@ -3286,40 +3276,40 @@
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="C50" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D50" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="E50" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="F50" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="G50" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="H50" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I50" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J50" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="K50" s="5" t="s">
         <v>210</v>
       </c>
-      <c r="E50" s="5" t="s">
-        <v>211</v>
-      </c>
-      <c r="F50" s="5" t="s">
-        <v>217</v>
-      </c>
-      <c r="G50" s="5" t="s">
-        <v>218</v>
-      </c>
-      <c r="H50" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I50" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J50" s="5" t="s">
-        <v>219</v>
-      </c>
-      <c r="K50" s="5" t="s">
+      <c r="L50" s="5" t="s">
         <v>215</v>
-      </c>
-      <c r="L50" s="5" t="s">
-        <v>220</v>
       </c>
       <c r="M50" s="5" t="s">
         <v>43</v>
@@ -3327,25 +3317,25 @@
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="C51" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="F51" s="5" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="G51" s="5" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="H51" s="5" t="s">
         <v>18</v>
@@ -3354,13 +3344,13 @@
         <v>19</v>
       </c>
       <c r="J51" s="5" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="K51" s="5" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="L51" s="5" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="M51" s="5" t="s">
         <v>43</v>
@@ -3368,40 +3358,40 @@
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="C52" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D52" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="E52" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="F52" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="G52" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="H52" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I52" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J52" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="K52" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="L52" s="5" t="s">
         <v>222</v>
-      </c>
-      <c r="E52" s="5" t="s">
-        <v>211</v>
-      </c>
-      <c r="F52" s="5" t="s">
-        <v>217</v>
-      </c>
-      <c r="G52" s="5" t="s">
-        <v>218</v>
-      </c>
-      <c r="H52" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I52" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J52" s="5" t="s">
-        <v>226</v>
-      </c>
-      <c r="K52" s="5" t="s">
-        <v>224</v>
-      </c>
-      <c r="L52" s="5" t="s">
-        <v>227</v>
       </c>
       <c r="M52" s="5" t="s">
         <v>43</v>
@@ -3409,25 +3399,25 @@
     </row>
     <row r="53" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A53" s="5" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="C53" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="E53" s="5" t="s">
         <v>75</v>
       </c>
       <c r="F53" s="5" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="G53" s="5" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="H53" s="5" t="s">
         <v>78</v>
@@ -3436,39 +3426,39 @@
         <v>78</v>
       </c>
       <c r="J53" s="5" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="K53" s="5" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="L53" s="6" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="M53" s="5" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A54" s="5" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="C54" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="E54" s="5" t="s">
         <v>37</v>
       </c>
       <c r="F54" s="5" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="G54" s="5" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="H54" s="5" t="s">
         <v>18</v>
@@ -3477,13 +3467,13 @@
         <v>19</v>
       </c>
       <c r="J54" s="5" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="K54" s="5" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="L54" s="5" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="M54" s="5" t="s">
         <v>43</v>
@@ -3491,40 +3481,40 @@
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A55" s="5" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="C55" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D55" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="E55" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="F55" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="G55" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="H55" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I55" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J55" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="K55" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="L55" s="5" t="s">
         <v>242</v>
-      </c>
-      <c r="E55" s="5" t="s">
-        <v>211</v>
-      </c>
-      <c r="F55" s="5" t="s">
-        <v>243</v>
-      </c>
-      <c r="G55" s="5" t="s">
-        <v>244</v>
-      </c>
-      <c r="H55" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I55" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J55" s="5" t="s">
-        <v>245</v>
-      </c>
-      <c r="K55" s="5" t="s">
-        <v>246</v>
-      </c>
-      <c r="L55" s="5" t="s">
-        <v>247</v>
       </c>
       <c r="M55" s="5" t="s">
         <v>43</v>
@@ -3532,40 +3522,40 @@
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A56" s="5" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="C56" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="E56" s="5" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="F56" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="G56" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="H56" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I56" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J56" s="5" t="s">
         <v>243</v>
       </c>
-      <c r="G56" s="5" t="s">
+      <c r="K56" s="5" t="s">
         <v>244</v>
       </c>
-      <c r="H56" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I56" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J56" s="5" t="s">
-        <v>248</v>
-      </c>
-      <c r="K56" s="5" t="s">
-        <v>249</v>
-      </c>
       <c r="L56" s="5" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="M56" s="5" t="s">
         <v>43</v>

</xml_diff>

<commit_message>
Update Site Premium ADL007 Link 1 & Link 2
</commit_message>
<xml_diff>
--- a/data/premium-sites.xlsx
+++ b/data/premium-sites.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Local Repository\Telkom Projects\monitoring-site-premium-telegram-bot\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0989A925-0414-4AF4-BE19-B95DED8E4671}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99C7CF0D-888C-4BF7-B2D4-0D59641D045D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -266,26 +266,6 @@
     <t>zxr10</t>
   </si>
   <si>
-    <t>gei-0/1/1/7</t>
-  </si>
-  <si>
-    <t>enable
-show interface gei-0/1/1/7</t>
-  </si>
-  <si>
-    <t>gei-0/1/1/7 is up</t>
-  </si>
-  <si>
-    <t>gei-0/1/1/8</t>
-  </si>
-  <si>
-    <t>enable
-show interface gei-0/1/1/8</t>
-  </si>
-  <si>
-    <t>gei-0/1/1/8 is up</t>
-  </si>
-  <si>
     <t>BAU006</t>
   </si>
   <si>
@@ -900,6 +880,26 @@
   </si>
   <si>
     <t>show gpon onu detail gpon-onu_1/4/6:50</t>
+  </si>
+  <si>
+    <t>xgei-0/1/2/1</t>
+  </si>
+  <si>
+    <t>enable
+show interface xgei-0/1/2/1</t>
+  </si>
+  <si>
+    <t>xgei-0/1/2/1 is up</t>
+  </si>
+  <si>
+    <t>smartgroup1</t>
+  </si>
+  <si>
+    <t>enable
+show interface smartgroup1</t>
+  </si>
+  <si>
+    <t>smartgroup1 is up</t>
   </si>
 </sst>
 </file>
@@ -1239,8 +1239,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1290,10 +1290,10 @@
         <v>8</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="L1" s="4" t="s">
         <v>9</v>
@@ -1418,31 +1418,31 @@
         <v>29</v>
       </c>
       <c r="E4" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="L4" s="6" t="s">
         <v>260</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="M4" s="5" t="s">
         <v>261</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>262</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>263</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>263</v>
-      </c>
-      <c r="J4" s="5" t="s">
-        <v>264</v>
-      </c>
-      <c r="K4" s="5" t="s">
-        <v>265</v>
-      </c>
-      <c r="L4" s="6" t="s">
-        <v>266</v>
-      </c>
-      <c r="M4" s="5" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.3">
@@ -1459,31 +1459,31 @@
         <v>29</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="G5" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="J5" s="5" t="s">
         <v>262</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="K5" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="L5" s="5" t="s">
         <v>263</v>
       </c>
-      <c r="I5" s="5" t="s">
-        <v>263</v>
-      </c>
-      <c r="J5" s="5" t="s">
-        <v>268</v>
-      </c>
-      <c r="K5" s="5" t="s">
-        <v>265</v>
-      </c>
-      <c r="L5" s="5" t="s">
-        <v>269</v>
-      </c>
       <c r="M5" s="5" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
     </row>
     <row r="6" spans="1:33" ht="28.8" x14ac:dyDescent="0.3">
@@ -1535,7 +1535,7 @@
         <v>28</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>29</v>
@@ -1576,7 +1576,7 @@
         <v>28</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>29</v>
@@ -1641,7 +1641,7 @@
         <v>54</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="L9" s="5" t="s">
         <v>55</v>
@@ -1682,7 +1682,7 @@
         <v>57</v>
       </c>
       <c r="K10" s="5" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="L10" s="5" t="s">
         <v>58</v>
@@ -1786,16 +1786,16 @@
         <v>19</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="K13" s="5" t="s">
         <v>21</v>
       </c>
       <c r="L13" s="6" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="M13" s="5" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
     </row>
     <row r="14" spans="1:33" x14ac:dyDescent="0.3">
@@ -1827,16 +1827,16 @@
         <v>19</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="K14" s="5" t="s">
         <v>21</v>
       </c>
       <c r="L14" s="5" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="M14" s="5" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
     </row>
     <row r="15" spans="1:33" ht="28.8" x14ac:dyDescent="0.3">
@@ -1868,16 +1868,16 @@
         <v>78</v>
       </c>
       <c r="J15" s="5" t="s">
-        <v>79</v>
+        <v>284</v>
       </c>
       <c r="K15" s="5" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="L15" s="6" t="s">
-        <v>80</v>
+        <v>285</v>
       </c>
       <c r="M15" s="5" t="s">
-        <v>81</v>
+        <v>286</v>
       </c>
     </row>
     <row r="16" spans="1:33" ht="28.8" x14ac:dyDescent="0.3">
@@ -1909,16 +1909,16 @@
         <v>78</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>82</v>
+        <v>287</v>
       </c>
       <c r="K16" s="5" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="L16" s="6" t="s">
-        <v>83</v>
+        <v>288</v>
       </c>
       <c r="M16" s="5" t="s">
-        <v>84</v>
+        <v>289</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
@@ -1926,34 +1926,34 @@
         <v>72</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="J17" s="5" t="s">
         <v>54</v>
       </c>
       <c r="K17" s="5" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="L17" s="5" t="s">
         <v>55</v>
@@ -1967,34 +1967,34 @@
         <v>72</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="J18" s="5" t="s">
         <v>57</v>
       </c>
       <c r="K18" s="5" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="L18" s="5" t="s">
         <v>58</v>
@@ -2008,37 +2008,37 @@
         <v>72</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="E19" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="H19" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="J19" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="I19" s="5" t="s">
-        <v>249</v>
-      </c>
-      <c r="J19" s="5" t="s">
-        <v>95</v>
-      </c>
       <c r="K19" s="5" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="L19" s="5" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="M19" s="5" t="s">
         <v>56</v>
@@ -2049,37 +2049,37 @@
         <v>72</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F20" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="I20" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="J20" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="K20" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="L20" s="5" t="s">
         <v>93</v>
-      </c>
-      <c r="G20" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="H20" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="I20" s="5" t="s">
-        <v>249</v>
-      </c>
-      <c r="J20" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="K20" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="L20" s="5" t="s">
-        <v>99</v>
       </c>
       <c r="M20" s="5" t="s">
         <v>56</v>
@@ -2090,22 +2090,22 @@
         <v>72</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="E21" s="5" t="s">
         <v>15</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="H21" s="5" t="s">
         <v>18</v>
@@ -2114,16 +2114,16 @@
         <v>19</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="K21" s="5" t="s">
         <v>21</v>
       </c>
       <c r="L21" s="5" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="M21" s="5" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
@@ -2131,22 +2131,22 @@
         <v>72</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="E22" s="5" t="s">
         <v>15</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="H22" s="5" t="s">
         <v>18</v>
@@ -2155,16 +2155,16 @@
         <v>19</v>
       </c>
       <c r="J22" s="5" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="K22" s="5" t="s">
         <v>21</v>
       </c>
       <c r="L22" s="5" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="M22" s="5" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
@@ -2172,34 +2172,34 @@
         <v>72</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="E23" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="J23" s="5" t="s">
         <v>54</v>
       </c>
       <c r="K23" s="5" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="L23" s="6" t="s">
         <v>55</v>
@@ -2213,34 +2213,34 @@
         <v>72</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="E24" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="I24" s="5" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="J24" s="5" t="s">
         <v>57</v>
       </c>
       <c r="K24" s="5" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="L24" s="5" t="s">
         <v>58</v>
@@ -2251,40 +2251,40 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D25" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="H25" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I25" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J25" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="K25" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="L25" s="5" t="s">
         <v>116</v>
-      </c>
-      <c r="E25" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="F25" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="G25" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="H25" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I25" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J25" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="K25" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="L25" s="5" t="s">
-        <v>122</v>
       </c>
       <c r="M25" s="5" t="s">
         <v>43</v>
@@ -2292,25 +2292,25 @@
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="E26" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="F26" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="F26" s="5" t="s">
-        <v>123</v>
-      </c>
       <c r="G26" s="5" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="H26" s="5" t="s">
         <v>18</v>
@@ -2319,13 +2319,13 @@
         <v>19</v>
       </c>
       <c r="J26" s="5" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="K26" s="5" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="L26" s="5" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="M26" s="5" t="s">
         <v>43</v>
@@ -2333,37 +2333,37 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="E27" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="I27" s="5" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="J27" s="5" t="s">
         <v>54</v>
       </c>
       <c r="K27" s="5" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="L27" s="5" t="s">
         <v>55</v>
@@ -2374,37 +2374,37 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="E28" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="H28" s="5" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="I28" s="5" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="J28" s="5" t="s">
         <v>57</v>
       </c>
       <c r="K28" s="5" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="L28" s="5" t="s">
         <v>58</v>
@@ -2415,25 +2415,25 @@
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="E29" s="5" t="s">
         <v>37</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="H29" s="5" t="s">
         <v>18</v>
@@ -2442,13 +2442,13 @@
         <v>19</v>
       </c>
       <c r="J29" s="5" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="K29" s="5" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="L29" s="6" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="M29" s="5" t="s">
         <v>43</v>
@@ -2456,25 +2456,25 @@
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="E30" s="5" t="s">
         <v>37</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="H30" s="5" t="s">
         <v>18</v>
@@ -2483,13 +2483,13 @@
         <v>19</v>
       </c>
       <c r="J30" s="5" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="K30" s="5" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="L30" s="5" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="M30" s="5" t="s">
         <v>43</v>
@@ -2497,25 +2497,25 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C31" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="E31" s="5" t="s">
         <v>37</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="H31" s="5" t="s">
         <v>18</v>
@@ -2524,13 +2524,13 @@
         <v>19</v>
       </c>
       <c r="J31" s="5" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="K31" s="5" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="L31" s="5" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="M31" s="5" t="s">
         <v>43</v>
@@ -2538,25 +2538,25 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C32" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="E32" s="5" t="s">
         <v>37</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="H32" s="5" t="s">
         <v>18</v>
@@ -2565,13 +2565,13 @@
         <v>19</v>
       </c>
       <c r="J32" s="5" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="K32" s="5" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="L32" s="5" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="M32" s="5" t="s">
         <v>43</v>
@@ -2579,25 +2579,25 @@
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="C33" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="E33" s="5" t="s">
         <v>37</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="H33" s="5" t="s">
         <v>18</v>
@@ -2606,13 +2606,13 @@
         <v>19</v>
       </c>
       <c r="J33" s="5" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="K33" s="5" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="L33" s="5" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="M33" s="5" t="s">
         <v>43</v>
@@ -2620,25 +2620,25 @@
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="C34" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="E34" s="5" t="s">
         <v>37</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="G34" s="5" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="H34" s="5" t="s">
         <v>18</v>
@@ -2647,13 +2647,13 @@
         <v>19</v>
       </c>
       <c r="J34" s="5" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="K34" s="5" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="L34" s="5" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="M34" s="5" t="s">
         <v>43</v>
@@ -2661,25 +2661,25 @@
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="C35" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="H35" s="5" t="s">
         <v>18</v>
@@ -2691,36 +2691,36 @@
         <v>54</v>
       </c>
       <c r="K35" s="5" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="L35" s="5" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="M35" s="5" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="C36" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="G36" s="5" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="H36" s="5" t="s">
         <v>18</v>
@@ -2732,36 +2732,36 @@
         <v>57</v>
       </c>
       <c r="K36" s="5" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="L36" s="5" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="M36" s="5" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="C37" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="E37" s="5" t="s">
         <v>37</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="H37" s="5" t="s">
         <v>18</v>
@@ -2770,13 +2770,13 @@
         <v>19</v>
       </c>
       <c r="J37" s="5" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="K37" s="5" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="L37" s="6" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="M37" s="5" t="s">
         <v>43</v>
@@ -2784,25 +2784,25 @@
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="E38" s="5" t="s">
         <v>37</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="G38" s="5" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="H38" s="5" t="s">
         <v>18</v>
@@ -2811,13 +2811,13 @@
         <v>19</v>
       </c>
       <c r="J38" s="5" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="K38" s="5" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="L38" s="5" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="M38" s="5" t="s">
         <v>43</v>
@@ -2825,25 +2825,25 @@
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="E39" s="5" t="s">
         <v>37</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="H39" s="5" t="s">
         <v>18</v>
@@ -2852,13 +2852,13 @@
         <v>19</v>
       </c>
       <c r="J39" s="5" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="K39" s="5" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="L39" s="5" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="M39" s="5" t="s">
         <v>43</v>
@@ -2866,25 +2866,25 @@
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="C40" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="E40" s="5" t="s">
         <v>37</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="G40" s="5" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="H40" s="5" t="s">
         <v>18</v>
@@ -2893,13 +2893,13 @@
         <v>19</v>
       </c>
       <c r="J40" s="5" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="K40" s="5" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="L40" s="5" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="M40" s="5" t="s">
         <v>43</v>
@@ -2907,25 +2907,25 @@
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41" s="5" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="C41" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="E41" s="5" t="s">
         <v>37</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="H41" s="5" t="s">
         <v>18</v>
@@ -2934,13 +2934,13 @@
         <v>19</v>
       </c>
       <c r="J41" s="5" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="K41" s="5" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="L41" s="5" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="M41" s="5" t="s">
         <v>43</v>
@@ -2948,25 +2948,25 @@
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="C42" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="E42" s="5" t="s">
         <v>37</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="G42" s="5" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="H42" s="5" t="s">
         <v>18</v>
@@ -2975,13 +2975,13 @@
         <v>19</v>
       </c>
       <c r="J42" s="5" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="K42" s="5" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="L42" s="5" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="M42" s="5" t="s">
         <v>43</v>
@@ -2989,25 +2989,25 @@
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="C43" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="E43" s="5" t="s">
         <v>37</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="H43" s="5" t="s">
         <v>18</v>
@@ -3016,13 +3016,13 @@
         <v>19</v>
       </c>
       <c r="J43" s="5" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="K43" s="5" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="L43" s="5" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="M43" s="5" t="s">
         <v>43</v>
@@ -3030,40 +3030,40 @@
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="C44" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="E44" s="5" t="s">
         <v>37</v>
       </c>
       <c r="F44" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="G44" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="H44" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I44" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J44" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="K44" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="L44" s="5" t="s">
         <v>182</v>
-      </c>
-      <c r="G44" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="H44" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I44" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J44" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="K44" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="L44" s="5" t="s">
-        <v>188</v>
       </c>
       <c r="M44" s="5" t="s">
         <v>43</v>
@@ -3071,37 +3071,37 @@
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="C45" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="E45" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="G45" s="5" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="H45" s="5" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="I45" s="5" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="J45" s="5" t="s">
         <v>54</v>
       </c>
       <c r="K45" s="5" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="L45" s="5" t="s">
         <v>55</v>
@@ -3112,37 +3112,37 @@
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46" s="5" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="C46" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="E46" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="G46" s="5" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="H46" s="5" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="I46" s="5" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="J46" s="5" t="s">
         <v>57</v>
       </c>
       <c r="K46" s="5" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="L46" s="5" t="s">
         <v>58</v>
@@ -3153,25 +3153,25 @@
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A47" s="5" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="C47" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="E47" s="5" t="s">
         <v>15</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="G47" s="5" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="H47" s="5" t="s">
         <v>18</v>
@@ -3180,39 +3180,39 @@
         <v>19</v>
       </c>
       <c r="J47" s="5" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="K47" s="5" t="s">
         <v>21</v>
       </c>
       <c r="L47" s="5" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="M47" s="5" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="C48" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="E48" s="5" t="s">
         <v>15</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="G48" s="5" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="H48" s="5" t="s">
         <v>18</v>
@@ -3221,54 +3221,54 @@
         <v>19</v>
       </c>
       <c r="J48" s="5" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="K48" s="5" t="s">
         <v>21</v>
       </c>
       <c r="L48" s="5" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="M48" s="5" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="C49" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D49" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="E49" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="F49" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="G49" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="H49" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I49" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J49" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="K49" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="L49" s="5" t="s">
         <v>205</v>
-      </c>
-      <c r="E49" s="5" t="s">
-        <v>206</v>
-      </c>
-      <c r="F49" s="5" t="s">
-        <v>207</v>
-      </c>
-      <c r="G49" s="5" t="s">
-        <v>208</v>
-      </c>
-      <c r="H49" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I49" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J49" s="5" t="s">
-        <v>209</v>
-      </c>
-      <c r="K49" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="L49" s="5" t="s">
-        <v>211</v>
       </c>
       <c r="M49" s="5" t="s">
         <v>43</v>
@@ -3276,25 +3276,25 @@
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="C50" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="E50" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="F50" s="5" t="s">
         <v>206</v>
       </c>
-      <c r="F50" s="5" t="s">
-        <v>212</v>
-      </c>
       <c r="G50" s="5" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="H50" s="5" t="s">
         <v>18</v>
@@ -3303,13 +3303,13 @@
         <v>19</v>
       </c>
       <c r="J50" s="5" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="K50" s="5" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="L50" s="5" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="M50" s="5" t="s">
         <v>43</v>
@@ -3317,25 +3317,25 @@
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="C51" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="F51" s="5" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="G51" s="5" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="H51" s="5" t="s">
         <v>18</v>
@@ -3344,13 +3344,13 @@
         <v>19</v>
       </c>
       <c r="J51" s="5" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="K51" s="5" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="L51" s="5" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="M51" s="5" t="s">
         <v>43</v>
@@ -3358,40 +3358,40 @@
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="C52" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="E52" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="F52" s="5" t="s">
         <v>206</v>
       </c>
-      <c r="F52" s="5" t="s">
-        <v>212</v>
-      </c>
       <c r="G52" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="H52" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I52" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J52" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="K52" s="5" t="s">
         <v>213</v>
       </c>
-      <c r="H52" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I52" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J52" s="5" t="s">
-        <v>221</v>
-      </c>
-      <c r="K52" s="5" t="s">
-        <v>219</v>
-      </c>
       <c r="L52" s="5" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="M52" s="5" t="s">
         <v>43</v>
@@ -3399,25 +3399,25 @@
     </row>
     <row r="53" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A53" s="5" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="C53" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="E53" s="5" t="s">
         <v>75</v>
       </c>
       <c r="F53" s="5" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="G53" s="5" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="H53" s="5" t="s">
         <v>78</v>
@@ -3426,39 +3426,39 @@
         <v>78</v>
       </c>
       <c r="J53" s="5" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="K53" s="5" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="L53" s="6" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="M53" s="5" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A54" s="5" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="C54" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="E54" s="5" t="s">
         <v>37</v>
       </c>
       <c r="F54" s="5" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="G54" s="5" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="H54" s="5" t="s">
         <v>18</v>
@@ -3467,13 +3467,13 @@
         <v>19</v>
       </c>
       <c r="J54" s="5" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="K54" s="5" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="L54" s="5" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="M54" s="5" t="s">
         <v>43</v>
@@ -3481,25 +3481,25 @@
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A55" s="5" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="C55" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="E55" s="5" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="G55" s="5" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="H55" s="5" t="s">
         <v>18</v>
@@ -3508,13 +3508,13 @@
         <v>19</v>
       </c>
       <c r="J55" s="5" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="K55" s="5" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="L55" s="5" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="M55" s="5" t="s">
         <v>43</v>
@@ -3522,40 +3522,40 @@
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A56" s="5" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="C56" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D56" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="E56" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="F56" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="G56" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="H56" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I56" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J56" s="5" t="s">
         <v>237</v>
       </c>
-      <c r="E56" s="5" t="s">
-        <v>206</v>
-      </c>
-      <c r="F56" s="5" t="s">
+      <c r="K56" s="5" t="s">
         <v>238</v>
       </c>
-      <c r="G56" s="5" t="s">
+      <c r="L56" s="5" t="s">
         <v>239</v>
-      </c>
-      <c r="H56" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I56" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J56" s="5" t="s">
-        <v>243</v>
-      </c>
-      <c r="K56" s="5" t="s">
-        <v>244</v>
-      </c>
-      <c r="L56" s="5" t="s">
-        <v>245</v>
       </c>
       <c r="M56" s="5" t="s">
         <v>43</v>

</xml_diff>

<commit_message>
Update Site Premium BIA038 Link 1
</commit_message>
<xml_diff>
--- a/data/premium-sites.xlsx
+++ b/data/premium-sites.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Local Repository\Telkom Projects\monitoring-site-premium-telegram-bot\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99C7CF0D-888C-4BF7-B2D4-0D59641D045D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B33F717-3B87-4355-A15A-7113F304CD33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -732,13 +732,7 @@
     <t>172.25.109.25</t>
   </si>
   <si>
-    <t>1/17/2:51</t>
-  </si>
-  <si>
     <t>ZTEG90041234</t>
-  </si>
-  <si>
-    <t>show gpon onu detail-info gpon_onu-1/17/2:51</t>
   </si>
   <si>
     <t>1/17/1:50</t>
@@ -900,6 +894,12 @@
   </si>
   <si>
     <t>smartgroup1 is up</t>
+  </si>
+  <si>
+    <t>1/9/1:50</t>
+  </si>
+  <si>
+    <t>show gpon onu detail-info gpon_onu-1/9/1:50</t>
   </si>
 </sst>
 </file>
@@ -1239,8 +1239,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="E59" sqref="E59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1290,10 +1290,10 @@
         <v>8</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="L1" s="4" t="s">
         <v>9</v>
@@ -1418,31 +1418,31 @@
         <v>29</v>
       </c>
       <c r="E4" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>253</v>
+      </c>
+      <c r="G4" s="5" t="s">
         <v>254</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="H4" s="5" t="s">
         <v>255</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="I4" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="J4" s="5" t="s">
         <v>256</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="K4" s="5" t="s">
         <v>257</v>
       </c>
-      <c r="I4" s="5" t="s">
-        <v>257</v>
-      </c>
-      <c r="J4" s="5" t="s">
+      <c r="L4" s="6" t="s">
         <v>258</v>
       </c>
-      <c r="K4" s="5" t="s">
+      <c r="M4" s="5" t="s">
         <v>259</v>
-      </c>
-      <c r="L4" s="6" t="s">
-        <v>260</v>
-      </c>
-      <c r="M4" s="5" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.3">
@@ -1459,31 +1459,31 @@
         <v>29</v>
       </c>
       <c r="E5" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>253</v>
+      </c>
+      <c r="G5" s="5" t="s">
         <v>254</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="H5" s="5" t="s">
         <v>255</v>
       </c>
-      <c r="G5" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="H5" s="5" t="s">
+      <c r="I5" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="K5" s="5" t="s">
         <v>257</v>
       </c>
-      <c r="I5" s="5" t="s">
-        <v>257</v>
-      </c>
-      <c r="J5" s="5" t="s">
+      <c r="L5" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="M5" s="5" t="s">
         <v>262</v>
-      </c>
-      <c r="K5" s="5" t="s">
-        <v>259</v>
-      </c>
-      <c r="L5" s="5" t="s">
-        <v>263</v>
-      </c>
-      <c r="M5" s="5" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="6" spans="1:33" ht="28.8" x14ac:dyDescent="0.3">
@@ -1535,7 +1535,7 @@
         <v>28</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>29</v>
@@ -1576,7 +1576,7 @@
         <v>28</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>29</v>
@@ -1641,7 +1641,7 @@
         <v>54</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="L9" s="5" t="s">
         <v>55</v>
@@ -1682,7 +1682,7 @@
         <v>57</v>
       </c>
       <c r="K10" s="5" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="L10" s="5" t="s">
         <v>58</v>
@@ -1786,16 +1786,16 @@
         <v>19</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="K13" s="5" t="s">
         <v>21</v>
       </c>
       <c r="L13" s="6" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="M13" s="5" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="14" spans="1:33" x14ac:dyDescent="0.3">
@@ -1827,16 +1827,16 @@
         <v>19</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="K14" s="5" t="s">
         <v>21</v>
       </c>
       <c r="L14" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="M14" s="5" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="15" spans="1:33" ht="28.8" x14ac:dyDescent="0.3">
@@ -1868,16 +1868,16 @@
         <v>78</v>
       </c>
       <c r="J15" s="5" t="s">
+        <v>282</v>
+      </c>
+      <c r="K15" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="L15" s="6" t="s">
+        <v>283</v>
+      </c>
+      <c r="M15" s="5" t="s">
         <v>284</v>
-      </c>
-      <c r="K15" s="5" t="s">
-        <v>242</v>
-      </c>
-      <c r="L15" s="6" t="s">
-        <v>285</v>
-      </c>
-      <c r="M15" s="5" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="16" spans="1:33" ht="28.8" x14ac:dyDescent="0.3">
@@ -1909,16 +1909,16 @@
         <v>78</v>
       </c>
       <c r="J16" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="K16" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="L16" s="6" t="s">
+        <v>286</v>
+      </c>
+      <c r="M16" s="5" t="s">
         <v>287</v>
-      </c>
-      <c r="K16" s="5" t="s">
-        <v>242</v>
-      </c>
-      <c r="L16" s="6" t="s">
-        <v>288</v>
-      </c>
-      <c r="M16" s="5" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
@@ -1947,7 +1947,7 @@
         <v>83</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="J17" s="5" t="s">
         <v>54</v>
@@ -1988,7 +1988,7 @@
         <v>83</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="J18" s="5" t="s">
         <v>57</v>
@@ -2029,7 +2029,7 @@
         <v>83</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="J19" s="5" t="s">
         <v>89</v>
@@ -2070,7 +2070,7 @@
         <v>83</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="J20" s="5" t="s">
         <v>92</v>
@@ -2184,22 +2184,22 @@
         <v>51</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="H23" s="5" t="s">
         <v>83</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="J23" s="5" t="s">
         <v>54</v>
       </c>
       <c r="K23" s="5" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="L23" s="6" t="s">
         <v>55</v>
@@ -2225,22 +2225,22 @@
         <v>51</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="H24" s="5" t="s">
         <v>83</v>
       </c>
       <c r="I24" s="5" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="J24" s="5" t="s">
         <v>57</v>
       </c>
       <c r="K24" s="5" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="L24" s="5" t="s">
         <v>58</v>
@@ -2357,7 +2357,7 @@
         <v>83</v>
       </c>
       <c r="I27" s="5" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="J27" s="5" t="s">
         <v>54</v>
@@ -2398,7 +2398,7 @@
         <v>83</v>
       </c>
       <c r="I28" s="5" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="J28" s="5" t="s">
         <v>57</v>
@@ -2430,25 +2430,25 @@
         <v>37</v>
       </c>
       <c r="F29" s="5" t="s">
+        <v>269</v>
+      </c>
+      <c r="G29" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="H29" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I29" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J29" s="5" t="s">
         <v>271</v>
       </c>
-      <c r="G29" s="5" t="s">
+      <c r="K29" s="5" t="s">
         <v>272</v>
       </c>
-      <c r="H29" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I29" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J29" s="5" t="s">
+      <c r="L29" s="6" t="s">
         <v>273</v>
-      </c>
-      <c r="K29" s="5" t="s">
-        <v>274</v>
-      </c>
-      <c r="L29" s="6" t="s">
-        <v>275</v>
       </c>
       <c r="M29" s="5" t="s">
         <v>43</v>
@@ -2471,25 +2471,25 @@
         <v>37</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="G30" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="H30" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I30" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J30" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="K30" s="5" t="s">
         <v>272</v>
       </c>
-      <c r="H30" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I30" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J30" s="5" t="s">
-        <v>282</v>
-      </c>
-      <c r="K30" s="5" t="s">
-        <v>274</v>
-      </c>
       <c r="L30" s="5" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="M30" s="5" t="s">
         <v>43</v>
@@ -2691,7 +2691,7 @@
         <v>54</v>
       </c>
       <c r="K35" s="5" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="L35" s="5" t="s">
         <v>148</v>
@@ -2732,7 +2732,7 @@
         <v>57</v>
       </c>
       <c r="K36" s="5" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="L36" s="5" t="s">
         <v>150</v>
@@ -2758,10 +2758,10 @@
         <v>37</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="H37" s="5" t="s">
         <v>18</v>
@@ -2773,7 +2773,7 @@
         <v>161</v>
       </c>
       <c r="K37" s="5" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="L37" s="6" t="s">
         <v>162</v>
@@ -2799,25 +2799,25 @@
         <v>37</v>
       </c>
       <c r="F38" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="G38" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="H38" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I38" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J38" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="K38" s="5" t="s">
         <v>276</v>
       </c>
-      <c r="G38" s="5" t="s">
-        <v>277</v>
-      </c>
-      <c r="H38" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I38" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J38" s="5" t="s">
-        <v>279</v>
-      </c>
-      <c r="K38" s="5" t="s">
+      <c r="L38" s="5" t="s">
         <v>278</v>
-      </c>
-      <c r="L38" s="5" t="s">
-        <v>280</v>
       </c>
       <c r="M38" s="5" t="s">
         <v>43</v>
@@ -2855,7 +2855,7 @@
         <v>157</v>
       </c>
       <c r="K39" s="5" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="L39" s="5" t="s">
         <v>158</v>
@@ -2896,7 +2896,7 @@
         <v>161</v>
       </c>
       <c r="K40" s="5" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="L40" s="5" t="s">
         <v>162</v>
@@ -3095,13 +3095,13 @@
         <v>83</v>
       </c>
       <c r="I45" s="5" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="J45" s="5" t="s">
         <v>54</v>
       </c>
       <c r="K45" s="5" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="L45" s="5" t="s">
         <v>55</v>
@@ -3136,13 +3136,13 @@
         <v>83</v>
       </c>
       <c r="I46" s="5" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="J46" s="5" t="s">
         <v>57</v>
       </c>
       <c r="K46" s="5" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="L46" s="5" t="s">
         <v>58</v>
@@ -3429,7 +3429,7 @@
         <v>221</v>
       </c>
       <c r="K53" s="5" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="L53" s="6" t="s">
         <v>222</v>
@@ -3508,13 +3508,13 @@
         <v>19</v>
       </c>
       <c r="J55" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="K55" s="5" t="s">
         <v>234</v>
       </c>
-      <c r="K55" s="5" t="s">
-        <v>235</v>
-      </c>
       <c r="L55" s="5" t="s">
-        <v>236</v>
+        <v>289</v>
       </c>
       <c r="M55" s="5" t="s">
         <v>43</v>
@@ -3549,13 +3549,13 @@
         <v>19</v>
       </c>
       <c r="J56" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="K56" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="L56" s="5" t="s">
         <v>237</v>
-      </c>
-      <c r="K56" s="5" t="s">
-        <v>238</v>
-      </c>
-      <c r="L56" s="5" t="s">
-        <v>239</v>
       </c>
       <c r="M56" s="5" t="s">
         <v>43</v>

</xml_diff>

<commit_message>
Update Site Premium SDR006 Link 1 & Link 2
</commit_message>
<xml_diff>
--- a/data/premium-sites.xlsx
+++ b/data/premium-sites.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Local Repository\Telkom Projects\monitoring-site-premium-telegram-bot\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B33F717-3B87-4355-A15A-7113F304CD33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35C94808-0E9B-49C3-A089-43480CDC2CD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="728" uniqueCount="288">
   <si>
     <t>Subdistrict</t>
   </si>
@@ -214,31 +214,6 @@
     <t>Maiwa</t>
   </si>
   <si>
-    <t>OLT FH A5161</t>
-  </si>
-  <si>
-    <t>GPON00-D7-RPN-4MRA</t>
-  </si>
-  <si>
-    <t>172.25.212.135</t>
-  </si>
-  <si>
-    <t>1/13/1</t>
-  </si>
-  <si>
-    <t>FHTT05e879f2</t>
-  </si>
-  <si>
-    <t>cd onu
-show onu_state slot 1 pon 13 onu 1</t>
-  </si>
-  <si>
-    <t>status : active.</t>
-  </si>
-  <si>
-    <t>Unmonitor</t>
-  </si>
-  <si>
     <t>WTG001</t>
   </si>
   <si>
@@ -900,6 +875,24 @@
   </si>
   <si>
     <t>show gpon onu detail-info gpon_onu-1/9/1:50</t>
+  </si>
+  <si>
+    <t>SW-D7-TSEL-SDR006</t>
+  </si>
+  <si>
+    <t>10.199.152.207</t>
+  </si>
+  <si>
+    <t>Admin123</t>
+  </si>
+  <si>
+    <t>NYUKWIB20004</t>
+  </si>
+  <si>
+    <t>gigaethernet 1/0/4</t>
+  </si>
+  <si>
+    <t>show rlink interface gigaethernet 1/0/4</t>
   </si>
 </sst>
 </file>
@@ -1239,8 +1232,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="E59" sqref="E59"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1290,10 +1283,10 @@
         <v>8</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="L1" s="4" t="s">
         <v>9</v>
@@ -1418,31 +1411,31 @@
         <v>29</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="L4" s="6" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="M4" s="5" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.3">
@@ -1459,31 +1452,31 @@
         <v>29</v>
       </c>
       <c r="E5" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="J5" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="K5" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="L5" s="5" t="s">
         <v>253</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="M5" s="5" t="s">
         <v>254</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>255</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>255</v>
-      </c>
-      <c r="J5" s="5" t="s">
-        <v>260</v>
-      </c>
-      <c r="K5" s="5" t="s">
-        <v>257</v>
-      </c>
-      <c r="L5" s="5" t="s">
-        <v>261</v>
-      </c>
-      <c r="M5" s="5" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="6" spans="1:33" ht="28.8" x14ac:dyDescent="0.3">
@@ -1535,7 +1528,7 @@
         <v>28</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>29</v>
@@ -1576,7 +1569,7 @@
         <v>28</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>29</v>
@@ -1641,7 +1634,7 @@
         <v>54</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="L9" s="5" t="s">
         <v>55</v>
@@ -1682,7 +1675,7 @@
         <v>57</v>
       </c>
       <c r="K10" s="5" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="L10" s="5" t="s">
         <v>58</v>
@@ -1691,7 +1684,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="1:33" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>59</v>
       </c>
@@ -1705,31 +1698,31 @@
         <v>61</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>63</v>
+        <v>282</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>64</v>
+        <v>283</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>18</v>
+        <v>75</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>19</v>
+        <v>284</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="K11" s="5" t="s">
-        <v>66</v>
+        <v>285</v>
       </c>
       <c r="L11" s="6" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="M11" s="5" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:33" x14ac:dyDescent="0.3">
@@ -1746,29 +1739,45 @@
         <v>61</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="5"/>
-      <c r="L12" s="5"/>
-      <c r="M12" s="5"/>
+        <v>51</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>282</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="K12" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="L12" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="M12" s="5" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="13" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>59</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>15</v>
@@ -1786,16 +1795,16 @@
         <v>19</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="K13" s="5" t="s">
         <v>21</v>
       </c>
       <c r="L13" s="6" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="M13" s="5" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
     </row>
     <row r="14" spans="1:33" x14ac:dyDescent="0.3">
@@ -1803,13 +1812,13 @@
         <v>59</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>15</v>
@@ -1827,133 +1836,133 @@
         <v>19</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="K14" s="5" t="s">
         <v>21</v>
       </c>
       <c r="L14" s="5" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="M14" s="5" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
     </row>
     <row r="15" spans="1:33" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="J15" s="5" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="K15" s="5" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="L15" s="6" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="M15" s="5" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
     </row>
     <row r="16" spans="1:33" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
       <c r="K16" s="5" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="L16" s="6" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
       <c r="M16" s="5" t="s">
-        <v>287</v>
+        <v>279</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="J17" s="5" t="s">
         <v>54</v>
       </c>
       <c r="K17" s="5" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="L17" s="5" t="s">
         <v>55</v>
@@ -1964,37 +1973,37 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="J18" s="5" t="s">
         <v>57</v>
       </c>
       <c r="K18" s="5" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="L18" s="5" t="s">
         <v>58</v>
@@ -2005,40 +2014,40 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="E19" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="H19" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="J19" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="K19" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="L19" s="5" t="s">
         <v>83</v>
-      </c>
-      <c r="I19" s="5" t="s">
-        <v>241</v>
-      </c>
-      <c r="J19" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="K19" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="L19" s="5" t="s">
-        <v>91</v>
       </c>
       <c r="M19" s="5" t="s">
         <v>56</v>
@@ -2046,40 +2055,40 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="K20" s="5" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="L20" s="5" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="M20" s="5" t="s">
         <v>56</v>
@@ -2087,25 +2096,25 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="E21" s="5" t="s">
         <v>15</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="H21" s="5" t="s">
         <v>18</v>
@@ -2114,39 +2123,39 @@
         <v>19</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="K21" s="5" t="s">
         <v>21</v>
       </c>
       <c r="L21" s="5" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="M21" s="5" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="E22" s="5" t="s">
         <v>15</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="H22" s="5" t="s">
         <v>18</v>
@@ -2155,51 +2164,51 @@
         <v>19</v>
       </c>
       <c r="J22" s="5" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="K22" s="5" t="s">
         <v>21</v>
       </c>
       <c r="L22" s="5" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="M22" s="5" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="E23" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="J23" s="5" t="s">
         <v>54</v>
       </c>
       <c r="K23" s="5" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="L23" s="6" t="s">
         <v>55</v>
@@ -2210,37 +2219,37 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="E24" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="I24" s="5" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="J24" s="5" t="s">
         <v>57</v>
       </c>
       <c r="K24" s="5" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="L24" s="5" t="s">
         <v>58</v>
@@ -2251,25 +2260,25 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="H25" s="5" t="s">
         <v>18</v>
@@ -2278,13 +2287,13 @@
         <v>19</v>
       </c>
       <c r="J25" s="5" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="K25" s="5" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="L25" s="5" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="M25" s="5" t="s">
         <v>43</v>
@@ -2292,40 +2301,40 @@
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D26" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="G26" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="E26" s="5" t="s">
+      <c r="H26" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I26" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J26" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="F26" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="G26" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="H26" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I26" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J26" s="5" t="s">
-        <v>119</v>
-      </c>
       <c r="K26" s="5" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="L26" s="5" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="M26" s="5" t="s">
         <v>43</v>
@@ -2333,37 +2342,37 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="E27" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="I27" s="5" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="J27" s="5" t="s">
         <v>54</v>
       </c>
       <c r="K27" s="5" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="L27" s="5" t="s">
         <v>55</v>
@@ -2374,37 +2383,37 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="E28" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="H28" s="5" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="I28" s="5" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="J28" s="5" t="s">
         <v>57</v>
       </c>
       <c r="K28" s="5" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="L28" s="5" t="s">
         <v>58</v>
@@ -2415,25 +2424,25 @@
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="E29" s="5" t="s">
         <v>37</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
       <c r="H29" s="5" t="s">
         <v>18</v>
@@ -2442,13 +2451,13 @@
         <v>19</v>
       </c>
       <c r="J29" s="5" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
       <c r="K29" s="5" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="L29" s="6" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
       <c r="M29" s="5" t="s">
         <v>43</v>
@@ -2456,25 +2465,25 @@
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="E30" s="5" t="s">
         <v>37</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
       <c r="H30" s="5" t="s">
         <v>18</v>
@@ -2483,13 +2492,13 @@
         <v>19</v>
       </c>
       <c r="J30" s="5" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="K30" s="5" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="L30" s="5" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
       <c r="M30" s="5" t="s">
         <v>43</v>
@@ -2497,25 +2506,25 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="C31" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="E31" s="5" t="s">
         <v>37</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="H31" s="5" t="s">
         <v>18</v>
@@ -2524,13 +2533,13 @@
         <v>19</v>
       </c>
       <c r="J31" s="5" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="K31" s="5" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="L31" s="5" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="M31" s="5" t="s">
         <v>43</v>
@@ -2538,25 +2547,25 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="C32" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="E32" s="5" t="s">
         <v>37</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="H32" s="5" t="s">
         <v>18</v>
@@ -2565,13 +2574,13 @@
         <v>19</v>
       </c>
       <c r="J32" s="5" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="K32" s="5" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="L32" s="5" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="M32" s="5" t="s">
         <v>43</v>
@@ -2579,25 +2588,25 @@
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="C33" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="E33" s="5" t="s">
         <v>37</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="H33" s="5" t="s">
         <v>18</v>
@@ -2606,13 +2615,13 @@
         <v>19</v>
       </c>
       <c r="J33" s="5" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="K33" s="5" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="L33" s="5" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="M33" s="5" t="s">
         <v>43</v>
@@ -2620,25 +2629,25 @@
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="C34" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="E34" s="5" t="s">
         <v>37</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="G34" s="5" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="H34" s="5" t="s">
         <v>18</v>
@@ -2647,13 +2656,13 @@
         <v>19</v>
       </c>
       <c r="J34" s="5" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="K34" s="5" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="L34" s="5" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="M34" s="5" t="s">
         <v>43</v>
@@ -2661,25 +2670,25 @@
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="C35" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="H35" s="5" t="s">
         <v>18</v>
@@ -2691,36 +2700,36 @@
         <v>54</v>
       </c>
       <c r="K35" s="5" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="L35" s="5" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="M35" s="5" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="C36" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="G36" s="5" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="H36" s="5" t="s">
         <v>18</v>
@@ -2732,36 +2741,36 @@
         <v>57</v>
       </c>
       <c r="K36" s="5" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="L36" s="5" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="M36" s="5" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="C37" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="E37" s="5" t="s">
         <v>37</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
       <c r="H37" s="5" t="s">
         <v>18</v>
@@ -2770,13 +2779,13 @@
         <v>19</v>
       </c>
       <c r="J37" s="5" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="K37" s="5" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="L37" s="6" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="M37" s="5" t="s">
         <v>43</v>
@@ -2784,25 +2793,25 @@
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="E38" s="5" t="s">
         <v>37</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="G38" s="5" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
       <c r="H38" s="5" t="s">
         <v>18</v>
@@ -2811,13 +2820,13 @@
         <v>19</v>
       </c>
       <c r="J38" s="5" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="K38" s="5" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="L38" s="5" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="M38" s="5" t="s">
         <v>43</v>
@@ -2825,25 +2834,25 @@
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="E39" s="5" t="s">
         <v>37</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="H39" s="5" t="s">
         <v>18</v>
@@ -2852,13 +2861,13 @@
         <v>19</v>
       </c>
       <c r="J39" s="5" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="K39" s="5" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
       <c r="L39" s="5" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="M39" s="5" t="s">
         <v>43</v>
@@ -2866,25 +2875,25 @@
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="C40" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="E40" s="5" t="s">
         <v>37</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="G40" s="5" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="H40" s="5" t="s">
         <v>18</v>
@@ -2893,13 +2902,13 @@
         <v>19</v>
       </c>
       <c r="J40" s="5" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="K40" s="5" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
       <c r="L40" s="5" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="M40" s="5" t="s">
         <v>43</v>
@@ -2907,25 +2916,25 @@
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41" s="5" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="C41" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="E41" s="5" t="s">
         <v>37</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="H41" s="5" t="s">
         <v>18</v>
@@ -2934,13 +2943,13 @@
         <v>19</v>
       </c>
       <c r="J41" s="5" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="K41" s="5" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="L41" s="5" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="M41" s="5" t="s">
         <v>43</v>
@@ -2948,25 +2957,25 @@
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="C42" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="E42" s="5" t="s">
         <v>37</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="G42" s="5" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="H42" s="5" t="s">
         <v>18</v>
@@ -2975,13 +2984,13 @@
         <v>19</v>
       </c>
       <c r="J42" s="5" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="K42" s="5" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="L42" s="5" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="M42" s="5" t="s">
         <v>43</v>
@@ -2989,25 +2998,25 @@
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="C43" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="E43" s="5" t="s">
         <v>37</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="H43" s="5" t="s">
         <v>18</v>
@@ -3016,13 +3025,13 @@
         <v>19</v>
       </c>
       <c r="J43" s="5" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="K43" s="5" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="L43" s="5" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="M43" s="5" t="s">
         <v>43</v>
@@ -3030,25 +3039,25 @@
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="C44" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="E44" s="5" t="s">
         <v>37</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="G44" s="5" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="H44" s="5" t="s">
         <v>18</v>
@@ -3057,13 +3066,13 @@
         <v>19</v>
       </c>
       <c r="J44" s="5" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="K44" s="5" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="L44" s="5" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="M44" s="5" t="s">
         <v>43</v>
@@ -3071,37 +3080,37 @@
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="C45" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="E45" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="G45" s="5" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="H45" s="5" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="I45" s="5" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="J45" s="5" t="s">
         <v>54</v>
       </c>
       <c r="K45" s="5" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="L45" s="5" t="s">
         <v>55</v>
@@ -3112,37 +3121,37 @@
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46" s="5" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="C46" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="E46" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="G46" s="5" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="H46" s="5" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="I46" s="5" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="J46" s="5" t="s">
         <v>57</v>
       </c>
       <c r="K46" s="5" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="L46" s="5" t="s">
         <v>58</v>
@@ -3153,25 +3162,25 @@
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A47" s="5" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="C47" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="E47" s="5" t="s">
         <v>15</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="G47" s="5" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="H47" s="5" t="s">
         <v>18</v>
@@ -3180,39 +3189,39 @@
         <v>19</v>
       </c>
       <c r="J47" s="5" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="K47" s="5" t="s">
         <v>21</v>
       </c>
       <c r="L47" s="5" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="M47" s="5" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="C48" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="E48" s="5" t="s">
         <v>15</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="G48" s="5" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="H48" s="5" t="s">
         <v>18</v>
@@ -3221,39 +3230,39 @@
         <v>19</v>
       </c>
       <c r="J48" s="5" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="K48" s="5" t="s">
         <v>21</v>
       </c>
       <c r="L48" s="5" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="M48" s="5" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="C49" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="G49" s="5" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="H49" s="5" t="s">
         <v>18</v>
@@ -3262,13 +3271,13 @@
         <v>19</v>
       </c>
       <c r="J49" s="5" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="K49" s="5" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="L49" s="5" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="M49" s="5" t="s">
         <v>43</v>
@@ -3276,40 +3285,40 @@
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="C50" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D50" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="E50" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="F50" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="G50" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="E50" s="5" t="s">
+      <c r="H50" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I50" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J50" s="5" t="s">
         <v>200</v>
       </c>
-      <c r="F50" s="5" t="s">
-        <v>206</v>
-      </c>
-      <c r="G50" s="5" t="s">
-        <v>207</v>
-      </c>
-      <c r="H50" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I50" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J50" s="5" t="s">
-        <v>208</v>
-      </c>
       <c r="K50" s="5" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="L50" s="5" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="M50" s="5" t="s">
         <v>43</v>
@@ -3317,25 +3326,25 @@
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="C51" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="F51" s="5" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="G51" s="5" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="H51" s="5" t="s">
         <v>18</v>
@@ -3344,13 +3353,13 @@
         <v>19</v>
       </c>
       <c r="J51" s="5" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="K51" s="5" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="L51" s="5" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="M51" s="5" t="s">
         <v>43</v>
@@ -3358,40 +3367,40 @@
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="C52" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="F52" s="5" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="G52" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="H52" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I52" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J52" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="H52" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I52" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J52" s="5" t="s">
-        <v>215</v>
-      </c>
       <c r="K52" s="5" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="L52" s="5" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="M52" s="5" t="s">
         <v>43</v>
@@ -3399,66 +3408,66 @@
     </row>
     <row r="53" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A53" s="5" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="C53" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="F53" s="5" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="G53" s="5" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="H53" s="5" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="I53" s="5" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="J53" s="5" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="K53" s="5" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="L53" s="6" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="M53" s="5" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A54" s="5" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="C54" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="E54" s="5" t="s">
         <v>37</v>
       </c>
       <c r="F54" s="5" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="G54" s="5" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="H54" s="5" t="s">
         <v>18</v>
@@ -3467,13 +3476,13 @@
         <v>19</v>
       </c>
       <c r="J54" s="5" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="K54" s="5" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="L54" s="5" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
       <c r="M54" s="5" t="s">
         <v>43</v>
@@ -3481,25 +3490,25 @@
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A55" s="5" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="C55" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="E55" s="5" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="G55" s="5" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="H55" s="5" t="s">
         <v>18</v>
@@ -3508,13 +3517,13 @@
         <v>19</v>
       </c>
       <c r="J55" s="5" t="s">
-        <v>288</v>
+        <v>280</v>
       </c>
       <c r="K55" s="5" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="L55" s="5" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
       <c r="M55" s="5" t="s">
         <v>43</v>
@@ -3522,25 +3531,25 @@
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A56" s="5" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="C56" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="E56" s="5" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="F56" s="5" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="G56" s="5" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="H56" s="5" t="s">
         <v>18</v>
@@ -3549,13 +3558,13 @@
         <v>19</v>
       </c>
       <c r="J56" s="5" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="K56" s="5" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="L56" s="5" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
       <c r="M56" s="5" t="s">
         <v>43</v>

</xml_diff>

<commit_message>
Change BIA witel to Papua
</commit_message>
<xml_diff>
--- a/data/premium-sites.xlsx
+++ b/data/premium-sites.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Local Repository\Telkom Projects\monitoring-site-premium-telegram-bot\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DE2ACF0-BFCB-4000-9F97-DDA3DC83B924}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7529B6F3-B3C6-4985-8308-2DCA1F65DEF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="731" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="731" uniqueCount="289">
   <si>
     <t>Subdistrict</t>
   </si>
@@ -678,9 +678,6 @@
   </si>
   <si>
     <t>show gpon onu detail gpon-onu_1/3/1:12</t>
-  </si>
-  <si>
-    <t>PAPUA BARAT</t>
   </si>
   <si>
     <t>BIA038</t>
@@ -1238,8 +1235,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="I49" sqref="I49"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="E59" sqref="E59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1290,13 +1287,13 @@
         <v>8</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="M1" s="4" t="s">
         <v>9</v>
@@ -1422,32 +1419,32 @@
         <v>29</v>
       </c>
       <c r="E4" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="F4" s="5" t="s">
         <v>240</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="G4" s="5" t="s">
         <v>241</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="H4" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="H4" s="5" t="s">
-        <v>243</v>
-      </c>
       <c r="I4" s="5" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="J4" s="5"/>
       <c r="K4" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="L4" s="6" t="s">
         <v>244</v>
       </c>
-      <c r="L4" s="6" t="s">
+      <c r="M4" s="5" t="s">
         <v>245</v>
       </c>
-      <c r="M4" s="5" t="s">
+      <c r="N4" s="1" t="s">
         <v>246</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.3">
@@ -1464,32 +1461,32 @@
         <v>29</v>
       </c>
       <c r="E5" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="F5" s="5" t="s">
         <v>240</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="G5" s="5" t="s">
         <v>241</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="H5" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="H5" s="5" t="s">
-        <v>243</v>
-      </c>
       <c r="I5" s="5" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="J5" s="5"/>
       <c r="K5" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="L5" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="M5" s="5" t="s">
         <v>248</v>
       </c>
-      <c r="L5" s="5" t="s">
-        <v>245</v>
-      </c>
-      <c r="M5" s="5" t="s">
+      <c r="N5" s="1" t="s">
         <v>249</v>
-      </c>
-      <c r="N5" s="1" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="6" spans="1:33" ht="28.8" x14ac:dyDescent="0.3">
@@ -1542,7 +1539,7 @@
         <v>28</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>29</v>
@@ -1584,7 +1581,7 @@
         <v>28</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>29</v>
@@ -1651,7 +1648,7 @@
         <v>54</v>
       </c>
       <c r="L9" s="5" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="M9" s="5" t="s">
         <v>55</v>
@@ -1693,7 +1690,7 @@
         <v>57</v>
       </c>
       <c r="L10" s="5" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="M10" s="5" t="s">
         <v>58</v>
@@ -1719,23 +1716,23 @@
         <v>51</v>
       </c>
       <c r="F11" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="G11" s="5" t="s">
         <v>278</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>279</v>
       </c>
       <c r="H11" s="5" t="s">
         <v>75</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="J11" s="5"/>
       <c r="K11" s="5" t="s">
         <v>54</v>
       </c>
       <c r="L11" s="6" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="M11" s="5" t="s">
         <v>55</v>
@@ -1761,26 +1758,26 @@
         <v>51</v>
       </c>
       <c r="F12" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="G12" s="5" t="s">
         <v>278</v>
-      </c>
-      <c r="G12" s="5" t="s">
-        <v>279</v>
       </c>
       <c r="H12" s="5" t="s">
         <v>75</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="J12" s="5"/>
       <c r="K12" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="L12" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="M12" s="5" t="s">
         <v>282</v>
-      </c>
-      <c r="L12" s="5" t="s">
-        <v>281</v>
-      </c>
-      <c r="M12" s="5" t="s">
-        <v>283</v>
       </c>
       <c r="N12" s="1" t="s">
         <v>56</v>
@@ -1816,16 +1813,16 @@
       </c>
       <c r="J13" s="5"/>
       <c r="K13" s="5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="L13" s="6" t="s">
         <v>21</v>
       </c>
       <c r="M13" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="N13" s="1" t="s">
         <v>235</v>
-      </c>
-      <c r="N13" s="1" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="14" spans="1:33" x14ac:dyDescent="0.3">
@@ -1858,16 +1855,16 @@
       </c>
       <c r="J14" s="5"/>
       <c r="K14" s="5" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="L14" s="5" t="s">
         <v>21</v>
       </c>
       <c r="M14" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="N14" s="1" t="s">
         <v>238</v>
-      </c>
-      <c r="N14" s="1" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="15" spans="1:33" ht="28.8" x14ac:dyDescent="0.3">
@@ -1900,16 +1897,16 @@
       </c>
       <c r="J15" s="5"/>
       <c r="K15" s="5" t="s">
+        <v>269</v>
+      </c>
+      <c r="L15" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="M15" s="6" t="s">
         <v>270</v>
       </c>
-      <c r="L15" s="6" t="s">
-        <v>228</v>
-      </c>
-      <c r="M15" s="6" t="s">
+      <c r="N15" s="1" t="s">
         <v>271</v>
-      </c>
-      <c r="N15" s="1" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="16" spans="1:33" ht="28.8" x14ac:dyDescent="0.3">
@@ -1942,16 +1939,16 @@
       </c>
       <c r="J16" s="5"/>
       <c r="K16" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="L16" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="M16" s="6" t="s">
         <v>273</v>
       </c>
-      <c r="L16" s="6" t="s">
-        <v>228</v>
-      </c>
-      <c r="M16" s="6" t="s">
+      <c r="N16" s="1" t="s">
         <v>274</v>
-      </c>
-      <c r="N16" s="1" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.3">
@@ -1980,7 +1977,7 @@
         <v>75</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="J17" s="5"/>
       <c r="K17" s="5" t="s">
@@ -2022,7 +2019,7 @@
         <v>75</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="J18" s="5"/>
       <c r="K18" s="5" t="s">
@@ -2064,7 +2061,7 @@
         <v>75</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="J19" s="5"/>
       <c r="K19" s="5" t="s">
@@ -2106,7 +2103,7 @@
         <v>75</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="J20" s="5"/>
       <c r="K20" s="5" t="s">
@@ -2223,23 +2220,23 @@
         <v>51</v>
       </c>
       <c r="F23" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="G23" s="5" t="s">
         <v>253</v>
-      </c>
-      <c r="G23" s="5" t="s">
-        <v>254</v>
       </c>
       <c r="H23" s="5" t="s">
         <v>75</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="J23" s="5"/>
       <c r="K23" s="5" t="s">
         <v>54</v>
       </c>
       <c r="L23" s="6" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="M23" s="5" t="s">
         <v>55</v>
@@ -2265,23 +2262,23 @@
         <v>51</v>
       </c>
       <c r="F24" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="G24" s="5" t="s">
         <v>253</v>
-      </c>
-      <c r="G24" s="5" t="s">
-        <v>254</v>
       </c>
       <c r="H24" s="5" t="s">
         <v>75</v>
       </c>
       <c r="I24" s="5" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="J24" s="5"/>
       <c r="K24" s="5" t="s">
         <v>57</v>
       </c>
       <c r="L24" s="5" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="M24" s="5" t="s">
         <v>58</v>
@@ -2400,7 +2397,7 @@
         <v>75</v>
       </c>
       <c r="I27" s="5" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="J27" s="5"/>
       <c r="K27" s="5" t="s">
@@ -2442,7 +2439,7 @@
         <v>75</v>
       </c>
       <c r="I28" s="5" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="J28" s="5"/>
       <c r="K28" s="5" t="s">
@@ -2475,10 +2472,10 @@
         <v>37</v>
       </c>
       <c r="F29" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="G29" s="5" t="s">
         <v>257</v>
-      </c>
-      <c r="G29" s="5" t="s">
-        <v>258</v>
       </c>
       <c r="H29" s="5" t="s">
         <v>18</v>
@@ -2488,13 +2485,13 @@
       </c>
       <c r="J29" s="5"/>
       <c r="K29" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="L29" s="6" t="s">
         <v>259</v>
       </c>
-      <c r="L29" s="6" t="s">
+      <c r="M29" s="5" t="s">
         <v>260</v>
-      </c>
-      <c r="M29" s="5" t="s">
-        <v>261</v>
       </c>
       <c r="N29" s="1" t="s">
         <v>43</v>
@@ -2517,10 +2514,10 @@
         <v>37</v>
       </c>
       <c r="F30" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="G30" s="5" t="s">
         <v>257</v>
-      </c>
-      <c r="G30" s="5" t="s">
-        <v>258</v>
       </c>
       <c r="H30" s="5" t="s">
         <v>18</v>
@@ -2530,13 +2527,13 @@
       </c>
       <c r="J30" s="5"/>
       <c r="K30" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="L30" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="M30" s="5" t="s">
         <v>268</v>
-      </c>
-      <c r="L30" s="5" t="s">
-        <v>260</v>
-      </c>
-      <c r="M30" s="5" t="s">
-        <v>269</v>
       </c>
       <c r="N30" s="1" t="s">
         <v>43</v>
@@ -2743,7 +2740,7 @@
         <v>54</v>
       </c>
       <c r="L35" s="5" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="M35" s="5" t="s">
         <v>140</v>
@@ -2785,7 +2782,7 @@
         <v>57</v>
       </c>
       <c r="L36" s="5" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="M36" s="5" t="s">
         <v>142</v>
@@ -2811,10 +2808,10 @@
         <v>37</v>
       </c>
       <c r="F37" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="G37" s="5" t="s">
         <v>262</v>
-      </c>
-      <c r="G37" s="5" t="s">
-        <v>263</v>
       </c>
       <c r="H37" s="5" t="s">
         <v>18</v>
@@ -2827,7 +2824,7 @@
         <v>153</v>
       </c>
       <c r="L37" s="6" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="M37" s="5" t="s">
         <v>154</v>
@@ -2853,10 +2850,10 @@
         <v>37</v>
       </c>
       <c r="F38" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="G38" s="5" t="s">
         <v>262</v>
-      </c>
-      <c r="G38" s="5" t="s">
-        <v>263</v>
       </c>
       <c r="H38" s="5" t="s">
         <v>18</v>
@@ -2866,13 +2863,13 @@
       </c>
       <c r="J38" s="5"/>
       <c r="K38" s="5" t="s">
+        <v>264</v>
+      </c>
+      <c r="L38" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="M38" s="5" t="s">
         <v>265</v>
-      </c>
-      <c r="L38" s="5" t="s">
-        <v>264</v>
-      </c>
-      <c r="M38" s="5" t="s">
-        <v>266</v>
       </c>
       <c r="N38" s="1" t="s">
         <v>43</v>
@@ -2911,7 +2908,7 @@
         <v>149</v>
       </c>
       <c r="L39" s="5" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="M39" s="5" t="s">
         <v>150</v>
@@ -2953,7 +2950,7 @@
         <v>153</v>
       </c>
       <c r="L40" s="5" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="M40" s="5" t="s">
         <v>154</v>
@@ -3156,14 +3153,14 @@
         <v>75</v>
       </c>
       <c r="I45" s="5" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="J45" s="5"/>
       <c r="K45" s="5" t="s">
         <v>54</v>
       </c>
       <c r="L45" s="5" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="M45" s="5" t="s">
         <v>55</v>
@@ -3198,14 +3195,14 @@
         <v>75</v>
       </c>
       <c r="I46" s="5" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="J46" s="5"/>
       <c r="K46" s="5" t="s">
         <v>57</v>
       </c>
       <c r="L46" s="5" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="M46" s="5" t="s">
         <v>58</v>
@@ -3219,22 +3216,22 @@
         <v>179</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>180</v>
+        <v>217</v>
       </c>
       <c r="C47" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>181</v>
+        <v>218</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>289</v>
+        <v>188</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>182</v>
+        <v>219</v>
       </c>
       <c r="G47" s="5" t="s">
-        <v>183</v>
+        <v>220</v>
       </c>
       <c r="H47" s="5" t="s">
         <v>18</v>
@@ -3242,20 +3239,18 @@
       <c r="I47" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J47" s="5" t="s">
-        <v>285</v>
-      </c>
+      <c r="J47" s="5"/>
       <c r="K47" s="5" t="s">
-        <v>184</v>
+        <v>275</v>
       </c>
       <c r="L47" s="5" t="s">
-        <v>21</v>
+        <v>221</v>
       </c>
       <c r="M47" s="5" t="s">
-        <v>286</v>
+        <v>276</v>
       </c>
       <c r="N47" s="1" t="s">
-        <v>287</v>
+        <v>43</v>
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.3">
@@ -3263,22 +3258,22 @@
         <v>179</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>180</v>
+        <v>217</v>
       </c>
       <c r="C48" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>181</v>
+        <v>218</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>289</v>
+        <v>188</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>182</v>
+        <v>219</v>
       </c>
       <c r="G48" s="5" t="s">
-        <v>183</v>
+        <v>220</v>
       </c>
       <c r="H48" s="5" t="s">
         <v>18</v>
@@ -3286,20 +3281,18 @@
       <c r="I48" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J48" s="5" t="s">
-        <v>285</v>
-      </c>
+      <c r="J48" s="5"/>
       <c r="K48" s="5" t="s">
-        <v>185</v>
+        <v>222</v>
       </c>
       <c r="L48" s="5" t="s">
-        <v>21</v>
+        <v>223</v>
       </c>
       <c r="M48" s="5" t="s">
-        <v>286</v>
+        <v>224</v>
       </c>
       <c r="N48" s="1" t="s">
-        <v>288</v>
+        <v>43</v>
       </c>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.3">
@@ -3307,22 +3300,22 @@
         <v>179</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="C49" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>188</v>
+        <v>288</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="G49" s="5" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="H49" s="5" t="s">
         <v>18</v>
@@ -3330,18 +3323,20 @@
       <c r="I49" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J49" s="5"/>
+      <c r="J49" s="5" t="s">
+        <v>284</v>
+      </c>
       <c r="K49" s="5" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="L49" s="5" t="s">
-        <v>192</v>
+        <v>21</v>
       </c>
       <c r="M49" s="5" t="s">
-        <v>193</v>
+        <v>285</v>
       </c>
       <c r="N49" s="1" t="s">
-        <v>43</v>
+        <v>286</v>
       </c>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.3">
@@ -3349,22 +3344,22 @@
         <v>179</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="C50" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>188</v>
+        <v>288</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>194</v>
+        <v>182</v>
       </c>
       <c r="G50" s="5" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="H50" s="5" t="s">
         <v>18</v>
@@ -3372,18 +3367,20 @@
       <c r="I50" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J50" s="5"/>
+      <c r="J50" s="5" t="s">
+        <v>284</v>
+      </c>
       <c r="K50" s="5" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="L50" s="5" t="s">
-        <v>192</v>
+        <v>21</v>
       </c>
       <c r="M50" s="5" t="s">
-        <v>197</v>
+        <v>285</v>
       </c>
       <c r="N50" s="1" t="s">
-        <v>43</v>
+        <v>287</v>
       </c>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.3">
@@ -3391,13 +3388,13 @@
         <v>179</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>198</v>
+        <v>186</v>
       </c>
       <c r="C51" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>199</v>
+        <v>187</v>
       </c>
       <c r="E51" s="5" t="s">
         <v>188</v>
@@ -3416,13 +3413,13 @@
       </c>
       <c r="J51" s="5"/>
       <c r="K51" s="5" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="L51" s="5" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="M51" s="5" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="N51" s="1" t="s">
         <v>43</v>
@@ -3433,13 +3430,13 @@
         <v>179</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>198</v>
+        <v>186</v>
       </c>
       <c r="C52" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>199</v>
+        <v>187</v>
       </c>
       <c r="E52" s="5" t="s">
         <v>188</v>
@@ -3458,58 +3455,58 @@
       </c>
       <c r="J52" s="5"/>
       <c r="K52" s="5" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="L52" s="5" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="M52" s="5" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="N52" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="53" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A53" s="5" t="s">
         <v>179</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="C53" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>67</v>
+        <v>188</v>
       </c>
       <c r="F53" s="5" t="s">
-        <v>207</v>
+        <v>189</v>
       </c>
       <c r="G53" s="5" t="s">
-        <v>208</v>
+        <v>190</v>
       </c>
       <c r="H53" s="5" t="s">
-        <v>70</v>
+        <v>18</v>
       </c>
       <c r="I53" s="5" t="s">
-        <v>70</v>
+        <v>19</v>
       </c>
       <c r="J53" s="5"/>
       <c r="K53" s="5" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="L53" s="6" t="s">
-        <v>232</v>
+        <v>201</v>
       </c>
       <c r="M53" s="6" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="N53" s="1" t="s">
-        <v>211</v>
+        <v>43</v>
       </c>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.3">
@@ -3517,22 +3514,22 @@
         <v>179</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="C54" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="E54" s="5" t="s">
-        <v>37</v>
+        <v>188</v>
       </c>
       <c r="F54" s="5" t="s">
-        <v>212</v>
+        <v>194</v>
       </c>
       <c r="G54" s="5" t="s">
-        <v>213</v>
+        <v>195</v>
       </c>
       <c r="H54" s="5" t="s">
         <v>18</v>
@@ -3542,81 +3539,81 @@
       </c>
       <c r="J54" s="5"/>
       <c r="K54" s="5" t="s">
-        <v>214</v>
+        <v>203</v>
       </c>
       <c r="L54" s="5" t="s">
-        <v>215</v>
+        <v>201</v>
       </c>
       <c r="M54" s="5" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
       <c r="N54" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A55" s="5" t="s">
-        <v>217</v>
+        <v>179</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>218</v>
+        <v>205</v>
       </c>
       <c r="C55" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>219</v>
+        <v>206</v>
       </c>
       <c r="E55" s="5" t="s">
-        <v>188</v>
+        <v>67</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>220</v>
+        <v>207</v>
       </c>
       <c r="G55" s="5" t="s">
-        <v>221</v>
+        <v>208</v>
       </c>
       <c r="H55" s="5" t="s">
-        <v>18</v>
+        <v>70</v>
       </c>
       <c r="I55" s="5" t="s">
-        <v>19</v>
+        <v>70</v>
       </c>
       <c r="J55" s="5"/>
       <c r="K55" s="5" t="s">
-        <v>276</v>
+        <v>209</v>
       </c>
       <c r="L55" s="5" t="s">
-        <v>222</v>
-      </c>
-      <c r="M55" s="5" t="s">
-        <v>277</v>
+        <v>231</v>
+      </c>
+      <c r="M55" s="6" t="s">
+        <v>210</v>
       </c>
       <c r="N55" s="1" t="s">
-        <v>43</v>
+        <v>211</v>
       </c>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A56" s="5" t="s">
-        <v>217</v>
+        <v>179</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>218</v>
+        <v>205</v>
       </c>
       <c r="C56" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>219</v>
+        <v>206</v>
       </c>
       <c r="E56" s="5" t="s">
-        <v>188</v>
+        <v>37</v>
       </c>
       <c r="F56" s="5" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="G56" s="5" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="H56" s="5" t="s">
         <v>18</v>
@@ -3626,13 +3623,13 @@
       </c>
       <c r="J56" s="5"/>
       <c r="K56" s="5" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="L56" s="5" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="M56" s="5" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="N56" s="1" t="s">
         <v>43</v>

</xml_diff>

<commit_message>
Update Site Premium WTG001
</commit_message>
<xml_diff>
--- a/data/premium-sites.xlsx
+++ b/data/premium-sites.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Local Repository\Telkom Projects\monitoring-site-premium-telegram-bot\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7529B6F3-B3C6-4985-8308-2DCA1F65DEF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1589E596-9093-48C9-812D-17127948B9FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="731" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="731" uniqueCount="291">
   <si>
     <t>Subdistrict</t>
   </si>
@@ -896,6 +896,12 @@
   </si>
   <si>
     <t>METRO GROUP</t>
+  </si>
+  <si>
+    <t>ME-D7-WTG</t>
+  </si>
+  <si>
+    <t>172.32.250.73</t>
   </si>
 </sst>
 </file>
@@ -1235,8 +1241,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="E59" sqref="E59"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1800,10 +1806,10 @@
         <v>15</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>16</v>
+        <v>289</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>17</v>
+        <v>290</v>
       </c>
       <c r="H13" s="5" t="s">
         <v>18</v>
@@ -1842,10 +1848,10 @@
         <v>15</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>16</v>
+        <v>289</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>17</v>
+        <v>290</v>
       </c>
       <c r="H14" s="5" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
Update Site Premium JAP368
</commit_message>
<xml_diff>
--- a/data/premium-sites.xlsx
+++ b/data/premium-sites.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Local Repository\Telkom Projects\monitoring-site-premium-telegram-bot\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\Programming\Local Repository\Telkom Projects\monitoring-site-premium-telegram-bot\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1589E596-9093-48C9-812D-17127948B9FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D97CFED-DBA1-47E9-A985-925C51BE4E47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="731" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="731" uniqueCount="293">
   <si>
     <t>Subdistrict</t>
   </si>
@@ -601,13 +601,7 @@
     <t>172.25.109.29</t>
   </si>
   <si>
-    <t>1/1/16:1</t>
-  </si>
-  <si>
     <t>ZTEG9004E87D</t>
-  </si>
-  <si>
-    <t>show gpon onu detail-info gpon_onu-1/1/16:1</t>
   </si>
   <si>
     <t>GPON04-D7-JAP-3</t>
@@ -902,6 +896,18 @@
   </si>
   <si>
     <t>172.32.250.73</t>
+  </si>
+  <si>
+    <t>GPON00-D7-JPB-3</t>
+  </si>
+  <si>
+    <t>172.25.209.149</t>
+  </si>
+  <si>
+    <t>1/6/4:53</t>
+  </si>
+  <si>
+    <t>show gpon onu detail gpon-onu_1/6/4:53</t>
   </si>
 </sst>
 </file>
@@ -1241,30 +1247,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="I52" sqref="I52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="25.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="44.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="49.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="33" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="12.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.6328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="25.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="44.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="49.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="33" width="8.90625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:33" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1293,13 +1299,13 @@
         <v>8</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="M1" s="4" t="s">
         <v>9</v>
@@ -1327,7 +1333,7 @@
       <c r="AF1" s="2"/>
       <c r="AG1" s="2"/>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>11</v>
       </c>
@@ -1369,7 +1375,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>11</v>
       </c>
@@ -1411,7 +1417,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>11</v>
       </c>
@@ -1425,35 +1431,35 @@
         <v>29</v>
       </c>
       <c r="E4" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="G4" s="5" t="s">
         <v>239</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="H4" s="5" t="s">
         <v>240</v>
       </c>
-      <c r="G4" s="5" t="s">
-        <v>241</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>242</v>
-      </c>
       <c r="I4" s="5" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="J4" s="5"/>
       <c r="K4" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="L4" s="6" t="s">
+        <v>242</v>
+      </c>
+      <c r="M4" s="5" t="s">
         <v>243</v>
       </c>
-      <c r="L4" s="6" t="s">
+      <c r="N4" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="M4" s="5" t="s">
-        <v>245</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>11</v>
       </c>
@@ -1467,35 +1473,35 @@
         <v>29</v>
       </c>
       <c r="E5" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="G5" s="5" t="s">
         <v>239</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="H5" s="5" t="s">
         <v>240</v>
       </c>
-      <c r="G5" s="5" t="s">
-        <v>241</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>242</v>
-      </c>
       <c r="I5" s="5" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="J5" s="5"/>
       <c r="K5" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="L5" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="M5" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="N5" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="L5" s="5" t="s">
-        <v>244</v>
-      </c>
-      <c r="M5" s="5" t="s">
-        <v>248</v>
-      </c>
-      <c r="N5" s="1" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="6" spans="1:33" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:33" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>11</v>
       </c>
@@ -1537,7 +1543,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>11</v>
       </c>
@@ -1545,7 +1551,7 @@
         <v>28</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>29</v>
@@ -1579,7 +1585,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>11</v>
       </c>
@@ -1587,7 +1593,7 @@
         <v>28</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>29</v>
@@ -1621,7 +1627,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>11</v>
       </c>
@@ -1654,7 +1660,7 @@
         <v>54</v>
       </c>
       <c r="L9" s="5" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="M9" s="5" t="s">
         <v>55</v>
@@ -1663,7 +1669,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>11</v>
       </c>
@@ -1696,7 +1702,7 @@
         <v>57</v>
       </c>
       <c r="L10" s="5" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="M10" s="5" t="s">
         <v>58</v>
@@ -1705,7 +1711,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>59</v>
       </c>
@@ -1722,23 +1728,23 @@
         <v>51</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="H11" s="5" t="s">
         <v>75</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="J11" s="5"/>
       <c r="K11" s="5" t="s">
         <v>54</v>
       </c>
       <c r="L11" s="6" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="M11" s="5" t="s">
         <v>55</v>
@@ -1747,7 +1753,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
         <v>59</v>
       </c>
@@ -1764,32 +1770,32 @@
         <v>51</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="H12" s="5" t="s">
         <v>75</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="J12" s="5"/>
       <c r="K12" s="5" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="L12" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="M12" s="5" t="s">
         <v>280</v>
-      </c>
-      <c r="M12" s="5" t="s">
-        <v>282</v>
       </c>
       <c r="N12" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
         <v>59</v>
       </c>
@@ -1806,10 +1812,10 @@
         <v>15</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="H13" s="5" t="s">
         <v>18</v>
@@ -1819,19 +1825,19 @@
       </c>
       <c r="J13" s="5"/>
       <c r="K13" s="5" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="L13" s="6" t="s">
         <v>21</v>
       </c>
       <c r="M13" s="5" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.3">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="14" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
         <v>59</v>
       </c>
@@ -1848,10 +1854,10 @@
         <v>15</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="H14" s="5" t="s">
         <v>18</v>
@@ -1861,19 +1867,19 @@
       </c>
       <c r="J14" s="5"/>
       <c r="K14" s="5" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="L14" s="5" t="s">
         <v>21</v>
       </c>
       <c r="M14" s="5" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="15" spans="1:33" ht="28.8" x14ac:dyDescent="0.3">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="15" spans="1:33" ht="29" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
         <v>64</v>
       </c>
@@ -1903,19 +1909,19 @@
       </c>
       <c r="J15" s="5"/>
       <c r="K15" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="L15" s="6" t="s">
+        <v>225</v>
+      </c>
+      <c r="M15" s="6" t="s">
+        <v>268</v>
+      </c>
+      <c r="N15" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="L15" s="6" t="s">
-        <v>227</v>
-      </c>
-      <c r="M15" s="6" t="s">
-        <v>270</v>
-      </c>
-      <c r="N15" s="1" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="16" spans="1:33" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:33" ht="29" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
         <v>64</v>
       </c>
@@ -1945,19 +1951,19 @@
       </c>
       <c r="J16" s="5"/>
       <c r="K16" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="L16" s="6" t="s">
+        <v>225</v>
+      </c>
+      <c r="M16" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="N16" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="L16" s="6" t="s">
-        <v>227</v>
-      </c>
-      <c r="M16" s="6" t="s">
-        <v>273</v>
-      </c>
-      <c r="N16" s="1" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
         <v>64</v>
       </c>
@@ -1983,7 +1989,7 @@
         <v>75</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="J17" s="5"/>
       <c r="K17" s="5" t="s">
@@ -1999,7 +2005,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
         <v>64</v>
       </c>
@@ -2025,7 +2031,7 @@
         <v>75</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="J18" s="5"/>
       <c r="K18" s="5" t="s">
@@ -2041,7 +2047,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="s">
         <v>64</v>
       </c>
@@ -2067,7 +2073,7 @@
         <v>75</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="J19" s="5"/>
       <c r="K19" s="5" t="s">
@@ -2083,7 +2089,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A20" s="5" t="s">
         <v>64</v>
       </c>
@@ -2109,7 +2115,7 @@
         <v>75</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="J20" s="5"/>
       <c r="K20" s="5" t="s">
@@ -2125,7 +2131,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A21" s="5" t="s">
         <v>64</v>
       </c>
@@ -2167,7 +2173,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A22" s="5" t="s">
         <v>64</v>
       </c>
@@ -2209,7 +2215,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A23" s="5" t="s">
         <v>64</v>
       </c>
@@ -2226,23 +2232,23 @@
         <v>51</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="H23" s="5" t="s">
         <v>75</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="J23" s="5"/>
       <c r="K23" s="5" t="s">
         <v>54</v>
       </c>
       <c r="L23" s="6" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="M23" s="5" t="s">
         <v>55</v>
@@ -2251,7 +2257,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A24" s="5" t="s">
         <v>64</v>
       </c>
@@ -2268,23 +2274,23 @@
         <v>51</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="H24" s="5" t="s">
         <v>75</v>
       </c>
       <c r="I24" s="5" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="J24" s="5"/>
       <c r="K24" s="5" t="s">
         <v>57</v>
       </c>
       <c r="L24" s="5" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="M24" s="5" t="s">
         <v>58</v>
@@ -2293,7 +2299,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A25" s="5" t="s">
         <v>100</v>
       </c>
@@ -2335,7 +2341,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A26" s="5" t="s">
         <v>100</v>
       </c>
@@ -2377,7 +2383,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A27" s="5" t="s">
         <v>100</v>
       </c>
@@ -2403,7 +2409,7 @@
         <v>75</v>
       </c>
       <c r="I27" s="5" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="J27" s="5"/>
       <c r="K27" s="5" t="s">
@@ -2419,7 +2425,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A28" s="5" t="s">
         <v>100</v>
       </c>
@@ -2445,7 +2451,7 @@
         <v>75</v>
       </c>
       <c r="I28" s="5" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="J28" s="5"/>
       <c r="K28" s="5" t="s">
@@ -2461,7 +2467,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A29" s="5" t="s">
         <v>100</v>
       </c>
@@ -2478,10 +2484,10 @@
         <v>37</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="H29" s="5" t="s">
         <v>18</v>
@@ -2491,19 +2497,19 @@
       </c>
       <c r="J29" s="5"/>
       <c r="K29" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="L29" s="6" t="s">
+        <v>257</v>
+      </c>
+      <c r="M29" s="5" t="s">
         <v>258</v>
-      </c>
-      <c r="L29" s="6" t="s">
-        <v>259</v>
-      </c>
-      <c r="M29" s="5" t="s">
-        <v>260</v>
       </c>
       <c r="N29" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A30" s="5" t="s">
         <v>100</v>
       </c>
@@ -2520,10 +2526,10 @@
         <v>37</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="H30" s="5" t="s">
         <v>18</v>
@@ -2533,19 +2539,19 @@
       </c>
       <c r="J30" s="5"/>
       <c r="K30" s="5" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="L30" s="5" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="M30" s="5" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="N30" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A31" s="5" t="s">
         <v>100</v>
       </c>
@@ -2587,7 +2593,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A32" s="5" t="s">
         <v>100</v>
       </c>
@@ -2629,7 +2635,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A33" s="5" t="s">
         <v>100</v>
       </c>
@@ -2671,7 +2677,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A34" s="5" t="s">
         <v>100</v>
       </c>
@@ -2713,7 +2719,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A35" s="5" t="s">
         <v>134</v>
       </c>
@@ -2746,7 +2752,7 @@
         <v>54</v>
       </c>
       <c r="L35" s="5" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="M35" s="5" t="s">
         <v>140</v>
@@ -2755,7 +2761,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A36" s="5" t="s">
         <v>134</v>
       </c>
@@ -2788,7 +2794,7 @@
         <v>57</v>
       </c>
       <c r="L36" s="5" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="M36" s="5" t="s">
         <v>142</v>
@@ -2797,7 +2803,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A37" s="5" t="s">
         <v>134</v>
       </c>
@@ -2814,10 +2820,10 @@
         <v>37</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="H37" s="5" t="s">
         <v>18</v>
@@ -2830,7 +2836,7 @@
         <v>153</v>
       </c>
       <c r="L37" s="6" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="M37" s="5" t="s">
         <v>154</v>
@@ -2839,7 +2845,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A38" s="5" t="s">
         <v>134</v>
       </c>
@@ -2856,10 +2862,10 @@
         <v>37</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="G38" s="5" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="H38" s="5" t="s">
         <v>18</v>
@@ -2869,19 +2875,19 @@
       </c>
       <c r="J38" s="5"/>
       <c r="K38" s="5" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="L38" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="M38" s="5" t="s">
         <v>263</v>
-      </c>
-      <c r="M38" s="5" t="s">
-        <v>265</v>
       </c>
       <c r="N38" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A39" s="5" t="s">
         <v>134</v>
       </c>
@@ -2914,7 +2920,7 @@
         <v>149</v>
       </c>
       <c r="L39" s="5" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="M39" s="5" t="s">
         <v>150</v>
@@ -2923,7 +2929,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A40" s="5" t="s">
         <v>134</v>
       </c>
@@ -2956,7 +2962,7 @@
         <v>153</v>
       </c>
       <c r="L40" s="5" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="M40" s="5" t="s">
         <v>154</v>
@@ -2965,7 +2971,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A41" s="5" t="s">
         <v>134</v>
       </c>
@@ -3007,7 +3013,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A42" s="5" t="s">
         <v>134</v>
       </c>
@@ -3049,7 +3055,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A43" s="5" t="s">
         <v>134</v>
       </c>
@@ -3091,7 +3097,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A44" s="5" t="s">
         <v>134</v>
       </c>
@@ -3133,7 +3139,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A45" s="5" t="s">
         <v>134</v>
       </c>
@@ -3159,14 +3165,14 @@
         <v>75</v>
       </c>
       <c r="I45" s="5" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="J45" s="5"/>
       <c r="K45" s="5" t="s">
         <v>54</v>
       </c>
       <c r="L45" s="5" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="M45" s="5" t="s">
         <v>55</v>
@@ -3175,7 +3181,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A46" s="5" t="s">
         <v>134</v>
       </c>
@@ -3201,14 +3207,14 @@
         <v>75</v>
       </c>
       <c r="I46" s="5" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="J46" s="5"/>
       <c r="K46" s="5" t="s">
         <v>57</v>
       </c>
       <c r="L46" s="5" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="M46" s="5" t="s">
         <v>58</v>
@@ -3217,27 +3223,27 @@
         <v>56</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A47" s="5" t="s">
         <v>179</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C47" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E47" s="5" t="s">
         <v>188</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="G47" s="5" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="H47" s="5" t="s">
         <v>18</v>
@@ -3247,39 +3253,39 @@
       </c>
       <c r="J47" s="5"/>
       <c r="K47" s="5" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="L47" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="M47" s="5" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="N47" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A48" s="5" t="s">
         <v>179</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C48" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E48" s="5" t="s">
         <v>188</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="G48" s="5" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="H48" s="5" t="s">
         <v>18</v>
@@ -3289,19 +3295,19 @@
       </c>
       <c r="J48" s="5"/>
       <c r="K48" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="L48" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="M48" s="5" t="s">
         <v>222</v>
-      </c>
-      <c r="L48" s="5" t="s">
-        <v>223</v>
-      </c>
-      <c r="M48" s="5" t="s">
-        <v>224</v>
       </c>
       <c r="N48" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A49" s="5" t="s">
         <v>179</v>
       </c>
@@ -3315,7 +3321,7 @@
         <v>181</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="F49" s="5" t="s">
         <v>182</v>
@@ -3330,7 +3336,7 @@
         <v>19</v>
       </c>
       <c r="J49" s="5" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="K49" s="5" t="s">
         <v>184</v>
@@ -3339,13 +3345,13 @@
         <v>21</v>
       </c>
       <c r="M49" s="5" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="N49" s="1" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.3">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A50" s="5" t="s">
         <v>179</v>
       </c>
@@ -3359,7 +3365,7 @@
         <v>181</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="F50" s="5" t="s">
         <v>182</v>
@@ -3374,7 +3380,7 @@
         <v>19</v>
       </c>
       <c r="J50" s="5" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="K50" s="5" t="s">
         <v>185</v>
@@ -3383,13 +3389,13 @@
         <v>21</v>
       </c>
       <c r="M50" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="N50" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="N50" s="1" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A51" s="5" t="s">
         <v>179</v>
       </c>
@@ -3403,13 +3409,13 @@
         <v>187</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>188</v>
+        <v>37</v>
       </c>
       <c r="F51" s="5" t="s">
-        <v>189</v>
+        <v>289</v>
       </c>
       <c r="G51" s="5" t="s">
-        <v>190</v>
+        <v>290</v>
       </c>
       <c r="H51" s="5" t="s">
         <v>18</v>
@@ -3419,19 +3425,19 @@
       </c>
       <c r="J51" s="5"/>
       <c r="K51" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="L51" s="5" t="s">
         <v>191</v>
       </c>
-      <c r="L51" s="5" t="s">
-        <v>192</v>
-      </c>
       <c r="M51" s="5" t="s">
-        <v>193</v>
+        <v>292</v>
       </c>
       <c r="N51" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A52" s="5" t="s">
         <v>179</v>
       </c>
@@ -3448,10 +3454,10 @@
         <v>188</v>
       </c>
       <c r="F52" s="5" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="G52" s="5" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="H52" s="5" t="s">
         <v>18</v>
@@ -3461,30 +3467,30 @@
       </c>
       <c r="J52" s="5"/>
       <c r="K52" s="5" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="L52" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="M52" s="5" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="N52" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A53" s="5" t="s">
         <v>179</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C53" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E53" s="5" t="s">
         <v>188</v>
@@ -3503,39 +3509,39 @@
       </c>
       <c r="J53" s="5"/>
       <c r="K53" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="L53" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="M53" s="6" t="s">
         <v>200</v>
-      </c>
-      <c r="L53" s="6" t="s">
-        <v>201</v>
-      </c>
-      <c r="M53" s="6" t="s">
-        <v>202</v>
       </c>
       <c r="N53" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A54" s="5" t="s">
         <v>179</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C54" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E54" s="5" t="s">
         <v>188</v>
       </c>
       <c r="F54" s="5" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="G54" s="5" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="H54" s="5" t="s">
         <v>18</v>
@@ -3545,39 +3551,39 @@
       </c>
       <c r="J54" s="5"/>
       <c r="K54" s="5" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="L54" s="5" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="M54" s="5" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="N54" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="55" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A55" s="5" t="s">
         <v>179</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C55" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="E55" s="5" t="s">
         <v>67</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="G55" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="H55" s="5" t="s">
         <v>70</v>
@@ -3587,39 +3593,39 @@
       </c>
       <c r="J55" s="5"/>
       <c r="K55" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="L55" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="M55" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="N55" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="L55" s="5" t="s">
-        <v>231</v>
-      </c>
-      <c r="M55" s="6" t="s">
-        <v>210</v>
-      </c>
-      <c r="N55" s="1" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A56" s="5" t="s">
         <v>179</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C56" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="E56" s="5" t="s">
         <v>37</v>
       </c>
       <c r="F56" s="5" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="G56" s="5" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="H56" s="5" t="s">
         <v>18</v>
@@ -3629,13 +3635,13 @@
       </c>
       <c r="J56" s="5"/>
       <c r="K56" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="L56" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="M56" s="5" t="s">
         <v>214</v>
-      </c>
-      <c r="L56" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="M56" s="5" t="s">
-        <v>216</v>
       </c>
       <c r="N56" s="1" t="s">
         <v>43</v>

</xml_diff>

<commit_message>
Update Site Premium KDI010
</commit_message>
<xml_diff>
--- a/data/premium-sites.xlsx
+++ b/data/premium-sites.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\Programming\Local Repository\Telkom Projects\monitoring-site-premium-telegram-bot\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Local Repository\Telkom Projects\monitoring-site-premium-telegram-bot\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D97CFED-DBA1-47E9-A985-925C51BE4E47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB49A77A-2A2E-4CFA-BBFB-5270283BE676}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="731" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="731" uniqueCount="291">
   <si>
     <t>Subdistrict</t>
   </si>
@@ -307,21 +307,6 @@
     <t>Eth-Trunk24.352 current state : UP</t>
   </si>
   <si>
-    <t>ME-D7-KDR</t>
-  </si>
-  <si>
-    <t>172.32.250.22</t>
-  </si>
-  <si>
-    <t>GigabitEthernet8/0/8</t>
-  </si>
-  <si>
-    <t>display interface GigabitEthernet8/0/8</t>
-  </si>
-  <si>
-    <t>GigabitEthernet8/0/8 current state : UP</t>
-  </si>
-  <si>
     <t>UNH001</t>
   </si>
   <si>
@@ -908,6 +893,15 @@
   </si>
   <si>
     <t>show gpon onu detail gpon-onu_1/6/4:53</t>
+  </si>
+  <si>
+    <t>L2SW-D7-KDR-KDI010</t>
+  </si>
+  <si>
+    <t>10.199.154.248</t>
+  </si>
+  <si>
+    <t>729798100099</t>
   </si>
 </sst>
 </file>
@@ -1247,30 +1241,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="I52" sqref="I52"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.6328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="25.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="44.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="49.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="33" width="8.90625" style="1"/>
+    <col min="1" max="1" width="12.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="25.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="44.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="49.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="33" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:33" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1299,13 +1293,13 @@
         <v>8</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="M1" s="4" t="s">
         <v>9</v>
@@ -1333,7 +1327,7 @@
       <c r="AF1" s="2"/>
       <c r="AG1" s="2"/>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>11</v>
       </c>
@@ -1375,7 +1369,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>11</v>
       </c>
@@ -1417,7 +1411,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>11</v>
       </c>
@@ -1431,35 +1425,35 @@
         <v>29</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="J4" s="5"/>
       <c r="K4" s="5" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="L4" s="6" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="M4" s="5" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.35">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>11</v>
       </c>
@@ -1473,35 +1467,35 @@
         <v>29</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="J5" s="5"/>
       <c r="K5" s="5" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="L5" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="M5" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="N5" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="M5" s="5" t="s">
-        <v>246</v>
-      </c>
-      <c r="N5" s="1" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="6" spans="1:33" ht="43.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="1:33" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>11</v>
       </c>
@@ -1543,7 +1537,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>11</v>
       </c>
@@ -1551,7 +1545,7 @@
         <v>28</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>29</v>
@@ -1585,7 +1579,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>11</v>
       </c>
@@ -1593,7 +1587,7 @@
         <v>28</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>29</v>
@@ -1627,7 +1621,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>11</v>
       </c>
@@ -1660,7 +1654,7 @@
         <v>54</v>
       </c>
       <c r="L9" s="5" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="M9" s="5" t="s">
         <v>55</v>
@@ -1669,7 +1663,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>11</v>
       </c>
@@ -1702,7 +1696,7 @@
         <v>57</v>
       </c>
       <c r="L10" s="5" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="M10" s="5" t="s">
         <v>58</v>
@@ -1711,7 +1705,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>59</v>
       </c>
@@ -1728,23 +1722,23 @@
         <v>51</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="H11" s="5" t="s">
         <v>75</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="J11" s="5"/>
       <c r="K11" s="5" t="s">
         <v>54</v>
       </c>
       <c r="L11" s="6" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="M11" s="5" t="s">
         <v>55</v>
@@ -1753,7 +1747,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>59</v>
       </c>
@@ -1770,32 +1764,32 @@
         <v>51</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="H12" s="5" t="s">
         <v>75</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="J12" s="5"/>
       <c r="K12" s="5" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="L12" s="5" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="M12" s="5" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="N12" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>59</v>
       </c>
@@ -1812,10 +1806,10 @@
         <v>15</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="H13" s="5" t="s">
         <v>18</v>
@@ -1825,19 +1819,19 @@
       </c>
       <c r="J13" s="5"/>
       <c r="K13" s="5" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="L13" s="6" t="s">
         <v>21</v>
       </c>
       <c r="M13" s="5" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.35">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="14" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>59</v>
       </c>
@@ -1854,10 +1848,10 @@
         <v>15</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="H14" s="5" t="s">
         <v>18</v>
@@ -1867,19 +1861,19 @@
       </c>
       <c r="J14" s="5"/>
       <c r="K14" s="5" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="L14" s="5" t="s">
         <v>21</v>
       </c>
       <c r="M14" s="5" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="15" spans="1:33" ht="29" x14ac:dyDescent="0.35">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="15" spans="1:33" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>64</v>
       </c>
@@ -1909,19 +1903,19 @@
       </c>
       <c r="J15" s="5"/>
       <c r="K15" s="5" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="L15" s="6" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="M15" s="6" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="16" spans="1:33" ht="29" x14ac:dyDescent="0.35">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="16" spans="1:33" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>64</v>
       </c>
@@ -1951,19 +1945,19 @@
       </c>
       <c r="J16" s="5"/>
       <c r="K16" s="5" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="L16" s="6" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="M16" s="6" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>64</v>
       </c>
@@ -1989,7 +1983,7 @@
         <v>75</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="J17" s="5"/>
       <c r="K17" s="5" t="s">
@@ -2005,7 +1999,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>64</v>
       </c>
@@ -2031,7 +2025,7 @@
         <v>75</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="J18" s="5"/>
       <c r="K18" s="5" t="s">
@@ -2047,7 +2041,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>64</v>
       </c>
@@ -2073,7 +2067,7 @@
         <v>75</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="J19" s="5"/>
       <c r="K19" s="5" t="s">
@@ -2089,7 +2083,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
         <v>64</v>
       </c>
@@ -2115,7 +2109,7 @@
         <v>75</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="J20" s="5"/>
       <c r="K20" s="5" t="s">
@@ -2131,7 +2125,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>64</v>
       </c>
@@ -2173,7 +2167,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
         <v>64</v>
       </c>
@@ -2187,68 +2181,68 @@
         <v>87</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>15</v>
+        <v>67</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>93</v>
+        <v>288</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>94</v>
+        <v>289</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>18</v>
+        <v>70</v>
       </c>
       <c r="I22" s="5" t="s">
-        <v>19</v>
+        <v>70</v>
       </c>
       <c r="J22" s="5"/>
       <c r="K22" s="5" t="s">
-        <v>95</v>
+        <v>262</v>
       </c>
       <c r="L22" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="M22" s="5" t="s">
-        <v>96</v>
+        <v>290</v>
+      </c>
+      <c r="M22" s="6" t="s">
+        <v>263</v>
       </c>
       <c r="N22" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
         <v>64</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="E23" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="H23" s="5" t="s">
         <v>75</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="J23" s="5"/>
       <c r="K23" s="5" t="s">
         <v>54</v>
       </c>
       <c r="L23" s="6" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="M23" s="5" t="s">
         <v>55</v>
@@ -2257,40 +2251,40 @@
         <v>56</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>64</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="E24" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="H24" s="5" t="s">
         <v>75</v>
       </c>
       <c r="I24" s="5" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="J24" s="5"/>
       <c r="K24" s="5" t="s">
         <v>57</v>
       </c>
       <c r="L24" s="5" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="M24" s="5" t="s">
         <v>58</v>
@@ -2299,27 +2293,27 @@
         <v>56</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="H25" s="5" t="s">
         <v>18</v>
@@ -2329,39 +2323,39 @@
       </c>
       <c r="J25" s="5"/>
       <c r="K25" s="5" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="L25" s="5" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="M25" s="5" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="N25" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="H26" s="5" t="s">
         <v>18</v>
@@ -2371,52 +2365,52 @@
       </c>
       <c r="J26" s="5"/>
       <c r="K26" s="5" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="L26" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="M26" s="5" t="s">
         <v>107</v>
-      </c>
-      <c r="M26" s="5" t="s">
-        <v>112</v>
       </c>
       <c r="N26" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="E27" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="H27" s="5" t="s">
         <v>75</v>
       </c>
       <c r="I27" s="5" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="J27" s="5"/>
       <c r="K27" s="5" t="s">
         <v>54</v>
       </c>
       <c r="L27" s="5" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="M27" s="5" t="s">
         <v>55</v>
@@ -2425,40 +2419,40 @@
         <v>56</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="E28" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="H28" s="5" t="s">
         <v>75</v>
       </c>
       <c r="I28" s="5" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="J28" s="5"/>
       <c r="K28" s="5" t="s">
         <v>57</v>
       </c>
       <c r="L28" s="5" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="M28" s="5" t="s">
         <v>58</v>
@@ -2467,27 +2461,27 @@
         <v>56</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="E29" s="5" t="s">
         <v>37</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="H29" s="5" t="s">
         <v>18</v>
@@ -2497,39 +2491,39 @@
       </c>
       <c r="J29" s="5"/>
       <c r="K29" s="5" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="L29" s="6" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="M29" s="5" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="N29" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="E30" s="5" t="s">
         <v>37</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="H30" s="5" t="s">
         <v>18</v>
@@ -2539,39 +2533,39 @@
       </c>
       <c r="J30" s="5"/>
       <c r="K30" s="5" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="L30" s="5" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="M30" s="5" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="N30" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="C31" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="E31" s="5" t="s">
         <v>37</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="H31" s="5" t="s">
         <v>18</v>
@@ -2581,39 +2575,39 @@
       </c>
       <c r="J31" s="5"/>
       <c r="K31" s="5" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="L31" s="5" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="M31" s="5" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="N31" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="C32" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="E32" s="5" t="s">
         <v>37</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="H32" s="5" t="s">
         <v>18</v>
@@ -2623,39 +2617,39 @@
       </c>
       <c r="J32" s="5"/>
       <c r="K32" s="5" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="L32" s="5" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="M32" s="5" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="N32" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="C33" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="E33" s="5" t="s">
         <v>37</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="H33" s="5" t="s">
         <v>18</v>
@@ -2665,39 +2659,39 @@
       </c>
       <c r="J33" s="5"/>
       <c r="K33" s="5" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="L33" s="5" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="M33" s="5" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="N33" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="C34" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="E34" s="5" t="s">
         <v>37</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="G34" s="5" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="H34" s="5" t="s">
         <v>18</v>
@@ -2707,39 +2701,39 @@
       </c>
       <c r="J34" s="5"/>
       <c r="K34" s="5" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="L34" s="5" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="M34" s="5" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="N34" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="C35" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="H35" s="5" t="s">
         <v>18</v>
@@ -2752,36 +2746,36 @@
         <v>54</v>
       </c>
       <c r="L35" s="5" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="M35" s="5" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="N35" s="1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.35">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="C36" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="G36" s="5" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="H36" s="5" t="s">
         <v>18</v>
@@ -2794,36 +2788,36 @@
         <v>57</v>
       </c>
       <c r="L36" s="5" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="M36" s="5" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="N36" s="1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.35">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="C37" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="E37" s="5" t="s">
         <v>37</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="H37" s="5" t="s">
         <v>18</v>
@@ -2833,39 +2827,39 @@
       </c>
       <c r="J37" s="5"/>
       <c r="K37" s="5" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="L37" s="6" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="M37" s="5" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="N37" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="E38" s="5" t="s">
         <v>37</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="G38" s="5" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="H38" s="5" t="s">
         <v>18</v>
@@ -2875,39 +2869,39 @@
       </c>
       <c r="J38" s="5"/>
       <c r="K38" s="5" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="L38" s="5" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="M38" s="5" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="N38" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="E39" s="5" t="s">
         <v>37</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="H39" s="5" t="s">
         <v>18</v>
@@ -2917,39 +2911,39 @@
       </c>
       <c r="J39" s="5"/>
       <c r="K39" s="5" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="L39" s="5" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="M39" s="5" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="N39" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C40" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="E40" s="5" t="s">
         <v>37</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="G40" s="5" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="H40" s="5" t="s">
         <v>18</v>
@@ -2959,39 +2953,39 @@
       </c>
       <c r="J40" s="5"/>
       <c r="K40" s="5" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="L40" s="5" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="M40" s="5" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="N40" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A41" s="5" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="C41" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="E41" s="5" t="s">
         <v>37</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="H41" s="5" t="s">
         <v>18</v>
@@ -3001,39 +2995,39 @@
       </c>
       <c r="J41" s="5"/>
       <c r="K41" s="5" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="L41" s="5" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="M41" s="5" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="N41" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="C42" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="E42" s="5" t="s">
         <v>37</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="G42" s="5" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="H42" s="5" t="s">
         <v>18</v>
@@ -3043,39 +3037,39 @@
       </c>
       <c r="J42" s="5"/>
       <c r="K42" s="5" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="L42" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="M42" s="5" t="s">
         <v>160</v>
-      </c>
-      <c r="M42" s="5" t="s">
-        <v>165</v>
       </c>
       <c r="N42" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="C43" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="E43" s="5" t="s">
         <v>37</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="H43" s="5" t="s">
         <v>18</v>
@@ -3085,39 +3079,39 @@
       </c>
       <c r="J43" s="5"/>
       <c r="K43" s="5" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="L43" s="5" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="M43" s="5" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="N43" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="C44" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="E44" s="5" t="s">
         <v>37</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="G44" s="5" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="H44" s="5" t="s">
         <v>18</v>
@@ -3127,52 +3121,52 @@
       </c>
       <c r="J44" s="5"/>
       <c r="K44" s="5" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="L44" s="5" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="M44" s="5" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="N44" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="C45" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="E45" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="G45" s="5" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="H45" s="5" t="s">
         <v>75</v>
       </c>
       <c r="I45" s="5" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="J45" s="5"/>
       <c r="K45" s="5" t="s">
         <v>54</v>
       </c>
       <c r="L45" s="5" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="M45" s="5" t="s">
         <v>55</v>
@@ -3181,40 +3175,40 @@
         <v>56</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A46" s="5" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="C46" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="E46" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="G46" s="5" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="H46" s="5" t="s">
         <v>75</v>
       </c>
       <c r="I46" s="5" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="J46" s="5"/>
       <c r="K46" s="5" t="s">
         <v>57</v>
       </c>
       <c r="L46" s="5" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="M46" s="5" t="s">
         <v>58</v>
@@ -3223,27 +3217,27 @@
         <v>56</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A47" s="5" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="C47" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="G47" s="5" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="H47" s="5" t="s">
         <v>18</v>
@@ -3253,39 +3247,39 @@
       </c>
       <c r="J47" s="5"/>
       <c r="K47" s="5" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="L47" s="5" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="M47" s="5" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="N47" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="C48" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="G48" s="5" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="H48" s="5" t="s">
         <v>18</v>
@@ -3295,39 +3289,39 @@
       </c>
       <c r="J48" s="5"/>
       <c r="K48" s="5" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="L48" s="5" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="M48" s="5" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="N48" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="C49" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="G49" s="5" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="H49" s="5" t="s">
         <v>18</v>
@@ -3336,42 +3330,42 @@
         <v>19</v>
       </c>
       <c r="J49" s="5" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="K49" s="5" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="L49" s="5" t="s">
         <v>21</v>
       </c>
       <c r="M49" s="5" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="N49" s="1" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.35">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="C50" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="G50" s="5" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="H50" s="5" t="s">
         <v>18</v>
@@ -3380,42 +3374,42 @@
         <v>19</v>
       </c>
       <c r="J50" s="5" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="K50" s="5" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="L50" s="5" t="s">
         <v>21</v>
       </c>
       <c r="M50" s="5" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="N50" s="1" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.35">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="C51" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="E51" s="5" t="s">
         <v>37</v>
       </c>
       <c r="F51" s="5" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="G51" s="5" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="H51" s="5" t="s">
         <v>18</v>
@@ -3425,39 +3419,39 @@
       </c>
       <c r="J51" s="5"/>
       <c r="K51" s="5" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="L51" s="5" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="M51" s="5" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="N51" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="C52" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D52" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="E52" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="F52" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="E52" s="5" t="s">
+      <c r="G52" s="5" t="s">
         <v>188</v>
-      </c>
-      <c r="F52" s="5" t="s">
-        <v>192</v>
-      </c>
-      <c r="G52" s="5" t="s">
-        <v>193</v>
       </c>
       <c r="H52" s="5" t="s">
         <v>18</v>
@@ -3467,39 +3461,39 @@
       </c>
       <c r="J52" s="5"/>
       <c r="K52" s="5" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="L52" s="5" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="M52" s="5" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="N52" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A53" s="5" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="C53" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="F53" s="5" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="G53" s="5" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="H53" s="5" t="s">
         <v>18</v>
@@ -3509,39 +3503,39 @@
       </c>
       <c r="J53" s="5"/>
       <c r="K53" s="5" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="L53" s="6" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="M53" s="6" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="N53" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A54" s="5" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="C54" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="E54" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="F54" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="G54" s="5" t="s">
         <v>188</v>
-      </c>
-      <c r="F54" s="5" t="s">
-        <v>192</v>
-      </c>
-      <c r="G54" s="5" t="s">
-        <v>193</v>
       </c>
       <c r="H54" s="5" t="s">
         <v>18</v>
@@ -3551,39 +3545,39 @@
       </c>
       <c r="J54" s="5"/>
       <c r="K54" s="5" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="L54" s="5" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="M54" s="5" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="N54" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="55" spans="1:14" ht="29" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A55" s="5" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C55" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="E55" s="5" t="s">
         <v>67</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="G55" s="5" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="H55" s="5" t="s">
         <v>70</v>
@@ -3593,39 +3587,39 @@
       </c>
       <c r="J55" s="5"/>
       <c r="K55" s="5" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="L55" s="5" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="M55" s="6" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="N55" s="1" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.35">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A56" s="5" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C56" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="E56" s="5" t="s">
         <v>37</v>
       </c>
       <c r="F56" s="5" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="G56" s="5" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="H56" s="5" t="s">
         <v>18</v>
@@ -3635,13 +3629,13 @@
       </c>
       <c r="J56" s="5"/>
       <c r="K56" s="5" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="L56" s="5" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="M56" s="5" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="N56" s="1" t="s">
         <v>43</v>

</xml_diff>